<commit_message>
added password cic to metadata spreadsheet
</commit_message>
<xml_diff>
--- a/metadata/InventaireCampa.xlsx
+++ b/metadata/InventaireCampa.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
-  <fileSharing readOnlyRecommended="1" userName="Microsoft Office User" algorithmName="SHA-512" hashValue="AeiEt4xr0OCEy7CtjETfKVhSmUVAtKTmwHHl7TTvvLeU3sF7bi5a33VfHPInya18S1QOspay6dbFigibT2XudQ==" saltValue="FEwYxjwfNy6JlgkfgunnaQ==" spinCount="100000"/>
+  <fileSharing readOnlyRecommended="1" userName="Microsoft Office User" algorithmName="SHA-512" hashValue="UnG+o7R59VgX65WVs+ji3HTvfzo0sunkoL8BqnVOB2lIbjYUNILgvx4poeuKhCh+2BB7Bd2bAPc/AnOX0WZOdA==" saltValue="Ncv7cTDbBFcSFZismwlwuA==" spinCount="100000"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arlogriffiths/Documents/GitHub/DHARMA/tfc-campa-epigraphy/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3115C9FC-1872-B04D-BF74-CD0D5C6A1CB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0410FF27-023E-B541-A74D-9E6F1FA07684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3660" windowWidth="33520" windowHeight="15380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
changed rtfs and metadata
</commit_message>
<xml_diff>
--- a/metadata/InventaireCampa.xlsx
+++ b/metadata/InventaireCampa.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arlogriffiths/Documents/GitHub/DHARMA/tfc-campa-epigraphy/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{9E5FE007-AB32-ED45-BD4D-D204D8B3DCEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{F4B522BB-FCF7-B841-8B8E-CA7952F591A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1280" windowWidth="33520" windowHeight="15380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$Z$453</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$Z$454</definedName>
   </definedNames>
   <calcPr calcId="110000"/>
   <extLst>
@@ -10873,9 +10873,6 @@
     <t>*Hue1</t>
   </si>
   <si>
-    <t>*Hue2</t>
-  </si>
-  <si>
     <t>Quảng Thọ</t>
   </si>
   <si>
@@ -12233,6 +12230,9 @@
       </rPr>
       <t>; XV (2), 11, 47. — P., 79. — ECIC II, 294-295. — ECIC III, 446, 481-484, 486.</t>
     </r>
+  </si>
+  <si>
+    <t>*252</t>
   </si>
 </sst>
 </file>
@@ -13188,12 +13188,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC455"/>
+  <dimension ref="A1:AC456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1300" topLeftCell="A225" activePane="bottomLeft"/>
-      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
-      <selection pane="bottomLeft" activeCell="F228" sqref="F228"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1300" topLeftCell="A425" activePane="bottomLeft"/>
+      <selection activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="J429" sqref="J429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13240,7 +13240,7 @@
         <v>898</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>1786</v>
@@ -13415,13 +13415,13 @@
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
       <c r="X3" s="57" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="Y3" s="57" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="Z3" s="58" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="AA3" s="23"/>
       <c r="AC3" s="1"/>
@@ -13611,7 +13611,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="140" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" ht="123" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>4</v>
       </c>
@@ -13671,7 +13671,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="140" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" ht="123" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>4</v>
       </c>
@@ -13901,7 +13901,7 @@
       </c>
       <c r="Z11" s="15"/>
     </row>
-    <row r="12" spans="1:29" ht="140" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="123" x14ac:dyDescent="0.2">
       <c r="A12" s="26">
         <v>7</v>
       </c>
@@ -13961,7 +13961,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="140" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="123" x14ac:dyDescent="0.2">
       <c r="A13" s="26">
         <v>7</v>
       </c>
@@ -14021,7 +14021,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="121" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="104" x14ac:dyDescent="0.2">
       <c r="A14" s="26">
         <v>8</v>
       </c>
@@ -14081,7 +14081,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="121" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="104" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>8</v>
       </c>
@@ -14139,7 +14139,7 @@
       </c>
       <c r="Z15" s="15"/>
     </row>
-    <row r="16" spans="1:29" ht="121" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="104" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>8</v>
       </c>
@@ -14197,7 +14197,7 @@
       </c>
       <c r="Z16" s="15"/>
     </row>
-    <row r="17" spans="1:26" ht="121" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="104" x14ac:dyDescent="0.2">
       <c r="A17" s="47">
         <v>9</v>
       </c>
@@ -14255,7 +14255,7 @@
       </c>
       <c r="Z17" s="15"/>
     </row>
-    <row r="18" spans="1:26" ht="121" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="104" x14ac:dyDescent="0.2">
       <c r="A18" s="47">
         <v>9</v>
       </c>
@@ -14313,7 +14313,7 @@
       </c>
       <c r="Z18" s="15"/>
     </row>
-    <row r="19" spans="1:26" ht="121" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="104" x14ac:dyDescent="0.2">
       <c r="A19" s="47">
         <v>9</v>
       </c>
@@ -14373,7 +14373,7 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="121" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="104" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>10</v>
       </c>
@@ -14429,7 +14429,7 @@
       </c>
       <c r="Z20" s="15"/>
     </row>
-    <row r="21" spans="1:26" ht="121" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="104" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>11</v>
       </c>
@@ -15005,7 +15005,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="138" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" ht="121" x14ac:dyDescent="0.2">
       <c r="A31" s="26">
         <v>17</v>
       </c>
@@ -15052,7 +15052,7 @@
       </c>
       <c r="S31" s="10"/>
       <c r="T31" s="10" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="U31" s="10" t="s">
         <v>882</v>
@@ -15116,10 +15116,10 @@
         <v>1553</v>
       </c>
       <c r="Z32" s="14" t="s">
-        <v>1953</v>
-      </c>
-    </row>
-    <row r="33" spans="1:27" ht="138" x14ac:dyDescent="0.2">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" ht="121" x14ac:dyDescent="0.2">
       <c r="A33" s="18">
         <v>19</v>
       </c>
@@ -15177,7 +15177,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="138" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" ht="121" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <v>20</v>
       </c>
@@ -15235,7 +15235,7 @@
       </c>
       <c r="Z34" s="15"/>
     </row>
-    <row r="35" spans="1:27" ht="138" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" ht="121" x14ac:dyDescent="0.2">
       <c r="A35" s="18">
         <v>20</v>
       </c>
@@ -15342,10 +15342,10 @@
         <v>729</v>
       </c>
       <c r="Z36" s="14" t="s">
-        <v>1952</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27" ht="155" x14ac:dyDescent="0.2">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" ht="138" x14ac:dyDescent="0.2">
       <c r="A37" s="18">
         <v>22</v>
       </c>
@@ -15399,7 +15399,7 @@
       </c>
       <c r="Z37" s="15"/>
     </row>
-    <row r="38" spans="1:27" ht="155" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" ht="138" x14ac:dyDescent="0.2">
       <c r="A38" s="26">
         <v>22</v>
       </c>
@@ -15511,7 +15511,7 @@
         <v>1090</v>
       </c>
       <c r="Y39" s="10" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="Z39" s="15" t="s">
         <v>425</v>
@@ -16037,10 +16037,10 @@
       <c r="X48" s="10"/>
       <c r="Y48" s="10"/>
       <c r="Z48" s="15" t="s">
-        <v>1948</v>
-      </c>
-    </row>
-    <row r="49" spans="1:26" ht="204" x14ac:dyDescent="0.2">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" ht="187" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
         <v>28</v>
       </c>
@@ -16096,7 +16096,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="153" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A50" s="26">
         <v>29</v>
       </c>
@@ -16152,7 +16152,7 @@
       </c>
       <c r="Z50" s="15"/>
     </row>
-    <row r="51" spans="1:26" ht="68" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="18">
         <v>29</v>
       </c>
@@ -17146,7 +17146,7 @@
       <c r="Y68" s="10"/>
       <c r="Z68" s="15"/>
     </row>
-    <row r="69" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A69" s="18">
         <v>32</v>
       </c>
@@ -17202,7 +17202,7 @@
       </c>
       <c r="Z69" s="15"/>
     </row>
-    <row r="70" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A70" s="18">
         <v>32</v>
       </c>
@@ -17522,7 +17522,7 @@
       </c>
       <c r="Z75" s="15"/>
     </row>
-    <row r="76" spans="1:26" ht="85" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A76" s="18">
         <v>37</v>
       </c>
@@ -17953,7 +17953,7 @@
         <v>962</v>
       </c>
       <c r="Z82" s="15" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="83" spans="1:26" ht="68" x14ac:dyDescent="0.2">
@@ -18014,7 +18014,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="84" spans="1:26" ht="289" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:26" ht="272" x14ac:dyDescent="0.2">
       <c r="A84" s="18">
         <v>40</v>
       </c>
@@ -18116,7 +18116,7 @@
       <c r="S85" s="10"/>
       <c r="T85" s="10"/>
       <c r="U85" s="7" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="V85" s="10"/>
       <c r="W85" s="10"/>
@@ -18182,7 +18182,7 @@
       </c>
       <c r="Z86" s="15"/>
     </row>
-    <row r="87" spans="1:26" ht="238" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:26" ht="204" x14ac:dyDescent="0.2">
       <c r="A87" s="18">
         <v>42</v>
       </c>
@@ -18236,7 +18236,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="88" spans="1:26" ht="187" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A88" s="18">
         <v>43</v>
       </c>
@@ -18279,7 +18279,7 @@
       </c>
       <c r="S88" s="10"/>
       <c r="T88" s="10" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="U88" s="10"/>
       <c r="V88" s="10"/>
@@ -18292,7 +18292,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="89" spans="1:26" ht="187" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A89" s="18">
         <v>43</v>
       </c>
@@ -18335,7 +18335,7 @@
       </c>
       <c r="S89" s="10"/>
       <c r="T89" s="10" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="U89" s="10"/>
       <c r="V89" s="10"/>
@@ -18348,7 +18348,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="90" spans="1:26" ht="187" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A90" s="26">
         <v>43</v>
       </c>
@@ -18391,7 +18391,7 @@
       </c>
       <c r="S90" s="10"/>
       <c r="T90" s="10" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="U90" s="10"/>
       <c r="V90" s="10"/>
@@ -18404,7 +18404,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="91" spans="1:26" ht="187" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A91" s="26">
         <v>43</v>
       </c>
@@ -18447,7 +18447,7 @@
       </c>
       <c r="S91" s="10"/>
       <c r="T91" s="7" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="U91" s="10"/>
       <c r="V91" s="10"/>
@@ -18778,7 +18778,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="98" spans="1:26" ht="85" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A98" s="18">
         <v>50</v>
       </c>
@@ -18814,7 +18814,7 @@
         <v>775</v>
       </c>
       <c r="Q98" s="7" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="R98" s="10" t="s">
         <v>1065</v>
@@ -18928,7 +18928,7 @@
       </c>
       <c r="Z100" s="15"/>
     </row>
-    <row r="101" spans="1:26" ht="170" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A101" s="18">
         <v>52</v>
       </c>
@@ -19086,7 +19086,7 @@
       </c>
       <c r="Z103" s="15"/>
     </row>
-    <row r="104" spans="1:26" ht="170" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A104" s="18">
         <v>54</v>
       </c>
@@ -19140,7 +19140,7 @@
       </c>
       <c r="Z104" s="15"/>
     </row>
-    <row r="105" spans="1:26" ht="170" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A105" s="18">
         <v>54</v>
       </c>
@@ -19194,7 +19194,7 @@
       </c>
       <c r="Z105" s="15"/>
     </row>
-    <row r="106" spans="1:26" ht="170" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A106" s="18">
         <v>55</v>
       </c>
@@ -19246,7 +19246,7 @@
       </c>
       <c r="Z106" s="15"/>
     </row>
-    <row r="107" spans="1:26" ht="170" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A107" s="18">
         <v>55</v>
       </c>
@@ -19298,7 +19298,7 @@
       </c>
       <c r="Z107" s="15"/>
     </row>
-    <row r="108" spans="1:26" ht="238" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:26" ht="204" x14ac:dyDescent="0.2">
       <c r="A108" s="18">
         <v>56</v>
       </c>
@@ -19322,7 +19322,7 @@
         <v>775</v>
       </c>
       <c r="M108" s="57" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="N108" s="10" t="s">
         <v>443</v>
@@ -19346,11 +19346,11 @@
       <c r="W108" s="10"/>
       <c r="X108" s="10"/>
       <c r="Y108" s="57" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="Z108" s="15"/>
     </row>
-    <row r="109" spans="1:26" ht="238" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:26" ht="204" x14ac:dyDescent="0.2">
       <c r="A109" s="26">
         <v>56</v>
       </c>
@@ -19374,7 +19374,7 @@
         <v>775</v>
       </c>
       <c r="M109" s="57" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="N109" s="10" t="s">
         <v>611</v>
@@ -19398,11 +19398,11 @@
       <c r="W109" s="10"/>
       <c r="X109" s="10"/>
       <c r="Y109" s="57" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="Z109" s="15"/>
     </row>
-    <row r="110" spans="1:26" ht="238" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:26" ht="204" x14ac:dyDescent="0.2">
       <c r="A110" s="18">
         <v>56</v>
       </c>
@@ -19426,7 +19426,7 @@
         <v>775</v>
       </c>
       <c r="M110" s="57" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="N110" s="10" t="s">
         <v>972</v>
@@ -19450,7 +19450,7 @@
       <c r="W110" s="10"/>
       <c r="X110" s="10"/>
       <c r="Y110" s="57" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="Z110" s="15"/>
     </row>
@@ -19474,7 +19474,7 @@
         <v>1755</v>
       </c>
       <c r="K111" s="53" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="L111" s="10" t="s">
         <v>815</v>
@@ -19631,7 +19631,7 @@
         <v>1432</v>
       </c>
       <c r="J114" s="10" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="K114" s="10" t="s">
         <v>1564</v>
@@ -20069,13 +20069,13 @@
       <c r="V121" s="10"/>
       <c r="W121" s="10"/>
       <c r="X121" s="57" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="Y121" s="10" t="s">
         <v>890</v>
       </c>
       <c r="Z121" s="15" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="122" spans="1:26" ht="170" x14ac:dyDescent="0.2">
@@ -20121,13 +20121,13 @@
       <c r="R122" s="10"/>
       <c r="S122" s="10"/>
       <c r="T122" s="57" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="U122" s="10"/>
       <c r="V122" s="10"/>
       <c r="W122" s="10"/>
       <c r="X122" s="57" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="Y122" s="10" t="s">
         <v>890</v>
@@ -20196,7 +20196,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="124" spans="1:26" ht="170" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A124" s="18">
         <v>64</v>
       </c>
@@ -20254,7 +20254,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="125" spans="1:26" ht="170" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A125" s="18">
         <v>64</v>
       </c>
@@ -21087,7 +21087,7 @@
       </c>
       <c r="S139" s="10"/>
       <c r="T139" s="10" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="U139" s="10" t="s">
         <v>1095</v>
@@ -21149,7 +21149,7 @@
       </c>
       <c r="S140" s="10"/>
       <c r="T140" s="10" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="U140" s="10" t="s">
         <v>1095</v>
@@ -21580,7 +21580,7 @@
       </c>
       <c r="Z147" s="15"/>
     </row>
-    <row r="148" spans="1:26" ht="70" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A148" s="18">
         <v>78</v>
       </c>
@@ -21926,7 +21926,7 @@
       </c>
       <c r="Z153" s="15"/>
     </row>
-    <row r="154" spans="1:26" ht="187" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:26" ht="170" x14ac:dyDescent="0.2">
       <c r="A154" s="18">
         <v>82</v>
       </c>
@@ -22544,7 +22544,7 @@
       </c>
       <c r="Z164" s="15"/>
     </row>
-    <row r="165" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A165" s="18">
         <v>87</v>
       </c>
@@ -22604,7 +22604,7 @@
       </c>
       <c r="Z165" s="15"/>
     </row>
-    <row r="166" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A166" s="18">
         <v>87</v>
       </c>
@@ -22664,7 +22664,7 @@
       </c>
       <c r="Z166" s="15"/>
     </row>
-    <row r="167" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A167" s="18">
         <v>87</v>
       </c>
@@ -22761,7 +22761,7 @@
       <c r="R168" s="10"/>
       <c r="S168" s="10"/>
       <c r="T168" s="10" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="U168" s="10"/>
       <c r="V168" s="10"/>
@@ -24022,7 +24022,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="189" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A189" s="26">
         <v>96</v>
       </c>
@@ -24078,7 +24078,7 @@
       </c>
       <c r="Z189" s="15"/>
     </row>
-    <row r="190" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A190" s="26">
         <v>96</v>
       </c>
@@ -24913,7 +24913,7 @@
         <v>1020</v>
       </c>
       <c r="Z204" s="15" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="205" spans="1:27" ht="153" x14ac:dyDescent="0.2">
@@ -24933,7 +24933,7 @@
       <c r="H205" s="10"/>
       <c r="I205" s="10"/>
       <c r="J205" s="7" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="K205" s="10"/>
       <c r="L205" s="10" t="s">
@@ -24969,7 +24969,7 @@
         <v>648</v>
       </c>
       <c r="Z205" s="14" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="206" spans="1:27" ht="85" x14ac:dyDescent="0.2">
@@ -26038,7 +26038,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="223" spans="1:27" ht="136" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A223" s="18">
         <v>109</v>
       </c>
@@ -26059,7 +26059,7 @@
         <v>1808</v>
       </c>
       <c r="J223" s="7" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="K223" s="7" t="s">
         <v>1810</v>
@@ -26072,13 +26072,13 @@
       </c>
       <c r="N223" s="7"/>
       <c r="O223" s="7" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="P223" s="7" t="s">
         <v>653</v>
       </c>
       <c r="Q223" s="7" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="R223" s="7" t="s">
         <v>8</v>
@@ -26095,10 +26095,10 @@
         <v>465</v>
       </c>
       <c r="Z223" s="15" t="s">
-        <v>1894</v>
-      </c>
-    </row>
-    <row r="224" spans="1:27" ht="289" x14ac:dyDescent="0.2">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="224" spans="1:27" ht="272" x14ac:dyDescent="0.2">
       <c r="A224" s="18">
         <v>110</v>
       </c>
@@ -26119,7 +26119,7 @@
         <v>1808</v>
       </c>
       <c r="J224" s="7" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="K224" s="7" t="s">
         <v>1810</v>
@@ -26132,20 +26132,20 @@
       </c>
       <c r="N224" s="7"/>
       <c r="O224" s="7" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="P224" s="7" t="s">
         <v>653</v>
       </c>
       <c r="Q224" s="7" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="R224" s="7" t="s">
         <v>8</v>
       </c>
       <c r="S224" s="7"/>
       <c r="T224" s="7" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="U224" s="10"/>
       <c r="V224" s="10"/>
@@ -26155,7 +26155,7 @@
         <v>466</v>
       </c>
       <c r="Z224" s="15" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="225" spans="1:26" ht="85" x14ac:dyDescent="0.2">
@@ -26173,13 +26173,13 @@
         <v>1807</v>
       </c>
       <c r="H225" s="7" t="s">
+        <v>1899</v>
+      </c>
+      <c r="I225" s="53" t="s">
+        <v>1894</v>
+      </c>
+      <c r="J225" s="10" t="s">
         <v>1900</v>
-      </c>
-      <c r="I225" s="53" t="s">
-        <v>1895</v>
-      </c>
-      <c r="J225" s="10" t="s">
-        <v>1901</v>
       </c>
       <c r="K225" s="7" t="s">
         <v>1481</v>
@@ -26241,7 +26241,7 @@
         <v>1542</v>
       </c>
       <c r="J226" s="7" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="K226" s="7" t="s">
         <v>1538</v>
@@ -26267,7 +26267,7 @@
       </c>
       <c r="S226" s="10"/>
       <c r="T226" s="10" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="U226" s="10" t="s">
         <v>469</v>
@@ -26278,7 +26278,7 @@
         <v>470</v>
       </c>
       <c r="Y226" s="10" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="Z226" s="15"/>
     </row>
@@ -26303,7 +26303,7 @@
         <v>1542</v>
       </c>
       <c r="J227" s="7" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="K227" s="7" t="s">
         <v>1539</v>
@@ -26329,7 +26329,7 @@
       </c>
       <c r="S227" s="10"/>
       <c r="T227" s="10" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="U227" s="10" t="s">
         <v>469</v>
@@ -26340,7 +26340,7 @@
         <v>470</v>
       </c>
       <c r="Y227" s="10" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="Z227" s="15"/>
     </row>
@@ -26365,7 +26365,7 @@
         <v>1542</v>
       </c>
       <c r="J228" s="7" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="K228" s="7" t="s">
         <v>1539</v>
@@ -26391,7 +26391,7 @@
       </c>
       <c r="S228" s="10"/>
       <c r="T228" s="10" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="U228" s="10" t="s">
         <v>469</v>
@@ -26402,7 +26402,7 @@
         <v>470</v>
       </c>
       <c r="Y228" s="10" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="Z228" s="15"/>
     </row>
@@ -26427,7 +26427,7 @@
         <v>1542</v>
       </c>
       <c r="J229" s="7" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="K229" s="7" t="s">
         <v>1539</v>
@@ -26453,7 +26453,7 @@
       </c>
       <c r="S229" s="10"/>
       <c r="T229" s="57" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="U229" s="10"/>
       <c r="V229" s="10"/>
@@ -26461,7 +26461,7 @@
       <c r="X229" s="10"/>
       <c r="Y229" s="10"/>
       <c r="Z229" s="15" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="230" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -26479,13 +26479,13 @@
         <v>39</v>
       </c>
       <c r="H230" s="7" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="I230" s="7" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="J230" s="7" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="K230" s="7" t="s">
         <v>815</v>
@@ -26497,7 +26497,7 @@
         <v>1119</v>
       </c>
       <c r="N230" s="57" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="O230" s="57">
         <v>10</v>
@@ -26506,7 +26506,7 @@
         <v>653</v>
       </c>
       <c r="Q230" s="57" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="R230" s="10">
         <v>838</v>
@@ -26522,10 +26522,10 @@
       <c r="W230" s="10"/>
       <c r="X230" s="10"/>
       <c r="Y230" s="10" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="Z230" s="15" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="231" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -26543,13 +26543,13 @@
         <v>39</v>
       </c>
       <c r="H231" s="7" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="I231" s="7" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="J231" s="7" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="K231" s="7" t="s">
         <v>815</v>
@@ -26561,7 +26561,7 @@
         <v>1119</v>
       </c>
       <c r="N231" s="57" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="O231" s="57">
         <v>10</v>
@@ -26570,14 +26570,14 @@
         <v>653</v>
       </c>
       <c r="Q231" s="57" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="R231" s="10">
         <v>838</v>
       </c>
       <c r="S231" s="10"/>
       <c r="T231" s="10" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="U231" s="57" t="s">
         <v>1004</v>
@@ -26586,7 +26586,7 @@
       <c r="W231" s="10"/>
       <c r="X231" s="10"/>
       <c r="Y231" s="10" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="Z231" s="15"/>
     </row>
@@ -26605,13 +26605,13 @@
         <v>39</v>
       </c>
       <c r="H232" s="7" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="I232" s="7" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="J232" s="7" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="K232" s="7" t="s">
         <v>815</v>
@@ -26623,7 +26623,7 @@
         <v>1119</v>
       </c>
       <c r="N232" s="57" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="O232" s="57">
         <v>20</v>
@@ -26632,14 +26632,14 @@
         <v>779</v>
       </c>
       <c r="Q232" s="57" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="R232" s="10">
         <v>838</v>
       </c>
       <c r="S232" s="10"/>
       <c r="T232" s="10" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="U232" s="57" t="s">
         <v>1004</v>
@@ -26648,10 +26648,10 @@
       <c r="W232" s="10"/>
       <c r="X232" s="10"/>
       <c r="Y232" s="10" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="Z232" s="15" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="233" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -26669,13 +26669,13 @@
         <v>39</v>
       </c>
       <c r="H233" s="7" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="I233" s="7" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="J233" s="7" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="K233" s="7" t="s">
         <v>815</v>
@@ -26687,7 +26687,7 @@
         <v>1119</v>
       </c>
       <c r="N233" s="57" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="O233" s="57">
         <v>19</v>
@@ -26696,14 +26696,14 @@
         <v>779</v>
       </c>
       <c r="Q233" s="57" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="R233" s="10">
         <v>838</v>
       </c>
       <c r="S233" s="10"/>
       <c r="T233" s="10" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="U233" s="57" t="s">
         <v>1004</v>
@@ -26712,7 +26712,7 @@
       <c r="W233" s="10"/>
       <c r="X233" s="10"/>
       <c r="Y233" s="10" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="Z233" s="15"/>
     </row>
@@ -26731,13 +26731,13 @@
         <v>39</v>
       </c>
       <c r="H234" s="7" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="I234" s="7" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="J234" s="7" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="K234" s="7" t="s">
         <v>815</v>
@@ -26749,7 +26749,7 @@
         <v>1119</v>
       </c>
       <c r="N234" s="57" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="O234" s="53">
         <v>18</v>
@@ -26758,7 +26758,7 @@
         <v>779</v>
       </c>
       <c r="Q234" s="57" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="R234" s="10">
         <v>838</v>
@@ -26774,10 +26774,10 @@
       <c r="W234" s="10"/>
       <c r="X234" s="10"/>
       <c r="Y234" s="10" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="Z234" s="15" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="235" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -26795,13 +26795,13 @@
         <v>39</v>
       </c>
       <c r="H235" s="7" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="I235" s="7" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="J235" s="7" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="K235" s="7" t="s">
         <v>815</v>
@@ -26822,14 +26822,14 @@
         <v>653</v>
       </c>
       <c r="Q235" s="57" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="R235" s="10">
         <v>838</v>
       </c>
       <c r="S235" s="10"/>
       <c r="T235" s="10" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="U235" s="57" t="s">
         <v>1004</v>
@@ -26838,11 +26838,11 @@
       <c r="W235" s="10"/>
       <c r="X235" s="10"/>
       <c r="Y235" s="10" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="Z235" s="15"/>
     </row>
-    <row r="236" spans="1:26" ht="356" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:26" ht="340" x14ac:dyDescent="0.2">
       <c r="A236" s="18">
         <v>114</v>
       </c>
@@ -26854,25 +26854,25 @@
         <v>591</v>
       </c>
       <c r="G236" s="7" t="s">
+        <v>1824</v>
+      </c>
+      <c r="H236" s="7" t="s">
+        <v>1828</v>
+      </c>
+      <c r="I236" s="7" t="s">
+        <v>1827</v>
+      </c>
+      <c r="J236" s="7" t="s">
+        <v>1826</v>
+      </c>
+      <c r="K236" s="7" t="s">
         <v>1825</v>
-      </c>
-      <c r="H236" s="7" t="s">
-        <v>1829</v>
-      </c>
-      <c r="I236" s="7" t="s">
-        <v>1828</v>
-      </c>
-      <c r="J236" s="7" t="s">
-        <v>1827</v>
-      </c>
-      <c r="K236" s="7" t="s">
-        <v>1826</v>
       </c>
       <c r="L236" s="7" t="s">
         <v>815</v>
       </c>
       <c r="M236" s="10" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="N236" s="10"/>
       <c r="O236" s="10"/>
@@ -26892,10 +26892,10 @@
       <c r="W236" s="10"/>
       <c r="X236" s="10"/>
       <c r="Y236" s="10" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="Z236" s="15" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="237" spans="1:26" ht="153" x14ac:dyDescent="0.2">
@@ -26910,16 +26910,16 @@
         <v>591</v>
       </c>
       <c r="G237" s="7" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="H237" s="53" t="s">
+        <v>1915</v>
+      </c>
+      <c r="I237" s="53" t="s">
         <v>1916</v>
       </c>
-      <c r="I237" s="53" t="s">
-        <v>1917</v>
-      </c>
       <c r="J237" s="10" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="K237" s="10"/>
       <c r="L237" s="10" t="s">
@@ -26998,7 +26998,7 @@
       <c r="W238" s="10"/>
       <c r="X238" s="10"/>
       <c r="Y238" s="10" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="Z238" s="15" t="s">
         <v>1502</v>
@@ -27054,7 +27054,7 @@
       <c r="W239" s="10"/>
       <c r="X239" s="10"/>
       <c r="Y239" s="10" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="Z239" s="15" t="s">
         <v>1662</v>
@@ -27108,10 +27108,10 @@
       <c r="W240" s="10"/>
       <c r="X240" s="10"/>
       <c r="Y240" s="10" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="Z240" s="15" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="241" spans="1:26" ht="170" x14ac:dyDescent="0.2">
@@ -27164,7 +27164,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="242" spans="1:26" ht="170" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A242" s="18">
         <v>118</v>
       </c>
@@ -27216,7 +27216,7 @@
       </c>
       <c r="Z242" s="15"/>
     </row>
-    <row r="243" spans="1:26" ht="153" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A243" s="18">
         <v>119</v>
       </c>
@@ -27270,7 +27270,7 @@
       </c>
       <c r="Z243" s="15"/>
     </row>
-    <row r="244" spans="1:26" ht="153" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A244" s="18">
         <v>119</v>
       </c>
@@ -27324,7 +27324,7 @@
       </c>
       <c r="Z244" s="15"/>
     </row>
-    <row r="245" spans="1:26" ht="153" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A245" s="18">
         <v>119</v>
       </c>
@@ -27378,7 +27378,7 @@
       </c>
       <c r="Z245" s="15"/>
     </row>
-    <row r="246" spans="1:26" ht="153" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A246" s="18">
         <v>120</v>
       </c>
@@ -27434,7 +27434,7 @@
       </c>
       <c r="Z246" s="15"/>
     </row>
-    <row r="247" spans="1:26" ht="153" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A247" s="18">
         <v>120</v>
       </c>
@@ -27490,7 +27490,7 @@
       </c>
       <c r="Z247" s="15"/>
     </row>
-    <row r="248" spans="1:26" ht="153" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A248" s="18">
         <v>120</v>
       </c>
@@ -27600,13 +27600,13 @@
       <c r="W249" s="10"/>
       <c r="X249" s="10"/>
       <c r="Y249" s="10" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="Z249" s="15" t="s">
         <v>1721</v>
       </c>
     </row>
-    <row r="250" spans="1:26" ht="51" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A250" s="18">
         <v>122</v>
       </c>
@@ -27712,7 +27712,7 @@
         <v>1116</v>
       </c>
       <c r="U251" s="7" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="V251" s="10"/>
       <c r="W251" s="10"/>
@@ -27888,7 +27888,7 @@
       </c>
       <c r="Z254" s="15"/>
     </row>
-    <row r="255" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A255" s="18">
         <v>127</v>
       </c>
@@ -27961,13 +27961,13 @@
         <v>46</v>
       </c>
       <c r="H256" s="10" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="I256" s="10" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="J256" s="10" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="K256" s="7" t="s">
         <v>298</v>
@@ -28119,7 +28119,7 @@
       <c r="H259" s="10"/>
       <c r="I259" s="10"/>
       <c r="J259" s="10" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="K259" s="10"/>
       <c r="L259" s="10" t="s">
@@ -28171,10 +28171,10 @@
         <v>1700</v>
       </c>
       <c r="J260" s="57" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="K260" s="57" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="L260" s="57" t="s">
         <v>815</v>
@@ -28197,15 +28197,15 @@
       </c>
       <c r="U260" s="10"/>
       <c r="V260" s="57" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="W260" s="10"/>
       <c r="X260" s="10"/>
       <c r="Y260" s="10" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="Z260" s="15" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="261" spans="1:26" ht="68" x14ac:dyDescent="0.2">
@@ -28259,7 +28259,7 @@
         <v>603</v>
       </c>
       <c r="Z261" s="15" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="262" spans="1:26" ht="102" x14ac:dyDescent="0.2">
@@ -28362,7 +28362,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="264" spans="1:26" ht="153" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A264" s="18">
         <v>136</v>
       </c>
@@ -28411,10 +28411,10 @@
       <c r="V264" s="10"/>
       <c r="W264" s="10"/>
       <c r="X264" s="7" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="Y264" s="7" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="Z264" s="15" t="s">
         <v>102</v>
@@ -28532,7 +28532,7 @@
         <v>799</v>
       </c>
       <c r="Y266" s="10" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="Z266" s="15"/>
     </row>
@@ -28592,7 +28592,7 @@
         <v>799</v>
       </c>
       <c r="Y267" s="10" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="Z267" s="15"/>
     </row>
@@ -28652,7 +28652,7 @@
         <v>799</v>
       </c>
       <c r="Y268" s="10" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="Z268" s="15"/>
     </row>
@@ -28673,7 +28673,7 @@
       <c r="H269" s="10"/>
       <c r="I269" s="10"/>
       <c r="J269" s="7" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="K269" s="7" t="s">
         <v>1446</v>
@@ -28771,7 +28771,7 @@
         <v>1166</v>
       </c>
       <c r="Z270" s="14" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="271" spans="1:26" ht="34" x14ac:dyDescent="0.2">
@@ -29431,7 +29431,7 @@
       <c r="H282" s="10"/>
       <c r="I282" s="10"/>
       <c r="J282" s="10" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="K282" s="10"/>
       <c r="L282" s="10" t="s">
@@ -29479,7 +29479,7 @@
       <c r="H283" s="10"/>
       <c r="I283" s="10"/>
       <c r="J283" s="7" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="K283" s="7" t="s">
         <v>815</v>
@@ -29512,7 +29512,7 @@
         <v>1032</v>
       </c>
       <c r="Y283" s="10" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="Z283" s="13" t="s">
         <v>35</v>
@@ -29542,7 +29542,7 @@
         <v>1813</v>
       </c>
       <c r="K284" s="7" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="L284" s="7" t="s">
         <v>815</v>
@@ -29551,7 +29551,7 @@
         <v>498</v>
       </c>
       <c r="N284" s="57" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="O284" s="57">
         <v>3</v>
@@ -29560,14 +29560,14 @@
         <v>653</v>
       </c>
       <c r="Q284" s="7" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="R284" s="10">
         <v>843</v>
       </c>
       <c r="S284" s="10"/>
       <c r="T284" s="10" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="U284" s="10"/>
       <c r="V284" s="10"/>
@@ -29576,10 +29576,10 @@
         <v>641</v>
       </c>
       <c r="Y284" s="7" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="Z284" s="15" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="285" spans="1:26" ht="85" x14ac:dyDescent="0.2">
@@ -29606,7 +29606,7 @@
         <v>1813</v>
       </c>
       <c r="K285" s="7" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="L285" s="7" t="s">
         <v>815</v>
@@ -29624,14 +29624,14 @@
         <v>653</v>
       </c>
       <c r="Q285" s="7" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="R285" s="10">
         <v>843</v>
       </c>
       <c r="S285" s="10"/>
       <c r="T285" s="10" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="U285" s="10"/>
       <c r="V285" s="10"/>
@@ -29640,10 +29640,10 @@
         <v>641</v>
       </c>
       <c r="Y285" s="7" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="Z285" s="15" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="286" spans="1:26" ht="51" x14ac:dyDescent="0.2">
@@ -29670,7 +29670,7 @@
         <v>1813</v>
       </c>
       <c r="K286" s="7" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="L286" s="7" t="s">
         <v>815</v>
@@ -29688,14 +29688,14 @@
         <v>779</v>
       </c>
       <c r="Q286" s="7" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="R286" s="10">
         <v>843</v>
       </c>
       <c r="S286" s="10"/>
       <c r="T286" s="10" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="U286" s="10"/>
       <c r="V286" s="10"/>
@@ -29704,10 +29704,10 @@
         <v>641</v>
       </c>
       <c r="Y286" s="7" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="Z286" s="15" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="287" spans="1:26" ht="51" x14ac:dyDescent="0.2">
@@ -29734,7 +29734,7 @@
         <v>1813</v>
       </c>
       <c r="K287" s="7" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="L287" s="7" t="s">
         <v>815</v>
@@ -29752,14 +29752,14 @@
         <v>653</v>
       </c>
       <c r="Q287" s="7" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="R287" s="10">
         <v>843</v>
       </c>
       <c r="S287" s="10"/>
       <c r="T287" s="10" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="U287" s="10"/>
       <c r="V287" s="10"/>
@@ -29768,10 +29768,10 @@
         <v>641</v>
       </c>
       <c r="Y287" s="7" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="Z287" s="15" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="288" spans="1:26" ht="119" x14ac:dyDescent="0.2">
@@ -29798,7 +29798,7 @@
         <v>1813</v>
       </c>
       <c r="K288" s="7" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="L288" s="7" t="s">
         <v>815</v>
@@ -29807,23 +29807,23 @@
         <v>498</v>
       </c>
       <c r="N288" s="57" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="O288" s="57" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="P288" s="57" t="s">
         <v>779</v>
       </c>
       <c r="Q288" s="7" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="R288" s="10">
         <v>843</v>
       </c>
       <c r="S288" s="10"/>
       <c r="T288" s="10" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="U288" s="10"/>
       <c r="V288" s="10"/>
@@ -29832,10 +29832,10 @@
         <v>641</v>
       </c>
       <c r="Y288" s="7" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="Z288" s="15" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="289" spans="1:26" ht="119" x14ac:dyDescent="0.2">
@@ -29862,7 +29862,7 @@
         <v>1813</v>
       </c>
       <c r="K289" s="7" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="L289" s="7" t="s">
         <v>815</v>
@@ -29871,23 +29871,23 @@
         <v>498</v>
       </c>
       <c r="N289" s="57" t="s">
+        <v>1973</v>
+      </c>
+      <c r="O289" s="57" t="s">
         <v>1974</v>
-      </c>
-      <c r="O289" s="57" t="s">
-        <v>1975</v>
       </c>
       <c r="P289" s="57" t="s">
         <v>653</v>
       </c>
       <c r="Q289" s="7" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="R289" s="10">
         <v>843</v>
       </c>
       <c r="S289" s="10"/>
       <c r="T289" s="10" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="U289" s="10"/>
       <c r="V289" s="10"/>
@@ -29896,10 +29896,10 @@
         <v>641</v>
       </c>
       <c r="Y289" s="7" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="Z289" s="15" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="290" spans="1:26" ht="51" x14ac:dyDescent="0.2">
@@ -29917,13 +29917,13 @@
         <v>39</v>
       </c>
       <c r="H290" s="10" t="s">
+        <v>1822</v>
+      </c>
+      <c r="I290" s="10" t="s">
+        <v>1821</v>
+      </c>
+      <c r="J290" s="10" t="s">
         <v>1823</v>
-      </c>
-      <c r="I290" s="10" t="s">
-        <v>1822</v>
-      </c>
-      <c r="J290" s="10" t="s">
-        <v>1824</v>
       </c>
       <c r="K290" s="7" t="s">
         <v>194</v>
@@ -29981,13 +29981,13 @@
         <v>39</v>
       </c>
       <c r="H291" s="10" t="s">
+        <v>1822</v>
+      </c>
+      <c r="I291" s="10" t="s">
+        <v>1821</v>
+      </c>
+      <c r="J291" s="10" t="s">
         <v>1823</v>
-      </c>
-      <c r="I291" s="10" t="s">
-        <v>1822</v>
-      </c>
-      <c r="J291" s="10" t="s">
-        <v>1824</v>
       </c>
       <c r="K291" s="7" t="s">
         <v>194</v>
@@ -30045,13 +30045,13 @@
         <v>39</v>
       </c>
       <c r="H292" s="10" t="s">
+        <v>1822</v>
+      </c>
+      <c r="I292" s="10" t="s">
+        <v>1821</v>
+      </c>
+      <c r="J292" s="10" t="s">
         <v>1823</v>
-      </c>
-      <c r="I292" s="10" t="s">
-        <v>1822</v>
-      </c>
-      <c r="J292" s="10" t="s">
-        <v>1824</v>
       </c>
       <c r="K292" s="7" t="s">
         <v>194</v>
@@ -30109,13 +30109,13 @@
         <v>39</v>
       </c>
       <c r="H293" s="10" t="s">
+        <v>1822</v>
+      </c>
+      <c r="I293" s="10" t="s">
+        <v>1821</v>
+      </c>
+      <c r="J293" s="10" t="s">
         <v>1823</v>
-      </c>
-      <c r="I293" s="10" t="s">
-        <v>1822</v>
-      </c>
-      <c r="J293" s="10" t="s">
-        <v>1824</v>
       </c>
       <c r="K293" s="7" t="s">
         <v>162</v>
@@ -30173,13 +30173,13 @@
         <v>1577</v>
       </c>
       <c r="H294" s="53" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="I294" s="53" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="J294" s="10" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="K294" s="7" t="s">
         <v>388</v>
@@ -30211,16 +30211,16 @@
       <c r="V294" s="10"/>
       <c r="W294" s="7"/>
       <c r="X294" s="7" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="Y294" s="7" t="s">
         <v>831</v>
       </c>
       <c r="Z294" s="15" t="s">
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="295" spans="1:26" ht="85" x14ac:dyDescent="0.2">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="295" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A295" s="18">
         <v>151</v>
       </c>
@@ -30731,7 +30731,7 @@
       <c r="H305" s="10"/>
       <c r="I305" s="10"/>
       <c r="J305" s="10" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="K305" s="10"/>
       <c r="L305" s="10" t="s">
@@ -30757,7 +30757,7 @@
       <c r="X305" s="10"/>
       <c r="Y305" s="10"/>
       <c r="Z305" s="15" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="306" spans="1:27" ht="68" x14ac:dyDescent="0.2">
@@ -30779,7 +30779,7 @@
       <c r="H306" s="10"/>
       <c r="I306" s="10"/>
       <c r="J306" s="10" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="K306" s="10"/>
       <c r="L306" s="10" t="s">
@@ -30805,10 +30805,10 @@
       <c r="X306" s="10"/>
       <c r="Y306" s="10"/>
       <c r="Z306" s="15" t="s">
-        <v>1959</v>
-      </c>
-    </row>
-    <row r="307" spans="1:27" ht="136" x14ac:dyDescent="0.2">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="307" spans="1:27" ht="119" x14ac:dyDescent="0.2">
       <c r="A307" s="7">
         <v>161</v>
       </c>
@@ -31037,7 +31037,7 @@
       <c r="Y311" s="10"/>
       <c r="Z311" s="15"/>
     </row>
-    <row r="312" spans="1:27" ht="153" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:27" ht="136" x14ac:dyDescent="0.2">
       <c r="A312" s="26">
         <v>166</v>
       </c>
@@ -31441,7 +31441,7 @@
       <c r="W319" s="10"/>
       <c r="X319" s="10"/>
       <c r="Y319" s="10" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="Z319" s="15"/>
     </row>
@@ -31506,13 +31506,13 @@
         <v>1470</v>
       </c>
       <c r="H321" s="7" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="I321" s="7" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="J321" s="7" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="K321" s="7" t="s">
         <v>245</v>
@@ -31559,22 +31559,22 @@
         <v>591</v>
       </c>
       <c r="G322" s="7" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="H322" s="7" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="I322" s="7" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="J322" s="7" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="K322" s="7" t="s">
         <v>1729</v>
       </c>
       <c r="L322" s="7" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="M322" s="7" t="s">
         <v>751</v>
@@ -31588,7 +31588,7 @@
       </c>
       <c r="Q322" s="7"/>
       <c r="R322" s="7" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="S322" s="10"/>
       <c r="T322" s="7">
@@ -31598,14 +31598,14 @@
       <c r="V322" s="10"/>
       <c r="W322" s="10"/>
       <c r="X322" s="7" t="s">
+        <v>1922</v>
+      </c>
+      <c r="Y322" s="7" t="s">
         <v>1923</v>
       </c>
-      <c r="Y322" s="7" t="s">
-        <v>1924</v>
-      </c>
       <c r="Z322" s="15"/>
     </row>
-    <row r="323" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A323" s="18">
         <v>173</v>
       </c>
@@ -31713,7 +31713,7 @@
       </c>
       <c r="Z324" s="15"/>
     </row>
-    <row r="325" spans="1:26" ht="153" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A325" s="18">
         <v>175</v>
       </c>
@@ -31756,10 +31756,10 @@
       <c r="V325" s="10"/>
       <c r="W325" s="10"/>
       <c r="X325" s="7" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="Y325" s="7" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="Z325" s="15"/>
     </row>
@@ -32016,19 +32016,19 @@
         <v>249</v>
       </c>
       <c r="H331" s="53" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="I331" s="53" t="s">
+        <v>1906</v>
+      </c>
+      <c r="J331" s="53" t="s">
         <v>1907</v>
-      </c>
-      <c r="J331" s="53" t="s">
-        <v>1908</v>
       </c>
       <c r="K331" s="7" t="s">
         <v>87</v>
       </c>
       <c r="L331" s="7" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="M331" s="7" t="s">
         <v>1178</v>
@@ -32052,14 +32052,14 @@
       <c r="V331" s="10"/>
       <c r="W331" s="10"/>
       <c r="X331" s="7" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="Y331" s="10"/>
       <c r="Z331" s="54" t="s">
-        <v>1925</v>
-      </c>
-    </row>
-    <row r="332" spans="1:26" ht="187" x14ac:dyDescent="0.2">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="332" spans="1:26" ht="170" x14ac:dyDescent="0.2">
       <c r="A332" s="18">
         <v>182</v>
       </c>
@@ -32221,7 +32221,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="335" spans="1:26" ht="289" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:26" ht="255" x14ac:dyDescent="0.2">
       <c r="A335" s="18">
         <v>184</v>
       </c>
@@ -32319,7 +32319,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="337" spans="1:26" ht="340" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:26" ht="323" x14ac:dyDescent="0.2">
       <c r="A337" s="18">
         <v>186</v>
       </c>
@@ -32338,10 +32338,10 @@
       <c r="H337" s="57"/>
       <c r="I337" s="57"/>
       <c r="J337" s="57" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="K337" s="57" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="L337" s="57" t="s">
         <v>815</v>
@@ -32358,7 +32358,7 @@
       </c>
       <c r="Q337" s="57"/>
       <c r="R337" s="57" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="S337" s="57">
         <v>1881</v>
@@ -32370,13 +32370,13 @@
       <c r="V337" s="10"/>
       <c r="W337" s="10"/>
       <c r="X337" s="57" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="Y337" s="57" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="Z337" s="14" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="338" spans="1:26" ht="85" x14ac:dyDescent="0.2">
@@ -33099,14 +33099,14 @@
       <c r="Q352" s="10"/>
       <c r="R352" s="10"/>
       <c r="S352" s="10" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="T352" s="10"/>
       <c r="U352" s="10"/>
       <c r="V352" s="10"/>
       <c r="W352" s="10"/>
       <c r="X352" s="7" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="Y352" s="10"/>
       <c r="Z352" s="14" t="s">
@@ -33361,7 +33361,7 @@
       </c>
       <c r="Z357" s="14"/>
     </row>
-    <row r="358" spans="1:26" ht="68" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A358" s="25">
         <v>202</v>
       </c>
@@ -33413,7 +33413,7 @@
       </c>
       <c r="Z358" s="14"/>
     </row>
-    <row r="359" spans="1:26" ht="153" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:26" ht="119" x14ac:dyDescent="0.2">
       <c r="A359" s="26">
         <v>202</v>
       </c>
@@ -34278,7 +34278,7 @@
       </c>
       <c r="S375" s="6"/>
       <c r="T375" s="6" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="U375" s="6"/>
       <c r="V375" s="6"/>
@@ -34293,7 +34293,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="376" spans="1:26" ht="119" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A376" s="19">
         <v>213</v>
       </c>
@@ -34349,7 +34349,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="377" spans="1:26" ht="119" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A377" s="19">
         <v>213</v>
       </c>
@@ -34405,7 +34405,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="378" spans="1:26" ht="119" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A378" s="19">
         <v>213</v>
       </c>
@@ -34479,7 +34479,7 @@
         <v>1507</v>
       </c>
       <c r="I379" s="6" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="J379" s="6" t="s">
         <v>1506</v>
@@ -34515,7 +34515,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="380" spans="1:26" ht="255" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:26" ht="238" x14ac:dyDescent="0.2">
       <c r="A380" s="19">
         <v>215</v>
       </c>
@@ -35051,14 +35051,14 @@
       <c r="Y388" s="6"/>
       <c r="Z388" s="14"/>
     </row>
-    <row r="389" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A389" s="19">
         <v>218</v>
       </c>
       <c r="B389" s="6"/>
       <c r="C389" s="6"/>
       <c r="D389" s="41" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="E389" s="6"/>
       <c r="F389" s="7" t="s">
@@ -35209,7 +35209,7 @@
       <c r="Y391" s="6"/>
       <c r="Z391" s="14"/>
     </row>
-    <row r="392" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A392" s="19">
         <v>220</v>
       </c>
@@ -35582,10 +35582,10 @@
         <v>40</v>
       </c>
       <c r="H399" s="6" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="I399" s="6" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="J399" s="7" t="s">
         <v>1610</v>
@@ -35614,7 +35614,7 @@
         <v>1268</v>
       </c>
       <c r="T399" s="7" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="U399" s="7"/>
       <c r="V399" s="7"/>
@@ -35640,10 +35640,10 @@
         <v>40</v>
       </c>
       <c r="H400" s="6" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="I400" s="6" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="J400" s="7" t="s">
         <v>294</v>
@@ -35672,7 +35672,7 @@
         <v>1268</v>
       </c>
       <c r="T400" s="7" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="U400" s="7"/>
       <c r="V400" s="7"/>
@@ -35698,10 +35698,10 @@
         <v>210</v>
       </c>
       <c r="H401" s="6" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="I401" s="6" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="J401" s="7" t="s">
         <v>295</v>
@@ -35746,10 +35746,10 @@
         <v>210</v>
       </c>
       <c r="H402" s="6" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="I402" s="6" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="J402" s="7" t="s">
         <v>295</v>
@@ -35794,10 +35794,10 @@
         <v>210</v>
       </c>
       <c r="H403" s="6" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="I403" s="6" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="J403" s="7" t="s">
         <v>295</v>
@@ -35916,7 +35916,7 @@
       <c r="V405" s="7"/>
       <c r="W405" s="7"/>
       <c r="X405" s="7" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="Y405" s="7"/>
       <c r="Z405" s="15" t="s">
@@ -36159,7 +36159,7 @@
       <c r="I410" s="10"/>
       <c r="J410" s="7"/>
       <c r="K410" s="7" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="L410" s="7"/>
       <c r="M410" s="6" t="s">
@@ -36235,7 +36235,7 @@
     </row>
     <row r="412" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A412" s="47" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="B412" s="7"/>
       <c r="C412" s="7"/>
@@ -36274,7 +36274,7 @@
       <c r="V412" s="7"/>
       <c r="W412" s="7"/>
       <c r="X412" s="7" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="Y412" s="7"/>
       <c r="Z412" s="14"/>
@@ -36294,20 +36294,20 @@
         <v>1591</v>
       </c>
       <c r="H413" s="57" t="s">
+        <v>2048</v>
+      </c>
+      <c r="I413" s="57" t="s">
         <v>2049</v>
       </c>
-      <c r="I413" s="57" t="s">
+      <c r="J413" s="57" t="s">
         <v>2050</v>
-      </c>
-      <c r="J413" s="57" t="s">
-        <v>2051</v>
       </c>
       <c r="K413" s="7" t="s">
         <v>1627</v>
       </c>
       <c r="L413" s="7"/>
       <c r="M413" s="57" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="N413" s="57" t="s">
         <v>1628</v>
@@ -36319,24 +36319,24 @@
         <v>653</v>
       </c>
       <c r="Q413" s="7" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="R413" s="57">
         <v>1360</v>
       </c>
       <c r="S413" s="6"/>
       <c r="T413" s="57" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="U413" s="7"/>
       <c r="V413" s="7"/>
       <c r="W413" s="7"/>
       <c r="X413" s="7"/>
       <c r="Y413" s="7" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="Z413" s="15" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="414" spans="1:26" s="42" customFormat="1" ht="153" x14ac:dyDescent="0.15">
@@ -36354,20 +36354,20 @@
         <v>1591</v>
       </c>
       <c r="H414" s="57" t="s">
+        <v>2048</v>
+      </c>
+      <c r="I414" s="57" t="s">
         <v>2049</v>
       </c>
-      <c r="I414" s="57" t="s">
+      <c r="J414" s="57" t="s">
         <v>2050</v>
-      </c>
-      <c r="J414" s="57" t="s">
-        <v>2051</v>
       </c>
       <c r="K414" s="7" t="s">
         <v>1627</v>
       </c>
       <c r="L414" s="7"/>
       <c r="M414" s="57" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="N414" s="57" t="s">
         <v>1629</v>
@@ -36379,35 +36379,35 @@
         <v>653</v>
       </c>
       <c r="Q414" s="7" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="R414" s="57">
         <v>1360</v>
       </c>
       <c r="S414" s="6"/>
       <c r="T414" s="57" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="U414" s="7"/>
       <c r="V414" s="7"/>
       <c r="W414" s="7"/>
       <c r="X414" s="7"/>
       <c r="Y414" s="7" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="Z414" s="15" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="415" spans="1:26" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A415" s="47" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B415" s="7"/>
       <c r="C415" s="7"/>
       <c r="D415" s="7"/>
       <c r="E415" s="7" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="F415" s="7" t="s">
         <v>722</v>
@@ -36418,37 +36418,37 @@
       <c r="H415" s="6"/>
       <c r="I415" s="6"/>
       <c r="J415" s="57" t="s">
+        <v>2023</v>
+      </c>
+      <c r="K415" s="7" t="s">
         <v>2024</v>
-      </c>
-      <c r="K415" s="7" t="s">
-        <v>2025</v>
       </c>
       <c r="L415" s="7"/>
       <c r="M415" s="57" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="N415" s="6"/>
       <c r="O415" s="6">
         <v>6</v>
       </c>
       <c r="P415" s="7" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="Q415" s="7"/>
       <c r="R415" s="57" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="S415" s="57">
         <v>1881</v>
       </c>
       <c r="T415" s="53" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="U415" s="7"/>
       <c r="V415" s="7"/>
       <c r="W415" s="7"/>
       <c r="X415" s="57" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="Y415" s="7"/>
       <c r="Z415" s="15"/>
@@ -36461,7 +36461,7 @@
       <c r="C416" s="7"/>
       <c r="D416" s="7"/>
       <c r="E416" s="7" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="F416" s="7" t="s">
         <v>722</v>
@@ -36472,14 +36472,14 @@
       <c r="H416" s="6"/>
       <c r="I416" s="6"/>
       <c r="J416" s="53" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="K416" s="53" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="L416" s="7"/>
       <c r="M416" s="57" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="N416" s="6"/>
       <c r="O416" s="6">
@@ -36494,17 +36494,17 @@
         <v>614</v>
       </c>
       <c r="T416" s="57" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="U416" s="7"/>
       <c r="V416" s="7"/>
       <c r="W416" s="7"/>
       <c r="X416" s="57" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="Y416" s="7"/>
       <c r="Z416" s="15" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="417" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
@@ -36519,19 +36519,19 @@
         <v>591</v>
       </c>
       <c r="G417" s="57" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="H417" s="57" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="I417" s="6"/>
       <c r="J417" s="6"/>
       <c r="K417" s="57" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="L417" s="7"/>
       <c r="M417" s="6" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="N417" s="7"/>
       <c r="O417" s="7">
@@ -36541,23 +36541,23 @@
         <v>779</v>
       </c>
       <c r="Q417" s="7" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="R417" s="7"/>
       <c r="S417" s="7" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="T417" s="57" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="U417" s="7"/>
       <c r="V417" s="7"/>
       <c r="W417" s="7"/>
       <c r="X417" s="57" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="Y417" s="7" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="Z417" s="15" t="s">
         <v>1767</v>
@@ -36575,45 +36575,45 @@
         <v>591</v>
       </c>
       <c r="G418" s="57" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="H418" s="57" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="I418" s="6"/>
       <c r="J418" s="6"/>
       <c r="K418" s="57" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="L418" s="7"/>
       <c r="M418" s="6" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="N418" s="7"/>
       <c r="O418" s="7" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="P418" s="7" t="s">
         <v>779</v>
       </c>
       <c r="Q418" s="7" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="R418" s="7"/>
       <c r="S418" s="7" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="T418" s="57" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="U418" s="7"/>
       <c r="V418" s="7"/>
       <c r="W418" s="7"/>
       <c r="X418" s="57" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="Y418" s="7" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="Z418" s="15" t="s">
         <v>1767</v>
@@ -36719,7 +36719,7 @@
     </row>
     <row r="421" spans="1:29" ht="85" x14ac:dyDescent="0.2">
       <c r="A421" s="47" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B421" s="7"/>
       <c r="C421" s="7"/>
@@ -36769,7 +36769,7 @@
     </row>
     <row r="422" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A422" s="26" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B422" s="7"/>
       <c r="C422" s="7"/>
@@ -36827,7 +36827,7 @@
     </row>
     <row r="423" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A423" s="47" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="B423" s="7"/>
       <c r="C423" s="7"/>
@@ -36869,9 +36869,9 @@
         <v>1759</v>
       </c>
     </row>
-    <row r="424" spans="1:29" ht="68" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A424" s="47" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="B424" s="7"/>
       <c r="C424" s="7"/>
@@ -36885,11 +36885,11 @@
       <c r="I424" s="53"/>
       <c r="J424" s="55"/>
       <c r="K424" s="7" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="L424" s="7"/>
       <c r="M424" s="57" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="N424" s="7"/>
       <c r="O424" s="7"/>
@@ -36908,12 +36908,12 @@
       <c r="X424" s="53"/>
       <c r="Y424" s="7"/>
       <c r="Z424" s="15" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="425" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A425" s="47" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="B425" s="7"/>
       <c r="C425" s="7"/>
@@ -36929,11 +36929,11 @@
       <c r="I425" s="6"/>
       <c r="J425" s="7"/>
       <c r="K425" s="53" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="L425" s="7"/>
       <c r="M425" s="53" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="N425" s="7"/>
       <c r="O425" s="6">
@@ -36944,21 +36944,21 @@
       </c>
       <c r="Q425" s="7"/>
       <c r="R425" s="7" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="S425" s="7"/>
       <c r="T425" s="7" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="U425" s="7"/>
       <c r="V425" s="7"/>
       <c r="W425" s="7"/>
       <c r="X425" s="53"/>
       <c r="Y425" s="53" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="Z425" s="15" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="AA425"/>
       <c r="AB425"/>
@@ -36966,7 +36966,7 @@
     </row>
     <row r="426" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A426" s="47" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="B426" s="7"/>
       <c r="C426" s="7"/>
@@ -36982,11 +36982,11 @@
       <c r="I426" s="6"/>
       <c r="J426" s="7"/>
       <c r="K426" s="53" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="L426" s="7"/>
       <c r="M426" s="53" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="N426" s="7"/>
       <c r="O426" s="6">
@@ -36997,21 +36997,21 @@
       </c>
       <c r="Q426" s="7"/>
       <c r="R426" s="7" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="S426" s="7"/>
       <c r="T426" s="7" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="U426" s="7"/>
       <c r="V426" s="7"/>
       <c r="W426" s="7"/>
       <c r="X426" s="53"/>
       <c r="Y426" s="53" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="Z426" s="15" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="AA426"/>
       <c r="AB426"/>
@@ -37019,7 +37019,7 @@
     </row>
     <row r="427" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A427" s="47" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="B427" s="7"/>
       <c r="C427" s="7"/>
@@ -37035,11 +37035,11 @@
       <c r="I427" s="6"/>
       <c r="J427" s="7"/>
       <c r="K427" s="53" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="L427" s="7"/>
       <c r="M427" s="53" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="N427" s="7"/>
       <c r="O427" s="6">
@@ -37050,21 +37050,21 @@
       </c>
       <c r="Q427" s="7"/>
       <c r="R427" s="7" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="S427" s="7"/>
       <c r="T427" s="7" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="U427" s="7"/>
       <c r="V427" s="7"/>
       <c r="W427" s="7"/>
       <c r="X427" s="53"/>
       <c r="Y427" s="53" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="Z427" s="15" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="AA427"/>
       <c r="AB427"/>
@@ -37072,7 +37072,7 @@
     </row>
     <row r="428" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A428" s="47" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="B428" s="7"/>
       <c r="C428" s="7"/>
@@ -37088,11 +37088,11 @@
       <c r="I428" s="6"/>
       <c r="J428" s="7"/>
       <c r="K428" s="53" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="L428" s="7"/>
       <c r="M428" s="53" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="N428" s="7"/>
       <c r="O428" s="6">
@@ -37103,29 +37103,29 @@
       </c>
       <c r="Q428" s="7"/>
       <c r="R428" s="7" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="S428" s="7"/>
       <c r="T428" s="7" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="U428" s="7"/>
       <c r="V428" s="7"/>
       <c r="W428" s="7"/>
       <c r="X428" s="53"/>
       <c r="Y428" s="53" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="Z428" s="15" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="AA428"/>
       <c r="AB428"/>
       <c r="AC428"/>
     </row>
-    <row r="429" spans="1:29" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
+    <row r="429" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A429" s="47" t="s">
-        <v>2095</v>
+        <v>2114</v>
       </c>
       <c r="B429" s="7"/>
       <c r="C429" s="7"/>
@@ -37135,48 +37135,51 @@
         <v>591</v>
       </c>
       <c r="G429" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H429" s="6"/>
-      <c r="I429" s="6"/>
-      <c r="J429" s="53"/>
-      <c r="K429" s="53" t="s">
-        <v>2104</v>
+        <v>1807</v>
+      </c>
+      <c r="H429" s="7" t="s">
+        <v>1812</v>
+      </c>
+      <c r="I429" s="7" t="s">
+        <v>1815</v>
+      </c>
+      <c r="J429" s="7" t="s">
+        <v>1816</v>
+      </c>
+      <c r="K429" s="6" t="s">
+        <v>1882</v>
       </c>
       <c r="L429" s="7"/>
-      <c r="M429" s="53" t="s">
-        <v>1854</v>
-      </c>
-      <c r="N429" s="7"/>
-      <c r="O429" s="6"/>
+      <c r="M429" s="7" t="s">
+        <v>1883</v>
+      </c>
+      <c r="N429" s="53"/>
+      <c r="O429" s="53"/>
       <c r="P429" s="7" t="s">
-        <v>653</v>
-      </c>
-      <c r="Q429" s="7"/>
-      <c r="R429" s="7" t="s">
-        <v>2090</v>
-      </c>
+        <v>1884</v>
+      </c>
+      <c r="Q429" s="7" t="s">
+        <v>1886</v>
+      </c>
+      <c r="R429" s="7"/>
       <c r="S429" s="7"/>
-      <c r="T429" s="7" t="s">
-        <v>1853</v>
+      <c r="T429" s="53" t="s">
+        <v>1987</v>
       </c>
       <c r="U429" s="7"/>
       <c r="V429" s="7"/>
       <c r="W429" s="7"/>
-      <c r="X429" s="7" t="s">
-        <v>2108</v>
-      </c>
+      <c r="X429" s="7"/>
       <c r="Y429" s="7" t="s">
-        <v>1930</v>
-      </c>
-      <c r="Z429" s="15"/>
-      <c r="AA429"/>
-      <c r="AB429"/>
-      <c r="AC429"/>
-    </row>
-    <row r="430" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+        <v>1914</v>
+      </c>
+      <c r="Z429" s="15" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="430" spans="1:29" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A430" s="47" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="B430" s="7"/>
       <c r="C430" s="7"/>
@@ -37190,43 +37193,44 @@
       </c>
       <c r="H430" s="6"/>
       <c r="I430" s="6"/>
+      <c r="J430" s="53"/>
       <c r="K430" s="53" t="s">
         <v>2103</v>
       </c>
       <c r="L430" s="7"/>
       <c r="M430" s="53" t="s">
-        <v>1858</v>
+        <v>1853</v>
       </c>
       <c r="N430" s="7"/>
-      <c r="O430" s="6">
-        <v>3</v>
-      </c>
+      <c r="O430" s="6"/>
       <c r="P430" s="7" t="s">
         <v>653</v>
       </c>
       <c r="Q430" s="7"/>
       <c r="R430" s="7" t="s">
-        <v>2106</v>
+        <v>2089</v>
       </c>
       <c r="S430" s="7"/>
-      <c r="T430" s="7"/>
+      <c r="T430" s="7" t="s">
+        <v>1852</v>
+      </c>
       <c r="U430" s="7"/>
       <c r="V430" s="7"/>
       <c r="W430" s="7"/>
       <c r="X430" s="7" t="s">
         <v>2107</v>
       </c>
-      <c r="Y430" s="7"/>
-      <c r="Z430" s="15" t="s">
-        <v>2109</v>
-      </c>
+      <c r="Y430" s="7" t="s">
+        <v>1929</v>
+      </c>
+      <c r="Z430" s="15"/>
       <c r="AA430"/>
       <c r="AB430"/>
       <c r="AC430"/>
     </row>
     <row r="431" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A431" s="47" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="B431" s="7"/>
       <c r="C431" s="7"/>
@@ -37241,22 +37245,22 @@
       <c r="H431" s="6"/>
       <c r="I431" s="6"/>
       <c r="K431" s="53" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
       <c r="L431" s="7"/>
       <c r="M431" s="53" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="N431" s="7"/>
       <c r="O431" s="6">
         <v>3</v>
       </c>
       <c r="P431" s="7" t="s">
-        <v>2105</v>
+        <v>653</v>
       </c>
       <c r="Q431" s="7"/>
       <c r="R431" s="7" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="S431" s="7"/>
       <c r="T431" s="7"/>
@@ -37264,67 +37268,69 @@
       <c r="V431" s="7"/>
       <c r="W431" s="7"/>
       <c r="X431" s="7" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="Y431" s="7"/>
       <c r="Z431" s="15" t="s">
-        <v>2110</v>
+        <v>2108</v>
       </c>
       <c r="AA431"/>
       <c r="AB431"/>
       <c r="AC431"/>
     </row>
-    <row r="432" spans="1:29" ht="51" x14ac:dyDescent="0.2">
-      <c r="A432" s="26" t="s">
-        <v>1411</v>
+    <row r="432" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+      <c r="A432" s="47" t="s">
+        <v>2094</v>
       </c>
       <c r="B432" s="7"/>
       <c r="C432" s="7"/>
       <c r="D432" s="7"/>
       <c r="E432" s="7"/>
       <c r="F432" s="7" t="s">
-        <v>1457</v>
-      </c>
-      <c r="G432" s="7"/>
+        <v>591</v>
+      </c>
+      <c r="G432" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="H432" s="6"/>
       <c r="I432" s="6"/>
-      <c r="J432" s="7"/>
-      <c r="K432" s="6" t="s">
-        <v>1410</v>
+      <c r="K432" s="53" t="s">
+        <v>2102</v>
       </c>
       <c r="L432" s="7"/>
-      <c r="M432" s="7" t="s">
-        <v>1458</v>
-      </c>
-      <c r="N432" s="7" t="s">
-        <v>1412</v>
-      </c>
-      <c r="O432" s="7">
-        <v>4</v>
+      <c r="M432" s="53" t="s">
+        <v>1857</v>
+      </c>
+      <c r="N432" s="7"/>
+      <c r="O432" s="6">
+        <v>3</v>
       </c>
       <c r="P432" s="7" t="s">
-        <v>1315</v>
-      </c>
-      <c r="Q432" s="7" t="s">
-        <v>1460</v>
-      </c>
-      <c r="R432" s="7"/>
-      <c r="S432" s="6" t="s">
-        <v>1327</v>
-      </c>
+        <v>2104</v>
+      </c>
+      <c r="Q432" s="7"/>
+      <c r="R432" s="7" t="s">
+        <v>2105</v>
+      </c>
+      <c r="S432" s="7"/>
       <c r="T432" s="7"/>
       <c r="U432" s="7"/>
       <c r="V432" s="7"/>
       <c r="W432" s="7"/>
-      <c r="X432" s="7"/>
+      <c r="X432" s="7" t="s">
+        <v>2106</v>
+      </c>
       <c r="Y432" s="7"/>
       <c r="Z432" s="15" t="s">
-        <v>1326</v>
-      </c>
-    </row>
-    <row r="433" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+        <v>2109</v>
+      </c>
+      <c r="AA432"/>
+      <c r="AB432"/>
+      <c r="AC432"/>
+    </row>
+    <row r="433" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A433" s="26" t="s">
-        <v>1399</v>
+        <v>1411</v>
       </c>
       <c r="B433" s="7"/>
       <c r="C433" s="7"/>
@@ -37342,19 +37348,19 @@
       </c>
       <c r="L433" s="7"/>
       <c r="M433" s="7" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="N433" s="7" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="O433" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P433" s="7" t="s">
-        <v>1397</v>
+        <v>1315</v>
       </c>
       <c r="Q433" s="7" t="s">
-        <v>1398</v>
+        <v>1460</v>
       </c>
       <c r="R433" s="7"/>
       <c r="S433" s="6" t="s">
@@ -37370,128 +37376,128 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="434" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
-      <c r="A434" s="41" t="s">
+    <row r="434" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+      <c r="A434" s="26" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B434" s="7"/>
+      <c r="C434" s="7"/>
+      <c r="D434" s="7"/>
+      <c r="E434" s="7"/>
+      <c r="F434" s="7" t="s">
+        <v>1457</v>
+      </c>
+      <c r="G434" s="7"/>
+      <c r="H434" s="6"/>
+      <c r="I434" s="6"/>
+      <c r="J434" s="7"/>
+      <c r="K434" s="6" t="s">
+        <v>1410</v>
+      </c>
+      <c r="L434" s="7"/>
+      <c r="M434" s="7" t="s">
+        <v>1459</v>
+      </c>
+      <c r="N434" s="7" t="s">
+        <v>1413</v>
+      </c>
+      <c r="O434" s="7">
+        <v>2</v>
+      </c>
+      <c r="P434" s="7" t="s">
+        <v>1397</v>
+      </c>
+      <c r="Q434" s="7" t="s">
+        <v>1398</v>
+      </c>
+      <c r="R434" s="7"/>
+      <c r="S434" s="6" t="s">
+        <v>1327</v>
+      </c>
+      <c r="T434" s="7"/>
+      <c r="U434" s="7"/>
+      <c r="V434" s="7"/>
+      <c r="W434" s="7"/>
+      <c r="X434" s="7"/>
+      <c r="Y434" s="7"/>
+      <c r="Z434" s="15" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="435" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
+      <c r="A435" s="41" t="s">
         <v>1396</v>
       </c>
-      <c r="B434" s="41"/>
-      <c r="C434" s="41"/>
-      <c r="D434" s="41"/>
-      <c r="E434" s="41"/>
-      <c r="F434" s="41" t="s">
+      <c r="B435" s="41"/>
+      <c r="C435" s="41"/>
+      <c r="D435" s="41"/>
+      <c r="E435" s="41"/>
+      <c r="F435" s="41" t="s">
         <v>1333</v>
       </c>
-      <c r="G434" s="7" t="s">
+      <c r="G435" s="7" t="s">
         <v>1630</v>
       </c>
-      <c r="H434" s="41"/>
-      <c r="I434" s="41"/>
-      <c r="J434" s="41" t="s">
+      <c r="H435" s="41"/>
+      <c r="I435" s="41"/>
+      <c r="J435" s="41" t="s">
         <v>1395</v>
       </c>
-      <c r="K434" s="41" t="s">
+      <c r="K435" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="L434" s="41"/>
-      <c r="M434" s="41" t="s">
+      <c r="L435" s="41"/>
+      <c r="M435" s="41" t="s">
         <v>1596</v>
       </c>
-      <c r="N434" s="41"/>
-      <c r="O434" s="7">
+      <c r="N435" s="41"/>
+      <c r="O435" s="7">
         <v>3</v>
       </c>
-      <c r="P434" s="41"/>
-      <c r="Q434" s="41"/>
-      <c r="R434" s="41"/>
-      <c r="S434" s="41"/>
-      <c r="T434" s="59" t="s">
-        <v>2066</v>
-      </c>
-      <c r="U434" s="41"/>
-      <c r="V434" s="41"/>
-      <c r="W434" s="41"/>
-      <c r="X434" s="41"/>
-      <c r="Y434" s="41"/>
-      <c r="Z434" s="43" t="s">
+      <c r="P435" s="41"/>
+      <c r="Q435" s="41"/>
+      <c r="R435" s="41"/>
+      <c r="S435" s="41"/>
+      <c r="T435" s="59" t="s">
+        <v>2065</v>
+      </c>
+      <c r="U435" s="41"/>
+      <c r="V435" s="41"/>
+      <c r="W435" s="41"/>
+      <c r="X435" s="41"/>
+      <c r="Y435" s="41"/>
+      <c r="Z435" s="43" t="s">
         <v>1387</v>
       </c>
     </row>
-    <row r="435" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
-      <c r="A435" s="26" t="s">
+    <row r="436" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
+      <c r="A436" s="26" t="s">
         <v>1328</v>
-      </c>
-      <c r="B435" s="7"/>
-      <c r="C435" s="7"/>
-      <c r="D435" s="7"/>
-      <c r="E435" s="7"/>
-      <c r="F435" s="7" t="s">
-        <v>1334</v>
-      </c>
-      <c r="G435" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H435" s="6"/>
-      <c r="I435" s="6"/>
-      <c r="J435" s="7" t="s">
-        <v>1427</v>
-      </c>
-      <c r="K435" s="7" t="s">
-        <v>1568</v>
-      </c>
-      <c r="L435" s="7"/>
-      <c r="M435" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="N435" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="O435" s="6">
-        <v>9</v>
-      </c>
-      <c r="P435" s="7"/>
-      <c r="Q435" s="7"/>
-      <c r="R435" s="7"/>
-      <c r="S435" s="7"/>
-      <c r="T435" s="53" t="s">
-        <v>2067</v>
-      </c>
-      <c r="U435" s="7"/>
-      <c r="V435" s="7"/>
-      <c r="W435" s="7"/>
-      <c r="X435" s="7"/>
-      <c r="Y435" s="7"/>
-      <c r="Z435" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="436" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
-      <c r="A436" s="47" t="s">
-        <v>68</v>
       </c>
       <c r="B436" s="7"/>
       <c r="C436" s="7"/>
       <c r="D436" s="7"/>
       <c r="E436" s="7"/>
       <c r="F436" s="7" t="s">
-        <v>591</v>
+        <v>1334</v>
       </c>
       <c r="G436" s="7" t="s">
-        <v>990</v>
+        <v>29</v>
       </c>
       <c r="H436" s="6"/>
       <c r="I436" s="6"/>
       <c r="J436" s="7" t="s">
-        <v>1395</v>
+        <v>1427</v>
       </c>
       <c r="K436" s="7" t="s">
-        <v>1936</v>
+        <v>1568</v>
       </c>
       <c r="L436" s="7"/>
       <c r="M436" s="7" t="s">
-        <v>167</v>
+        <v>66</v>
       </c>
       <c r="N436" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O436" s="6">
         <v>9</v>
@@ -37501,7 +37507,7 @@
       <c r="R436" s="7"/>
       <c r="S436" s="7"/>
       <c r="T436" s="53" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="U436" s="7"/>
       <c r="V436" s="7"/>
@@ -37509,15 +37515,12 @@
       <c r="X436" s="7"/>
       <c r="Y436" s="7"/>
       <c r="Z436" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="AA436"/>
-      <c r="AB436"/>
-      <c r="AC436"/>
-    </row>
-    <row r="437" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="437" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
       <c r="A437" s="47" t="s">
-        <v>1761</v>
+        <v>68</v>
       </c>
       <c r="B437" s="7"/>
       <c r="C437" s="7"/>
@@ -37531,32 +37534,44 @@
       </c>
       <c r="H437" s="6"/>
       <c r="I437" s="6"/>
-      <c r="J437" s="7"/>
-      <c r="K437" s="7"/>
+      <c r="J437" s="7" t="s">
+        <v>1395</v>
+      </c>
+      <c r="K437" s="7" t="s">
+        <v>1935</v>
+      </c>
       <c r="L437" s="7"/>
-      <c r="M437" s="7"/>
-      <c r="N437" s="7"/>
-      <c r="O437" s="6"/>
+      <c r="M437" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="N437" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O437" s="6">
+        <v>9</v>
+      </c>
       <c r="P437" s="7"/>
       <c r="Q437" s="7"/>
       <c r="R437" s="7"/>
       <c r="S437" s="7"/>
-      <c r="T437" s="7"/>
+      <c r="T437" s="53" t="s">
+        <v>2066</v>
+      </c>
       <c r="U437" s="7"/>
       <c r="V437" s="7"/>
       <c r="W437" s="7"/>
       <c r="X437" s="7"/>
       <c r="Y437" s="7"/>
       <c r="Z437" s="15" t="s">
-        <v>1762</v>
+        <v>206</v>
       </c>
       <c r="AA437"/>
       <c r="AB437"/>
       <c r="AC437"/>
     </row>
-    <row r="438" spans="1:29" s="42" customFormat="1" ht="170" x14ac:dyDescent="0.15">
+    <row r="438" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A438" s="47" t="s">
-        <v>1909</v>
+        <v>1761</v>
       </c>
       <c r="B438" s="7"/>
       <c r="C438" s="7"/>
@@ -37566,52 +37581,36 @@
         <v>591</v>
       </c>
       <c r="G438" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H438" s="7" t="s">
-        <v>1821</v>
-      </c>
-      <c r="I438" s="7" t="s">
-        <v>1820</v>
-      </c>
-      <c r="J438" s="7" t="s">
-        <v>1819</v>
-      </c>
-      <c r="K438" s="7" t="s">
-        <v>1937</v>
-      </c>
+        <v>990</v>
+      </c>
+      <c r="H438" s="6"/>
+      <c r="I438" s="6"/>
+      <c r="J438" s="7"/>
+      <c r="K438" s="7"/>
       <c r="L438" s="7"/>
-      <c r="M438" s="7" t="s">
-        <v>1910</v>
-      </c>
+      <c r="M438" s="7"/>
       <c r="N438" s="7"/>
-      <c r="O438" s="6" t="s">
-        <v>1911</v>
-      </c>
-      <c r="P438" s="7" t="s">
-        <v>779</v>
-      </c>
-      <c r="Q438" s="7" t="s">
-        <v>1912</v>
-      </c>
+      <c r="O438" s="6"/>
+      <c r="P438" s="7"/>
+      <c r="Q438" s="7"/>
       <c r="R438" s="7"/>
       <c r="S438" s="7"/>
-      <c r="T438" s="7" t="s">
-        <v>1964</v>
-      </c>
+      <c r="T438" s="7"/>
       <c r="U438" s="7"/>
       <c r="V438" s="7"/>
       <c r="W438" s="7"/>
       <c r="X438" s="7"/>
       <c r="Y438" s="7"/>
-      <c r="Z438" s="15"/>
+      <c r="Z438" s="15" t="s">
+        <v>1762</v>
+      </c>
       <c r="AA438"/>
       <c r="AB438"/>
       <c r="AC438"/>
     </row>
-    <row r="439" spans="1:29" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="439" spans="1:29" s="42" customFormat="1" ht="153" x14ac:dyDescent="0.15">
       <c r="A439" s="47" t="s">
-        <v>1856</v>
+        <v>1908</v>
       </c>
       <c r="B439" s="7"/>
       <c r="C439" s="7"/>
@@ -37620,43 +37619,53 @@
       <c r="F439" s="7" t="s">
         <v>591</v>
       </c>
-      <c r="G439" s="7"/>
-      <c r="H439" s="6"/>
-      <c r="I439" s="6"/>
-      <c r="J439" s="7"/>
-      <c r="K439" s="53" t="s">
-        <v>1938</v>
+      <c r="G439" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H439" s="7" t="s">
+        <v>1820</v>
+      </c>
+      <c r="I439" s="7" t="s">
+        <v>1819</v>
+      </c>
+      <c r="J439" s="7" t="s">
+        <v>1818</v>
+      </c>
+      <c r="K439" s="7" t="s">
+        <v>1936</v>
       </c>
       <c r="L439" s="7"/>
-      <c r="M439" s="53" t="s">
-        <v>1858</v>
+      <c r="M439" s="7" t="s">
+        <v>1909</v>
       </c>
       <c r="N439" s="7"/>
-      <c r="O439" s="6">
-        <v>1</v>
-      </c>
-      <c r="P439" s="7"/>
-      <c r="Q439" s="7"/>
+      <c r="O439" s="6" t="s">
+        <v>1910</v>
+      </c>
+      <c r="P439" s="7" t="s">
+        <v>779</v>
+      </c>
+      <c r="Q439" s="7" t="s">
+        <v>1911</v>
+      </c>
       <c r="R439" s="7"/>
       <c r="S439" s="7"/>
       <c r="T439" s="7" t="s">
-        <v>1857</v>
+        <v>1963</v>
       </c>
       <c r="U439" s="7"/>
       <c r="V439" s="7"/>
       <c r="W439" s="7"/>
-      <c r="X439" s="7" t="s">
-        <v>1929</v>
-      </c>
+      <c r="X439" s="7"/>
       <c r="Y439" s="7"/>
       <c r="Z439" s="15"/>
       <c r="AA439"/>
       <c r="AB439"/>
       <c r="AC439"/>
     </row>
-    <row r="440" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
+    <row r="440" spans="1:29" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A440" s="47" t="s">
-        <v>1852</v>
+        <v>1855</v>
       </c>
       <c r="B440" s="7"/>
       <c r="C440" s="7"/>
@@ -37665,133 +37674,128 @@
       <c r="F440" s="7" t="s">
         <v>591</v>
       </c>
-      <c r="G440" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H440" s="6" t="s">
-        <v>1848</v>
-      </c>
-      <c r="I440" s="6" t="s">
-        <v>1847</v>
-      </c>
-      <c r="J440" s="53" t="s">
-        <v>1845</v>
-      </c>
-      <c r="K440" s="7" t="s">
-        <v>1846</v>
+      <c r="G440" s="7"/>
+      <c r="H440" s="6"/>
+      <c r="I440" s="6"/>
+      <c r="J440" s="7"/>
+      <c r="K440" s="53" t="s">
+        <v>1937</v>
       </c>
       <c r="L440" s="7"/>
       <c r="M440" s="53" t="s">
-        <v>1849</v>
+        <v>1857</v>
       </c>
       <c r="N440" s="7"/>
       <c r="O440" s="6">
         <v>1</v>
       </c>
       <c r="P440" s="7"/>
-      <c r="Q440" s="7" t="s">
-        <v>1851</v>
-      </c>
+      <c r="Q440" s="7"/>
       <c r="R440" s="7"/>
       <c r="S440" s="7"/>
-      <c r="T440" s="7"/>
+      <c r="T440" s="7" t="s">
+        <v>1856</v>
+      </c>
       <c r="U440" s="7"/>
       <c r="V440" s="7"/>
       <c r="W440" s="7"/>
-      <c r="X440" s="7"/>
+      <c r="X440" s="7" t="s">
+        <v>1928</v>
+      </c>
       <c r="Y440" s="7"/>
-      <c r="Z440" s="15" t="s">
-        <v>1850</v>
-      </c>
+      <c r="Z440" s="15"/>
       <c r="AA440"/>
       <c r="AB440"/>
       <c r="AC440"/>
     </row>
     <row r="441" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
       <c r="A441" s="47" t="s">
-        <v>1516</v>
+        <v>1851</v>
       </c>
       <c r="B441" s="7"/>
       <c r="C441" s="7"/>
       <c r="D441" s="7"/>
       <c r="E441" s="7"/>
       <c r="F441" s="7" t="s">
-        <v>1517</v>
+        <v>591</v>
       </c>
       <c r="G441" s="7" t="s">
-        <v>1518</v>
+        <v>77</v>
       </c>
       <c r="H441" s="6" t="s">
-        <v>1520</v>
-      </c>
-      <c r="I441" s="6"/>
-      <c r="J441" s="6"/>
-      <c r="K441" s="6" t="s">
-        <v>109</v>
+        <v>1847</v>
+      </c>
+      <c r="I441" s="6" t="s">
+        <v>1846</v>
+      </c>
+      <c r="J441" s="53" t="s">
+        <v>1844</v>
+      </c>
+      <c r="K441" s="7" t="s">
+        <v>1845</v>
       </c>
       <c r="L441" s="7"/>
-      <c r="M441" s="6" t="s">
-        <v>1519</v>
+      <c r="M441" s="53" t="s">
+        <v>1848</v>
       </c>
       <c r="N441" s="7"/>
-      <c r="O441" s="7"/>
+      <c r="O441" s="6">
+        <v>1</v>
+      </c>
       <c r="P441" s="7"/>
-      <c r="Q441" s="7"/>
-      <c r="R441" s="6" t="s">
-        <v>1521</v>
-      </c>
-      <c r="S441" s="6"/>
+      <c r="Q441" s="7" t="s">
+        <v>1850</v>
+      </c>
+      <c r="R441" s="7"/>
+      <c r="S441" s="7"/>
       <c r="T441" s="7"/>
       <c r="U441" s="7"/>
       <c r="V441" s="7"/>
       <c r="W441" s="7"/>
       <c r="X441" s="7"/>
       <c r="Y441" s="7"/>
-      <c r="Z441" s="15"/>
-    </row>
-    <row r="442" spans="1:29" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+      <c r="Z441" s="15" t="s">
+        <v>1849</v>
+      </c>
+      <c r="AA441"/>
+      <c r="AB441"/>
+      <c r="AC441"/>
+    </row>
+    <row r="442" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
       <c r="A442" s="47" t="s">
-        <v>1631</v>
+        <v>1516</v>
       </c>
       <c r="B442" s="7"/>
       <c r="C442" s="7"/>
       <c r="D442" s="7"/>
       <c r="E442" s="7"/>
       <c r="F442" s="7" t="s">
-        <v>1632</v>
+        <v>1517</v>
       </c>
       <c r="G442" s="7" t="s">
-        <v>1602</v>
-      </c>
-      <c r="H442" s="7" t="s">
-        <v>1617</v>
-      </c>
-      <c r="I442" s="7" t="s">
-        <v>1618</v>
-      </c>
-      <c r="J442" s="6" t="s">
-        <v>1633</v>
-      </c>
-      <c r="K442" s="7" t="s">
-        <v>1429</v>
+        <v>1518</v>
+      </c>
+      <c r="H442" s="6" t="s">
+        <v>1520</v>
+      </c>
+      <c r="I442" s="6"/>
+      <c r="J442" s="6"/>
+      <c r="K442" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="L442" s="7"/>
       <c r="M442" s="6" t="s">
-        <v>1566</v>
-      </c>
-      <c r="N442" s="7" t="s">
-        <v>1567</v>
-      </c>
-      <c r="O442" s="6">
-        <v>4</v>
-      </c>
+        <v>1519</v>
+      </c>
+      <c r="N442" s="7"/>
+      <c r="O442" s="7"/>
       <c r="P442" s="7"/>
       <c r="Q442" s="7"/>
-      <c r="R442" s="6"/>
+      <c r="R442" s="6" t="s">
+        <v>1521</v>
+      </c>
       <c r="S442" s="6"/>
-      <c r="T442" s="7" t="s">
-        <v>1865</v>
-      </c>
+      <c r="T442" s="7"/>
       <c r="U442" s="7"/>
       <c r="V442" s="7"/>
       <c r="W442" s="7"/>
@@ -37799,65 +37803,59 @@
       <c r="Y442" s="7"/>
       <c r="Z442" s="15"/>
     </row>
-    <row r="443" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+    <row r="443" spans="1:29" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A443" s="47" t="s">
-        <v>1814</v>
+        <v>1631</v>
       </c>
       <c r="B443" s="7"/>
       <c r="C443" s="7"/>
       <c r="D443" s="7"/>
       <c r="E443" s="7"/>
       <c r="F443" s="7" t="s">
-        <v>591</v>
+        <v>1632</v>
       </c>
       <c r="G443" s="7" t="s">
-        <v>1807</v>
+        <v>1602</v>
       </c>
       <c r="H443" s="7" t="s">
-        <v>1888</v>
+        <v>1617</v>
       </c>
       <c r="I443" s="7" t="s">
-        <v>1679</v>
-      </c>
-      <c r="J443" s="7" t="s">
-        <v>1680</v>
+        <v>1618</v>
+      </c>
+      <c r="J443" s="6" t="s">
+        <v>1633</v>
       </c>
       <c r="K443" s="7" t="s">
-        <v>1889</v>
+        <v>1429</v>
       </c>
       <c r="L443" s="7"/>
-      <c r="M443" s="7" t="s">
-        <v>1890</v>
-      </c>
-      <c r="N443" s="53"/>
-      <c r="O443" s="7">
+      <c r="M443" s="6" t="s">
+        <v>1566</v>
+      </c>
+      <c r="N443" s="7" t="s">
+        <v>1567</v>
+      </c>
+      <c r="O443" s="6">
         <v>4</v>
       </c>
-      <c r="P443" s="7" t="s">
-        <v>653</v>
-      </c>
-      <c r="Q443" s="7" t="s">
-        <v>1891</v>
-      </c>
-      <c r="R443" s="53">
-        <v>1265</v>
-      </c>
-      <c r="S443" s="7"/>
+      <c r="P443" s="7"/>
+      <c r="Q443" s="7"/>
+      <c r="R443" s="6"/>
+      <c r="S443" s="6"/>
       <c r="T443" s="7" t="s">
-        <v>1981</v>
+        <v>1864</v>
       </c>
       <c r="U443" s="7"/>
       <c r="V443" s="7"/>
       <c r="W443" s="7"/>
       <c r="X443" s="7"/>
       <c r="Y443" s="7"/>
-      <c r="Z443" s="15" t="s">
-        <v>1681</v>
-      </c>
+      <c r="Z443" s="15"/>
     </row>
     <row r="444" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A444" s="47" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="B444" s="7"/>
       <c r="C444" s="7"/>
@@ -37870,106 +37868,50 @@
         <v>1807</v>
       </c>
       <c r="H444" s="7" t="s">
-        <v>1812</v>
+        <v>1887</v>
       </c>
       <c r="I444" s="7" t="s">
-        <v>1816</v>
+        <v>1679</v>
       </c>
       <c r="J444" s="7" t="s">
-        <v>1817</v>
-      </c>
-      <c r="K444" s="6" t="s">
-        <v>1883</v>
+        <v>1680</v>
+      </c>
+      <c r="K444" s="7" t="s">
+        <v>1888</v>
       </c>
       <c r="L444" s="7"/>
       <c r="M444" s="7" t="s">
-        <v>1884</v>
+        <v>1889</v>
       </c>
       <c r="N444" s="53"/>
-      <c r="O444" s="53"/>
+      <c r="O444" s="7">
+        <v>4</v>
+      </c>
       <c r="P444" s="7" t="s">
-        <v>1885</v>
+        <v>653</v>
       </c>
       <c r="Q444" s="7" t="s">
-        <v>1887</v>
-      </c>
-      <c r="R444" s="7"/>
+        <v>1890</v>
+      </c>
+      <c r="R444" s="53">
+        <v>1265</v>
+      </c>
       <c r="S444" s="7"/>
-      <c r="T444" s="53" t="s">
-        <v>1988</v>
+      <c r="T444" s="7" t="s">
+        <v>1980</v>
       </c>
       <c r="U444" s="7"/>
       <c r="V444" s="7"/>
       <c r="W444" s="7"/>
       <c r="X444" s="7"/>
-      <c r="Y444" s="7" t="s">
-        <v>1915</v>
-      </c>
+      <c r="Y444" s="7"/>
       <c r="Z444" s="15" t="s">
-        <v>1896</v>
-      </c>
-    </row>
-    <row r="445" spans="1:29" s="42" customFormat="1" ht="136" x14ac:dyDescent="0.15">
-      <c r="A445" s="47" t="s">
-        <v>1874</v>
-      </c>
-      <c r="B445" s="7"/>
-      <c r="C445" s="7"/>
-      <c r="D445" s="7"/>
-      <c r="E445" s="7"/>
-      <c r="F445" s="7" t="s">
-        <v>591</v>
-      </c>
-      <c r="G445" s="7" t="s">
-        <v>1807</v>
-      </c>
-      <c r="H445" s="7" t="s">
-        <v>1809</v>
-      </c>
-      <c r="I445" s="7" t="s">
-        <v>1808</v>
-      </c>
-      <c r="J445" s="7" t="s">
-        <v>1879</v>
-      </c>
-      <c r="K445" s="7" t="s">
-        <v>1982</v>
-      </c>
-      <c r="L445" s="7"/>
-      <c r="M445" s="6" t="s">
-        <v>1880</v>
-      </c>
-      <c r="N445" s="53" t="s">
-        <v>443</v>
-      </c>
-      <c r="O445" s="53">
-        <v>13</v>
-      </c>
-      <c r="P445" s="7" t="s">
-        <v>779</v>
-      </c>
-      <c r="Q445" s="7" t="s">
-        <v>1881</v>
-      </c>
-      <c r="R445" s="7"/>
-      <c r="S445" s="53" t="s">
-        <v>1882</v>
-      </c>
-      <c r="T445" s="7" t="s">
-        <v>1986</v>
-      </c>
-      <c r="U445" s="7"/>
-      <c r="V445" s="7"/>
-      <c r="W445" s="7"/>
-      <c r="X445" s="7"/>
-      <c r="Y445" s="53" t="s">
-        <v>1886</v>
-      </c>
-      <c r="Z445" s="15"/>
-    </row>
-    <row r="446" spans="1:29" s="42" customFormat="1" ht="136" x14ac:dyDescent="0.15">
+        <v>1681</v>
+      </c>
+    </row>
+    <row r="446" spans="1:29" s="42" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A446" s="47" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="B446" s="7"/>
       <c r="C446" s="7"/>
@@ -37988,44 +37930,46 @@
         <v>1808</v>
       </c>
       <c r="J446" s="7" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="K446" s="7" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="L446" s="7"/>
       <c r="M446" s="6" t="s">
+        <v>1879</v>
+      </c>
+      <c r="N446" s="53" t="s">
+        <v>443</v>
+      </c>
+      <c r="O446" s="53">
+        <v>13</v>
+      </c>
+      <c r="P446" s="7" t="s">
+        <v>779</v>
+      </c>
+      <c r="Q446" s="7" t="s">
         <v>1880</v>
-      </c>
-      <c r="N446" s="53" t="s">
-        <v>1251</v>
-      </c>
-      <c r="O446" s="53" t="s">
-        <v>680</v>
-      </c>
-      <c r="P446" s="53" t="s">
-        <v>680</v>
-      </c>
-      <c r="Q446" s="7" t="s">
-        <v>1881</v>
       </c>
       <c r="R446" s="7"/>
       <c r="S446" s="53" t="s">
-        <v>1882</v>
-      </c>
-      <c r="T446" s="7"/>
+        <v>1881</v>
+      </c>
+      <c r="T446" s="7" t="s">
+        <v>1985</v>
+      </c>
       <c r="U446" s="7"/>
       <c r="V446" s="7"/>
       <c r="W446" s="7"/>
       <c r="X446" s="7"/>
       <c r="Y446" s="53" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="Z446" s="15"/>
     </row>
-    <row r="447" spans="1:29" s="42" customFormat="1" ht="136" x14ac:dyDescent="0.15">
+    <row r="447" spans="1:29" s="42" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A447" s="47" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="B447" s="7"/>
       <c r="C447" s="7"/>
@@ -38044,46 +37988,44 @@
         <v>1808</v>
       </c>
       <c r="J447" s="7" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="K447" s="7" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="L447" s="7"/>
       <c r="M447" s="6" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="N447" s="53" t="s">
-        <v>444</v>
+        <v>1251</v>
       </c>
       <c r="O447" s="53" t="s">
-        <v>1984</v>
+        <v>680</v>
       </c>
       <c r="P447" s="53" t="s">
         <v>680</v>
       </c>
       <c r="Q447" s="7" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="R447" s="7"/>
       <c r="S447" s="53" t="s">
-        <v>1882</v>
-      </c>
-      <c r="T447" s="7" t="s">
-        <v>1983</v>
-      </c>
+        <v>1881</v>
+      </c>
+      <c r="T447" s="7"/>
       <c r="U447" s="7"/>
       <c r="V447" s="7"/>
       <c r="W447" s="7"/>
       <c r="X447" s="7"/>
       <c r="Y447" s="53" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="Z447" s="15"/>
     </row>
-    <row r="448" spans="1:29" s="42" customFormat="1" ht="136" x14ac:dyDescent="0.15">
+    <row r="448" spans="1:29" s="42" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A448" s="47" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="B448" s="7"/>
       <c r="C448" s="7"/>
@@ -38102,108 +38044,126 @@
         <v>1808</v>
       </c>
       <c r="J448" s="7" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="K448" s="7" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="L448" s="7"/>
       <c r="M448" s="6" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="N448" s="53" t="s">
-        <v>577</v>
+        <v>444</v>
       </c>
       <c r="O448" s="53" t="s">
-        <v>1985</v>
+        <v>1983</v>
       </c>
       <c r="P448" s="53" t="s">
         <v>680</v>
       </c>
       <c r="Q448" s="7" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="R448" s="7"/>
       <c r="S448" s="53" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="T448" s="7" t="s">
-        <v>1987</v>
+        <v>1982</v>
       </c>
       <c r="U448" s="7"/>
       <c r="V448" s="7"/>
       <c r="W448" s="7"/>
       <c r="X448" s="7"/>
       <c r="Y448" s="53" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="Z448" s="15"/>
     </row>
-    <row r="449" spans="1:26" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
-      <c r="A449" s="26" t="s">
-        <v>302</v>
+    <row r="449" spans="1:26" s="42" customFormat="1" ht="119" x14ac:dyDescent="0.15">
+      <c r="A449" s="47" t="s">
+        <v>1873</v>
       </c>
       <c r="B449" s="7"/>
       <c r="C449" s="7"/>
       <c r="D449" s="7"/>
       <c r="E449" s="7"/>
-      <c r="F449" s="6"/>
-      <c r="G449" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H449" s="6" t="s">
-        <v>2072</v>
-      </c>
-      <c r="I449" s="6" t="s">
-        <v>2073</v>
-      </c>
-      <c r="J449" s="6" t="s">
-        <v>2074</v>
-      </c>
-      <c r="K449" s="6"/>
+      <c r="F449" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="G449" s="7" t="s">
+        <v>1807</v>
+      </c>
+      <c r="H449" s="7" t="s">
+        <v>1809</v>
+      </c>
+      <c r="I449" s="7" t="s">
+        <v>1808</v>
+      </c>
+      <c r="J449" s="7" t="s">
+        <v>1878</v>
+      </c>
+      <c r="K449" s="7" t="s">
+        <v>1981</v>
+      </c>
       <c r="L449" s="7"/>
       <c r="M449" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="N449" s="7"/>
-      <c r="O449" s="7"/>
-      <c r="P449" s="7"/>
-      <c r="Q449" s="7"/>
+        <v>1879</v>
+      </c>
+      <c r="N449" s="53" t="s">
+        <v>577</v>
+      </c>
+      <c r="O449" s="53" t="s">
+        <v>1984</v>
+      </c>
+      <c r="P449" s="53" t="s">
+        <v>680</v>
+      </c>
+      <c r="Q449" s="7" t="s">
+        <v>1880</v>
+      </c>
       <c r="R449" s="7"/>
-      <c r="S449" s="7"/>
-      <c r="T449" s="7"/>
+      <c r="S449" s="53" t="s">
+        <v>1881</v>
+      </c>
+      <c r="T449" s="7" t="s">
+        <v>1986</v>
+      </c>
       <c r="U449" s="7"/>
       <c r="V449" s="7"/>
       <c r="W449" s="7"/>
       <c r="X449" s="7"/>
-      <c r="Y449" s="7"/>
-      <c r="Z449" s="15" t="s">
-        <v>2075</v>
-      </c>
-    </row>
-    <row r="450" spans="1:26" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
-      <c r="A450" s="47"/>
+      <c r="Y449" s="53" t="s">
+        <v>1885</v>
+      </c>
+      <c r="Z449" s="15"/>
+    </row>
+    <row r="450" spans="1:26" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
+      <c r="A450" s="26" t="s">
+        <v>302</v>
+      </c>
       <c r="B450" s="7"/>
       <c r="C450" s="7"/>
       <c r="D450" s="7"/>
       <c r="E450" s="7"/>
-      <c r="F450" s="6" t="s">
-        <v>591</v>
-      </c>
+      <c r="F450" s="6"/>
       <c r="G450" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="H450" s="6"/>
-      <c r="I450" s="6"/>
+        <v>45</v>
+      </c>
+      <c r="H450" s="6" t="s">
+        <v>2071</v>
+      </c>
+      <c r="I450" s="6" t="s">
+        <v>2072</v>
+      </c>
       <c r="J450" s="6" t="s">
-        <v>1942</v>
-      </c>
-      <c r="K450" s="6" t="s">
-        <v>1943</v>
-      </c>
+        <v>2073</v>
+      </c>
+      <c r="K450" s="6"/>
       <c r="L450" s="7"/>
       <c r="M450" s="6" t="s">
-        <v>1944</v>
+        <v>110</v>
       </c>
       <c r="N450" s="7"/>
       <c r="O450" s="7"/>
@@ -38216,50 +38176,54 @@
       <c r="V450" s="7"/>
       <c r="W450" s="7"/>
       <c r="X450" s="7"/>
-      <c r="Y450" s="7" t="s">
-        <v>1945</v>
-      </c>
-      <c r="Z450" s="15"/>
-    </row>
-    <row r="451" spans="1:26" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
-      <c r="A451" s="47" t="s">
-        <v>1653</v>
-      </c>
+      <c r="Y450" s="7"/>
+      <c r="Z450" s="15" t="s">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="451" spans="1:26" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+      <c r="A451" s="47"/>
       <c r="B451" s="7"/>
       <c r="C451" s="7"/>
       <c r="D451" s="7"/>
       <c r="E451" s="7"/>
-      <c r="F451" s="7"/>
-      <c r="G451" s="7"/>
+      <c r="F451" s="6" t="s">
+        <v>591</v>
+      </c>
+      <c r="G451" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="H451" s="6"/>
       <c r="I451" s="6"/>
-      <c r="J451" s="6"/>
-      <c r="K451" s="53" t="s">
-        <v>1763</v>
+      <c r="J451" s="6" t="s">
+        <v>1941</v>
+      </c>
+      <c r="K451" s="6" t="s">
+        <v>1942</v>
       </c>
       <c r="L451" s="7"/>
       <c r="M451" s="6" t="s">
-        <v>1655</v>
+        <v>1943</v>
       </c>
       <c r="N451" s="7"/>
-      <c r="O451" s="6"/>
+      <c r="O451" s="7"/>
       <c r="P451" s="7"/>
       <c r="Q451" s="7"/>
-      <c r="R451" s="6"/>
-      <c r="S451" s="6"/>
+      <c r="R451" s="7"/>
+      <c r="S451" s="7"/>
       <c r="T451" s="7"/>
       <c r="U451" s="7"/>
       <c r="V451" s="7"/>
       <c r="W451" s="7"/>
       <c r="X451" s="7"/>
-      <c r="Y451" s="7"/>
-      <c r="Z451" s="15" t="s">
-        <v>1657</v>
-      </c>
+      <c r="Y451" s="7" t="s">
+        <v>1944</v>
+      </c>
+      <c r="Z451" s="15"/>
     </row>
     <row r="452" spans="1:26" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A452" s="47" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="B452" s="7"/>
       <c r="C452" s="7"/>
@@ -38270,12 +38234,12 @@
       <c r="H452" s="6"/>
       <c r="I452" s="6"/>
       <c r="J452" s="6"/>
-      <c r="K452" s="7" t="s">
-        <v>1764</v>
+      <c r="K452" s="53" t="s">
+        <v>1763</v>
       </c>
       <c r="L452" s="7"/>
       <c r="M452" s="6" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="N452" s="7"/>
       <c r="O452" s="6"/>
@@ -38290,110 +38254,146 @@
       <c r="X452" s="7"/>
       <c r="Y452" s="7"/>
       <c r="Z452" s="15" t="s">
-        <v>1658</v>
-      </c>
-    </row>
-    <row r="453" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="453" spans="1:26" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A453" s="47" t="s">
-        <v>1659</v>
+        <v>1654</v>
       </c>
       <c r="B453" s="7"/>
       <c r="C453" s="7"/>
       <c r="D453" s="7"/>
       <c r="E453" s="7"/>
-      <c r="F453" s="6" t="s">
-        <v>1189</v>
-      </c>
-      <c r="G453" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="H453" s="10"/>
-      <c r="I453" s="10"/>
-      <c r="J453" s="6" t="s">
-        <v>1760</v>
-      </c>
+      <c r="F453" s="7"/>
+      <c r="G453" s="7"/>
+      <c r="H453" s="6"/>
+      <c r="I453" s="6"/>
+      <c r="J453" s="6"/>
       <c r="K453" s="7" t="s">
-        <v>897</v>
-      </c>
-      <c r="L453" s="6"/>
+        <v>1764</v>
+      </c>
+      <c r="L453" s="7"/>
       <c r="M453" s="6" t="s">
-        <v>1190</v>
+        <v>1656</v>
       </c>
       <c r="N453" s="7"/>
-      <c r="O453" s="7"/>
-      <c r="P453" s="7" t="s">
-        <v>676</v>
-      </c>
+      <c r="O453" s="6"/>
+      <c r="P453" s="7"/>
       <c r="Q453" s="7"/>
-      <c r="R453" s="7"/>
-      <c r="S453" s="7"/>
+      <c r="R453" s="6"/>
+      <c r="S453" s="6"/>
       <c r="T453" s="7"/>
       <c r="U453" s="7"/>
       <c r="V453" s="7"/>
       <c r="W453" s="7"/>
-      <c r="X453" s="7" t="s">
-        <v>796</v>
-      </c>
+      <c r="X453" s="7"/>
       <c r="Y453" s="7"/>
-      <c r="Z453" s="14" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="454" spans="1:26" s="42" customFormat="1" ht="289" x14ac:dyDescent="0.15">
-      <c r="A454" s="26" t="s">
-        <v>2076</v>
+      <c r="Z453" s="15" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="454" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+      <c r="A454" s="47" t="s">
+        <v>1659</v>
       </c>
       <c r="B454" s="7"/>
       <c r="C454" s="7"/>
       <c r="D454" s="7"/>
       <c r="E454" s="7"/>
       <c r="F454" s="6" t="s">
-        <v>591</v>
+        <v>1189</v>
       </c>
       <c r="G454" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H454" s="6" t="s">
-        <v>2077</v>
-      </c>
-      <c r="I454" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="H454" s="10"/>
+      <c r="I454" s="10"/>
       <c r="J454" s="6" t="s">
-        <v>2078</v>
-      </c>
-      <c r="K454" s="6" t="s">
-        <v>815</v>
-      </c>
-      <c r="L454" s="7"/>
-      <c r="M454" s="7" t="s">
-        <v>2079</v>
+        <v>1760</v>
+      </c>
+      <c r="K454" s="7" t="s">
+        <v>897</v>
+      </c>
+      <c r="L454" s="6"/>
+      <c r="M454" s="6" t="s">
+        <v>1190</v>
       </c>
       <c r="N454" s="7"/>
-      <c r="O454" s="60" t="s">
-        <v>2080</v>
-      </c>
-      <c r="P454" s="53" t="s">
-        <v>2082</v>
+      <c r="O454" s="7"/>
+      <c r="P454" s="7" t="s">
+        <v>676</v>
       </c>
       <c r="Q454" s="7"/>
       <c r="R454" s="7"/>
-      <c r="S454" s="53" t="s">
-        <v>2081</v>
-      </c>
+      <c r="S454" s="7"/>
       <c r="T454" s="7"/>
       <c r="U454" s="7"/>
       <c r="V454" s="7"/>
       <c r="W454" s="7"/>
-      <c r="X454" s="7"/>
+      <c r="X454" s="7" t="s">
+        <v>796</v>
+      </c>
       <c r="Y454" s="7"/>
-      <c r="Z454" s="15" t="s">
-        <v>2083</v>
-      </c>
-    </row>
-    <row r="455" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="Z455" s="8"/>
+      <c r="Z454" s="14" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="455" spans="1:26" s="42" customFormat="1" ht="255" x14ac:dyDescent="0.15">
+      <c r="A455" s="26" t="s">
+        <v>2075</v>
+      </c>
+      <c r="B455" s="7"/>
+      <c r="C455" s="7"/>
+      <c r="D455" s="7"/>
+      <c r="E455" s="7"/>
+      <c r="F455" s="6" t="s">
+        <v>591</v>
+      </c>
+      <c r="G455" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H455" s="6" t="s">
+        <v>2076</v>
+      </c>
+      <c r="I455" s="6"/>
+      <c r="J455" s="6" t="s">
+        <v>2077</v>
+      </c>
+      <c r="K455" s="6" t="s">
+        <v>815</v>
+      </c>
+      <c r="L455" s="7"/>
+      <c r="M455" s="7" t="s">
+        <v>2078</v>
+      </c>
+      <c r="N455" s="7"/>
+      <c r="O455" s="60" t="s">
+        <v>2079</v>
+      </c>
+      <c r="P455" s="53" t="s">
+        <v>2081</v>
+      </c>
+      <c r="Q455" s="7"/>
+      <c r="R455" s="7"/>
+      <c r="S455" s="53" t="s">
+        <v>2080</v>
+      </c>
+      <c r="T455" s="7"/>
+      <c r="U455" s="7"/>
+      <c r="V455" s="7"/>
+      <c r="W455" s="7"/>
+      <c r="X455" s="7"/>
+      <c r="Y455" s="7"/>
+      <c r="Z455" s="15" t="s">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="456" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z456" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z453" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Z454" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA417">
     <sortCondition ref="A3:A417"/>
   </sortState>

</xml_diff>

<commit_message>
small edits to inventory and C139xml
</commit_message>
<xml_diff>
--- a/metadata/InventaireCampa.xlsx
+++ b/metadata/InventaireCampa.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arlogriffiths/Documents/GitHub/DHARMA/tfc-campa-epigraphy/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{F4B522BB-FCF7-B841-8B8E-CA7952F591A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{1B66B7DA-D546-F345-B545-91F306B97D45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1280" windowWidth="33520" windowHeight="15380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6300" windowWidth="33520" windowHeight="15380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -10081,9 +10081,6 @@
     <t>Piédroit (converti en linteau)</t>
   </si>
   <si>
-    <t>n. ****, n. ****</t>
-  </si>
-  <si>
     <t>XIe</t>
   </si>
   <si>
@@ -12233,6 +12230,9 @@
   </si>
   <si>
     <t>*252</t>
+  </si>
+  <si>
+    <t>n. 2314, n. 2315</t>
   </si>
 </sst>
 </file>
@@ -13190,10 +13190,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1300" topLeftCell="A425" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1300" topLeftCell="A383" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="J429" sqref="J429"/>
+      <selection pane="bottomLeft" activeCell="S388" sqref="S388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13240,10 +13240,10 @@
         <v>898</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>1330</v>
@@ -13349,7 +13349,7 @@
       </c>
       <c r="S2" s="10"/>
       <c r="T2" s="7" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="U2" s="10"/>
       <c r="V2" s="10"/>
@@ -13386,10 +13386,10 @@
         <v>1475</v>
       </c>
       <c r="K3" s="57" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="L3" s="57" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="M3" s="57" t="s">
         <v>613</v>
@@ -13415,13 +13415,13 @@
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
       <c r="X3" s="57" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="Y3" s="57" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="Z3" s="58" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="AA3" s="23"/>
       <c r="AC3" s="1"/>
@@ -14761,7 +14761,7 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>591</v>
@@ -14770,13 +14770,13 @@
         <v>1532</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="I27" s="7" t="s">
+        <v>1725</v>
+      </c>
+      <c r="J27" s="7" t="s">
         <v>1726</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>1727</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>815</v>
@@ -14832,16 +14832,16 @@
         <v>1532</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>384</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="L28" s="7" t="s">
         <v>815</v>
@@ -14873,7 +14873,7 @@
         <v>893</v>
       </c>
       <c r="Y28" s="10" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="Z28" s="15"/>
     </row>
@@ -14892,10 +14892,10 @@
         <v>1532</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>671</v>
@@ -14956,10 +14956,10 @@
         <v>1532</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>671</v>
@@ -15022,13 +15022,13 @@
         <v>1678</v>
       </c>
       <c r="H31" s="7" t="s">
+        <v>1714</v>
+      </c>
+      <c r="I31" s="7" t="s">
         <v>1715</v>
       </c>
-      <c r="I31" s="7" t="s">
-        <v>1716</v>
-      </c>
       <c r="J31" s="7" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>815</v>
@@ -15052,7 +15052,7 @@
       </c>
       <c r="S31" s="10"/>
       <c r="T31" s="10" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="U31" s="10" t="s">
         <v>882</v>
@@ -15116,7 +15116,7 @@
         <v>1553</v>
       </c>
       <c r="Z32" s="14" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="33" spans="1:27" ht="121" x14ac:dyDescent="0.2">
@@ -15342,7 +15342,7 @@
         <v>729</v>
       </c>
       <c r="Z36" s="14" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="37" spans="1:27" ht="138" x14ac:dyDescent="0.2">
@@ -15511,7 +15511,7 @@
         <v>1090</v>
       </c>
       <c r="Y39" s="10" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="Z39" s="15" t="s">
         <v>425</v>
@@ -16037,7 +16037,7 @@
       <c r="X48" s="10"/>
       <c r="Y48" s="10"/>
       <c r="Z48" s="15" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="49" spans="1:26" ht="187" x14ac:dyDescent="0.2">
@@ -17953,7 +17953,7 @@
         <v>962</v>
       </c>
       <c r="Z82" s="15" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="83" spans="1:26" ht="68" x14ac:dyDescent="0.2">
@@ -18116,7 +18116,7 @@
       <c r="S85" s="10"/>
       <c r="T85" s="10"/>
       <c r="U85" s="7" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="V85" s="10"/>
       <c r="W85" s="10"/>
@@ -18279,7 +18279,7 @@
       </c>
       <c r="S88" s="10"/>
       <c r="T88" s="10" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="U88" s="10"/>
       <c r="V88" s="10"/>
@@ -18335,7 +18335,7 @@
       </c>
       <c r="S89" s="10"/>
       <c r="T89" s="10" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="U89" s="10"/>
       <c r="V89" s="10"/>
@@ -18391,7 +18391,7 @@
       </c>
       <c r="S90" s="10"/>
       <c r="T90" s="10" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="U90" s="10"/>
       <c r="V90" s="10"/>
@@ -18447,7 +18447,7 @@
       </c>
       <c r="S91" s="10"/>
       <c r="T91" s="7" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="U91" s="10"/>
       <c r="V91" s="10"/>
@@ -18593,7 +18593,7 @@
       </c>
       <c r="Q94" s="10"/>
       <c r="R94" s="10" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="S94" s="10"/>
       <c r="T94" s="10">
@@ -18607,7 +18607,7 @@
         <v>1100</v>
       </c>
       <c r="Z94" s="15" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="95" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -18814,7 +18814,7 @@
         <v>775</v>
       </c>
       <c r="Q98" s="7" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="R98" s="10" t="s">
         <v>1065</v>
@@ -19322,7 +19322,7 @@
         <v>775</v>
       </c>
       <c r="M108" s="57" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="N108" s="10" t="s">
         <v>443</v>
@@ -19346,7 +19346,7 @@
       <c r="W108" s="10"/>
       <c r="X108" s="10"/>
       <c r="Y108" s="57" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="Z108" s="15"/>
     </row>
@@ -19374,7 +19374,7 @@
         <v>775</v>
       </c>
       <c r="M109" s="57" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="N109" s="10" t="s">
         <v>611</v>
@@ -19398,7 +19398,7 @@
       <c r="W109" s="10"/>
       <c r="X109" s="10"/>
       <c r="Y109" s="57" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="Z109" s="15"/>
     </row>
@@ -19426,7 +19426,7 @@
         <v>775</v>
       </c>
       <c r="M110" s="57" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="N110" s="10" t="s">
         <v>972</v>
@@ -19450,7 +19450,7 @@
       <c r="W110" s="10"/>
       <c r="X110" s="10"/>
       <c r="Y110" s="57" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="Z110" s="15"/>
     </row>
@@ -19471,10 +19471,10 @@
       <c r="H111" s="10"/>
       <c r="I111" s="10"/>
       <c r="J111" s="10" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="K111" s="53" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="L111" s="10" t="s">
         <v>815</v>
@@ -19520,18 +19520,18 @@
         <v>591</v>
       </c>
       <c r="G112" s="7" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
       <c r="J112" s="7" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="K112" s="7" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="L112" s="7" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="M112" s="7" t="s">
         <v>156</v>
@@ -19631,7 +19631,7 @@
         <v>1432</v>
       </c>
       <c r="J114" s="10" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="K114" s="10" t="s">
         <v>1564</v>
@@ -20069,13 +20069,13 @@
       <c r="V121" s="10"/>
       <c r="W121" s="10"/>
       <c r="X121" s="57" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="Y121" s="10" t="s">
         <v>890</v>
       </c>
       <c r="Z121" s="15" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="122" spans="1:26" ht="170" x14ac:dyDescent="0.2">
@@ -20121,13 +20121,13 @@
       <c r="R122" s="10"/>
       <c r="S122" s="10"/>
       <c r="T122" s="57" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="U122" s="10"/>
       <c r="V122" s="10"/>
       <c r="W122" s="10"/>
       <c r="X122" s="57" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="Y122" s="10" t="s">
         <v>890</v>
@@ -21087,7 +21087,7 @@
       </c>
       <c r="S139" s="10"/>
       <c r="T139" s="10" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="U139" s="10" t="s">
         <v>1095</v>
@@ -21149,7 +21149,7 @@
       </c>
       <c r="S140" s="10"/>
       <c r="T140" s="10" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="U140" s="10" t="s">
         <v>1095</v>
@@ -21617,7 +21617,7 @@
       <c r="R148" s="10"/>
       <c r="S148" s="10"/>
       <c r="T148" s="10" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="U148" s="10"/>
       <c r="V148" s="10"/>
@@ -21679,7 +21679,7 @@
       <c r="V149" s="10"/>
       <c r="W149" s="10"/>
       <c r="X149" s="7" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="Y149" s="7" t="s">
         <v>1187</v>
@@ -21737,7 +21737,7 @@
       <c r="V150" s="7"/>
       <c r="W150" s="7"/>
       <c r="X150" s="7" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="Y150" s="7" t="s">
         <v>1187</v>
@@ -22761,7 +22761,7 @@
       <c r="R168" s="10"/>
       <c r="S168" s="10"/>
       <c r="T168" s="10" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="U168" s="10"/>
       <c r="V168" s="10"/>
@@ -24913,7 +24913,7 @@
         <v>1020</v>
       </c>
       <c r="Z204" s="15" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="205" spans="1:27" ht="153" x14ac:dyDescent="0.2">
@@ -24933,7 +24933,7 @@
       <c r="H205" s="10"/>
       <c r="I205" s="10"/>
       <c r="J205" s="7" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="K205" s="10"/>
       <c r="L205" s="10" t="s">
@@ -24969,7 +24969,7 @@
         <v>648</v>
       </c>
       <c r="Z205" s="14" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="206" spans="1:27" ht="85" x14ac:dyDescent="0.2">
@@ -25341,13 +25341,13 @@
         <v>1312</v>
       </c>
       <c r="H212" s="7" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="I212" s="7" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="J212" s="7" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="K212" s="7" t="s">
         <v>1295</v>
@@ -25375,7 +25375,7 @@
       </c>
       <c r="S212" s="10"/>
       <c r="T212" s="7" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="U212" s="10"/>
       <c r="V212" s="10"/>
@@ -25404,13 +25404,13 @@
         <v>1312</v>
       </c>
       <c r="H213" s="7" t="s">
+        <v>1786</v>
+      </c>
+      <c r="I213" s="7" t="s">
         <v>1787</v>
       </c>
-      <c r="I213" s="7" t="s">
-        <v>1788</v>
-      </c>
       <c r="J213" s="7" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="K213" s="7" t="s">
         <v>1349</v>
@@ -25438,7 +25438,7 @@
       </c>
       <c r="S213" s="10"/>
       <c r="T213" s="7" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="U213" s="10"/>
       <c r="V213" s="10"/>
@@ -25448,7 +25448,7 @@
         <v>850</v>
       </c>
       <c r="Z213" s="14" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="AA213"/>
     </row>
@@ -25469,13 +25469,13 @@
         <v>1312</v>
       </c>
       <c r="H214" s="7" t="s">
+        <v>1786</v>
+      </c>
+      <c r="I214" s="7" t="s">
         <v>1787</v>
       </c>
-      <c r="I214" s="7" t="s">
-        <v>1788</v>
-      </c>
       <c r="J214" s="7" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="K214" s="7" t="s">
         <v>1349</v>
@@ -25503,7 +25503,7 @@
       </c>
       <c r="S214" s="10"/>
       <c r="T214" s="7" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="U214" s="10"/>
       <c r="V214" s="10"/>
@@ -25513,7 +25513,7 @@
         <v>850</v>
       </c>
       <c r="Z214" s="14" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="215" spans="1:27" ht="68" x14ac:dyDescent="0.2">
@@ -25533,13 +25533,13 @@
         <v>1312</v>
       </c>
       <c r="H215" s="7" t="s">
+        <v>1786</v>
+      </c>
+      <c r="I215" s="7" t="s">
         <v>1787</v>
       </c>
-      <c r="I215" s="7" t="s">
-        <v>1788</v>
-      </c>
       <c r="J215" s="7" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="K215" s="7" t="s">
         <v>1295</v>
@@ -25567,7 +25567,7 @@
       </c>
       <c r="S215" s="10"/>
       <c r="T215" s="7" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="U215" s="10"/>
       <c r="V215" s="10"/>
@@ -25595,13 +25595,13 @@
         <v>1312</v>
       </c>
       <c r="H216" s="7" t="s">
+        <v>1786</v>
+      </c>
+      <c r="I216" s="7" t="s">
         <v>1787</v>
       </c>
-      <c r="I216" s="7" t="s">
-        <v>1788</v>
-      </c>
       <c r="J216" s="7" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="K216" s="7" t="s">
         <v>1295</v>
@@ -25629,7 +25629,7 @@
       </c>
       <c r="S216" s="10"/>
       <c r="T216" s="7" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="U216" s="10"/>
       <c r="V216" s="10"/>
@@ -25639,7 +25639,7 @@
         <v>850</v>
       </c>
       <c r="Z216" s="14" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="217" spans="1:27" ht="204" x14ac:dyDescent="0.2">
@@ -26050,19 +26050,19 @@
         <v>591</v>
       </c>
       <c r="G223" s="7" t="s">
+        <v>1806</v>
+      </c>
+      <c r="H223" s="7" t="s">
+        <v>1808</v>
+      </c>
+      <c r="I223" s="7" t="s">
         <v>1807</v>
       </c>
-      <c r="H223" s="7" t="s">
+      <c r="J223" s="7" t="s">
+        <v>1958</v>
+      </c>
+      <c r="K223" s="7" t="s">
         <v>1809</v>
-      </c>
-      <c r="I223" s="7" t="s">
-        <v>1808</v>
-      </c>
-      <c r="J223" s="7" t="s">
-        <v>1959</v>
-      </c>
-      <c r="K223" s="7" t="s">
-        <v>1810</v>
       </c>
       <c r="L223" s="7" t="s">
         <v>815</v>
@@ -26072,13 +26072,13 @@
       </c>
       <c r="N223" s="7"/>
       <c r="O223" s="7" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="P223" s="7" t="s">
         <v>653</v>
       </c>
       <c r="Q223" s="7" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="R223" s="7" t="s">
         <v>8</v>
@@ -26095,7 +26095,7 @@
         <v>465</v>
       </c>
       <c r="Z223" s="15" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="224" spans="1:27" ht="272" x14ac:dyDescent="0.2">
@@ -26110,19 +26110,19 @@
         <v>591</v>
       </c>
       <c r="G224" s="7" t="s">
+        <v>1806</v>
+      </c>
+      <c r="H224" s="7" t="s">
+        <v>1808</v>
+      </c>
+      <c r="I224" s="7" t="s">
         <v>1807</v>
       </c>
-      <c r="H224" s="7" t="s">
+      <c r="J224" s="7" t="s">
+        <v>1958</v>
+      </c>
+      <c r="K224" s="7" t="s">
         <v>1809</v>
-      </c>
-      <c r="I224" s="7" t="s">
-        <v>1808</v>
-      </c>
-      <c r="J224" s="7" t="s">
-        <v>1959</v>
-      </c>
-      <c r="K224" s="7" t="s">
-        <v>1810</v>
       </c>
       <c r="L224" s="7" t="s">
         <v>815</v>
@@ -26132,20 +26132,20 @@
       </c>
       <c r="N224" s="7"/>
       <c r="O224" s="7" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="P224" s="7" t="s">
         <v>653</v>
       </c>
       <c r="Q224" s="7" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="R224" s="7" t="s">
         <v>8</v>
       </c>
       <c r="S224" s="7"/>
       <c r="T224" s="7" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="U224" s="10"/>
       <c r="V224" s="10"/>
@@ -26155,7 +26155,7 @@
         <v>466</v>
       </c>
       <c r="Z224" s="15" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="225" spans="1:26" ht="85" x14ac:dyDescent="0.2">
@@ -26170,16 +26170,16 @@
         <v>591</v>
       </c>
       <c r="G225" s="7" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="H225" s="7" t="s">
+        <v>1898</v>
+      </c>
+      <c r="I225" s="53" t="s">
+        <v>1893</v>
+      </c>
+      <c r="J225" s="10" t="s">
         <v>1899</v>
-      </c>
-      <c r="I225" s="53" t="s">
-        <v>1894</v>
-      </c>
-      <c r="J225" s="10" t="s">
-        <v>1900</v>
       </c>
       <c r="K225" s="7" t="s">
         <v>1481</v>
@@ -26232,7 +26232,7 @@
         <v>591</v>
       </c>
       <c r="G226" s="7" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="H226" s="7" t="s">
         <v>1544</v>
@@ -26241,7 +26241,7 @@
         <v>1542</v>
       </c>
       <c r="J226" s="7" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="K226" s="7" t="s">
         <v>1538</v>
@@ -26267,7 +26267,7 @@
       </c>
       <c r="S226" s="10"/>
       <c r="T226" s="10" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="U226" s="10" t="s">
         <v>469</v>
@@ -26278,7 +26278,7 @@
         <v>470</v>
       </c>
       <c r="Y226" s="10" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="Z226" s="15"/>
     </row>
@@ -26303,7 +26303,7 @@
         <v>1542</v>
       </c>
       <c r="J227" s="7" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="K227" s="7" t="s">
         <v>1539</v>
@@ -26329,7 +26329,7 @@
       </c>
       <c r="S227" s="10"/>
       <c r="T227" s="10" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="U227" s="10" t="s">
         <v>469</v>
@@ -26340,7 +26340,7 @@
         <v>470</v>
       </c>
       <c r="Y227" s="10" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="Z227" s="15"/>
     </row>
@@ -26356,7 +26356,7 @@
         <v>591</v>
       </c>
       <c r="G228" s="7" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="H228" s="7" t="s">
         <v>1544</v>
@@ -26365,7 +26365,7 @@
         <v>1542</v>
       </c>
       <c r="J228" s="7" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="K228" s="7" t="s">
         <v>1539</v>
@@ -26391,7 +26391,7 @@
       </c>
       <c r="S228" s="10"/>
       <c r="T228" s="10" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="U228" s="10" t="s">
         <v>469</v>
@@ -26402,7 +26402,7 @@
         <v>470</v>
       </c>
       <c r="Y228" s="10" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="Z228" s="15"/>
     </row>
@@ -26418,7 +26418,7 @@
         <v>591</v>
       </c>
       <c r="G229" s="7" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="H229" s="7" t="s">
         <v>1544</v>
@@ -26427,7 +26427,7 @@
         <v>1542</v>
       </c>
       <c r="J229" s="7" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="K229" s="7" t="s">
         <v>1539</v>
@@ -26453,7 +26453,7 @@
       </c>
       <c r="S229" s="10"/>
       <c r="T229" s="57" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="U229" s="10"/>
       <c r="V229" s="10"/>
@@ -26461,7 +26461,7 @@
       <c r="X229" s="10"/>
       <c r="Y229" s="10"/>
       <c r="Z229" s="15" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="230" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -26479,13 +26479,13 @@
         <v>39</v>
       </c>
       <c r="H230" s="7" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="I230" s="7" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="J230" s="7" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="K230" s="7" t="s">
         <v>815</v>
@@ -26497,7 +26497,7 @@
         <v>1119</v>
       </c>
       <c r="N230" s="57" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="O230" s="57">
         <v>10</v>
@@ -26506,7 +26506,7 @@
         <v>653</v>
       </c>
       <c r="Q230" s="57" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="R230" s="10">
         <v>838</v>
@@ -26522,10 +26522,10 @@
       <c r="W230" s="10"/>
       <c r="X230" s="10"/>
       <c r="Y230" s="10" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="Z230" s="15" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="231" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -26543,13 +26543,13 @@
         <v>39</v>
       </c>
       <c r="H231" s="7" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="I231" s="7" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="J231" s="7" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="K231" s="7" t="s">
         <v>815</v>
@@ -26561,7 +26561,7 @@
         <v>1119</v>
       </c>
       <c r="N231" s="57" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="O231" s="57">
         <v>10</v>
@@ -26570,14 +26570,14 @@
         <v>653</v>
       </c>
       <c r="Q231" s="57" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="R231" s="10">
         <v>838</v>
       </c>
       <c r="S231" s="10"/>
       <c r="T231" s="10" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="U231" s="57" t="s">
         <v>1004</v>
@@ -26586,7 +26586,7 @@
       <c r="W231" s="10"/>
       <c r="X231" s="10"/>
       <c r="Y231" s="10" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="Z231" s="15"/>
     </row>
@@ -26605,13 +26605,13 @@
         <v>39</v>
       </c>
       <c r="H232" s="7" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="I232" s="7" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="J232" s="7" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="K232" s="7" t="s">
         <v>815</v>
@@ -26623,7 +26623,7 @@
         <v>1119</v>
       </c>
       <c r="N232" s="57" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="O232" s="57">
         <v>20</v>
@@ -26632,14 +26632,14 @@
         <v>779</v>
       </c>
       <c r="Q232" s="57" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="R232" s="10">
         <v>838</v>
       </c>
       <c r="S232" s="10"/>
       <c r="T232" s="10" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="U232" s="57" t="s">
         <v>1004</v>
@@ -26648,10 +26648,10 @@
       <c r="W232" s="10"/>
       <c r="X232" s="10"/>
       <c r="Y232" s="10" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="Z232" s="15" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="233" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -26669,13 +26669,13 @@
         <v>39</v>
       </c>
       <c r="H233" s="7" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="I233" s="7" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="J233" s="7" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="K233" s="7" t="s">
         <v>815</v>
@@ -26687,7 +26687,7 @@
         <v>1119</v>
       </c>
       <c r="N233" s="57" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="O233" s="57">
         <v>19</v>
@@ -26696,14 +26696,14 @@
         <v>779</v>
       </c>
       <c r="Q233" s="57" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="R233" s="10">
         <v>838</v>
       </c>
       <c r="S233" s="10"/>
       <c r="T233" s="10" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="U233" s="57" t="s">
         <v>1004</v>
@@ -26712,7 +26712,7 @@
       <c r="W233" s="10"/>
       <c r="X233" s="10"/>
       <c r="Y233" s="10" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="Z233" s="15"/>
     </row>
@@ -26731,13 +26731,13 @@
         <v>39</v>
       </c>
       <c r="H234" s="7" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="I234" s="7" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="J234" s="7" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="K234" s="7" t="s">
         <v>815</v>
@@ -26749,7 +26749,7 @@
         <v>1119</v>
       </c>
       <c r="N234" s="57" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="O234" s="53">
         <v>18</v>
@@ -26758,7 +26758,7 @@
         <v>779</v>
       </c>
       <c r="Q234" s="57" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="R234" s="10">
         <v>838</v>
@@ -26774,10 +26774,10 @@
       <c r="W234" s="10"/>
       <c r="X234" s="10"/>
       <c r="Y234" s="10" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="Z234" s="15" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="235" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -26795,13 +26795,13 @@
         <v>39</v>
       </c>
       <c r="H235" s="7" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="I235" s="7" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="J235" s="7" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="K235" s="7" t="s">
         <v>815</v>
@@ -26822,14 +26822,14 @@
         <v>653</v>
       </c>
       <c r="Q235" s="57" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="R235" s="10">
         <v>838</v>
       </c>
       <c r="S235" s="10"/>
       <c r="T235" s="10" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="U235" s="57" t="s">
         <v>1004</v>
@@ -26838,7 +26838,7 @@
       <c r="W235" s="10"/>
       <c r="X235" s="10"/>
       <c r="Y235" s="10" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="Z235" s="15"/>
     </row>
@@ -26854,25 +26854,25 @@
         <v>591</v>
       </c>
       <c r="G236" s="7" t="s">
+        <v>1823</v>
+      </c>
+      <c r="H236" s="7" t="s">
+        <v>1827</v>
+      </c>
+      <c r="I236" s="7" t="s">
+        <v>1826</v>
+      </c>
+      <c r="J236" s="7" t="s">
+        <v>1825</v>
+      </c>
+      <c r="K236" s="7" t="s">
         <v>1824</v>
-      </c>
-      <c r="H236" s="7" t="s">
-        <v>1828</v>
-      </c>
-      <c r="I236" s="7" t="s">
-        <v>1827</v>
-      </c>
-      <c r="J236" s="7" t="s">
-        <v>1826</v>
-      </c>
-      <c r="K236" s="7" t="s">
-        <v>1825</v>
       </c>
       <c r="L236" s="7" t="s">
         <v>815</v>
       </c>
       <c r="M236" s="10" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="N236" s="10"/>
       <c r="O236" s="10"/>
@@ -26892,10 +26892,10 @@
       <c r="W236" s="10"/>
       <c r="X236" s="10"/>
       <c r="Y236" s="10" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="Z236" s="15" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="237" spans="1:26" ht="153" x14ac:dyDescent="0.2">
@@ -26910,16 +26910,16 @@
         <v>591</v>
       </c>
       <c r="G237" s="7" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="H237" s="53" t="s">
+        <v>1914</v>
+      </c>
+      <c r="I237" s="53" t="s">
         <v>1915</v>
       </c>
-      <c r="I237" s="53" t="s">
-        <v>1916</v>
-      </c>
       <c r="J237" s="10" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="K237" s="10"/>
       <c r="L237" s="10" t="s">
@@ -26998,7 +26998,7 @@
       <c r="W238" s="10"/>
       <c r="X238" s="10"/>
       <c r="Y238" s="10" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="Z238" s="15" t="s">
         <v>1502</v>
@@ -27054,7 +27054,7 @@
       <c r="W239" s="10"/>
       <c r="X239" s="10"/>
       <c r="Y239" s="10" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="Z239" s="15" t="s">
         <v>1662</v>
@@ -27108,10 +27108,10 @@
       <c r="W240" s="10"/>
       <c r="X240" s="10"/>
       <c r="Y240" s="10" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="Z240" s="15" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="241" spans="1:26" ht="170" x14ac:dyDescent="0.2">
@@ -27184,13 +27184,13 @@
         <v>1522</v>
       </c>
       <c r="K242" s="7" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="L242" s="7" t="s">
+        <v>1746</v>
+      </c>
+      <c r="M242" s="7" t="s">
         <v>1747</v>
-      </c>
-      <c r="M242" s="7" t="s">
-        <v>1748</v>
       </c>
       <c r="N242" s="7"/>
       <c r="O242" s="7">
@@ -27209,10 +27209,10 @@
       <c r="V242" s="10"/>
       <c r="W242" s="10"/>
       <c r="X242" s="10" t="s">
+        <v>1741</v>
+      </c>
+      <c r="Y242" s="10" t="s">
         <v>1742</v>
-      </c>
-      <c r="Y242" s="10" t="s">
-        <v>1743</v>
       </c>
       <c r="Z242" s="15"/>
     </row>
@@ -27553,7 +27553,7 @@
       <c r="B249" s="7"/>
       <c r="C249" s="7"/>
       <c r="D249" s="7" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="E249" s="7"/>
       <c r="F249" s="7" t="s">
@@ -27563,13 +27563,13 @@
         <v>1678</v>
       </c>
       <c r="H249" s="7" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="I249" s="7" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="J249" s="7" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="K249" s="7" t="s">
         <v>815</v>
@@ -27600,10 +27600,10 @@
       <c r="W249" s="10"/>
       <c r="X249" s="10"/>
       <c r="Y249" s="10" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="Z249" s="15" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="250" spans="1:26" ht="34" x14ac:dyDescent="0.2">
@@ -27624,7 +27624,7 @@
       <c r="I250" s="10"/>
       <c r="J250" s="10"/>
       <c r="K250" s="53" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="L250" s="10" t="s">
         <v>815</v>
@@ -27657,7 +27657,7 @@
         <v>1281</v>
       </c>
       <c r="Z250" s="54" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="251" spans="1:26" ht="102" x14ac:dyDescent="0.2">
@@ -27667,7 +27667,7 @@
       <c r="B251" s="7"/>
       <c r="C251" s="7"/>
       <c r="D251" s="7" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="E251" s="7"/>
       <c r="F251" s="7" t="s">
@@ -27680,10 +27680,10 @@
         <v>353</v>
       </c>
       <c r="I251" s="7" t="s">
+        <v>1717</v>
+      </c>
+      <c r="J251" s="7" t="s">
         <v>1718</v>
-      </c>
-      <c r="J251" s="7" t="s">
-        <v>1719</v>
       </c>
       <c r="K251" s="7" t="s">
         <v>209</v>
@@ -27712,12 +27712,12 @@
         <v>1116</v>
       </c>
       <c r="U251" s="7" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="V251" s="10"/>
       <c r="W251" s="10"/>
       <c r="X251" s="7" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="Y251" s="10" t="s">
         <v>1580</v>
@@ -27740,7 +27740,7 @@
         <v>591</v>
       </c>
       <c r="G252" s="10" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="H252" s="10"/>
       <c r="I252" s="10"/>
@@ -27961,13 +27961,13 @@
         <v>46</v>
       </c>
       <c r="H256" s="10" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="I256" s="10" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="J256" s="10" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="K256" s="7" t="s">
         <v>298</v>
@@ -28119,7 +28119,7 @@
       <c r="H259" s="10"/>
       <c r="I259" s="10"/>
       <c r="J259" s="10" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="K259" s="10"/>
       <c r="L259" s="10" t="s">
@@ -28165,16 +28165,16 @@
         <v>990</v>
       </c>
       <c r="H260" s="57" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="I260" s="57" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="J260" s="57" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="K260" s="57" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="L260" s="57" t="s">
         <v>815</v>
@@ -28197,15 +28197,15 @@
       </c>
       <c r="U260" s="10"/>
       <c r="V260" s="57" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="W260" s="10"/>
       <c r="X260" s="10"/>
       <c r="Y260" s="10" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="Z260" s="15" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="261" spans="1:26" ht="68" x14ac:dyDescent="0.2">
@@ -28223,16 +28223,16 @@
         <v>990</v>
       </c>
       <c r="H261" s="10" t="s">
+        <v>1700</v>
+      </c>
+      <c r="I261" s="10" t="s">
         <v>1701</v>
       </c>
-      <c r="I261" s="10" t="s">
-        <v>1702</v>
-      </c>
       <c r="J261" s="10" t="s">
+        <v>1706</v>
+      </c>
+      <c r="K261" s="10" t="s">
         <v>1707</v>
-      </c>
-      <c r="K261" s="10" t="s">
-        <v>1708</v>
       </c>
       <c r="L261" s="10" t="s">
         <v>815</v>
@@ -28259,7 +28259,7 @@
         <v>603</v>
       </c>
       <c r="Z261" s="15" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="262" spans="1:26" ht="102" x14ac:dyDescent="0.2">
@@ -28411,10 +28411,10 @@
       <c r="V264" s="10"/>
       <c r="W264" s="10"/>
       <c r="X264" s="7" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="Y264" s="7" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="Z264" s="15" t="s">
         <v>102</v>
@@ -28532,7 +28532,7 @@
         <v>799</v>
       </c>
       <c r="Y266" s="10" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="Z266" s="15"/>
     </row>
@@ -28592,7 +28592,7 @@
         <v>799</v>
       </c>
       <c r="Y267" s="10" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="Z267" s="15"/>
     </row>
@@ -28652,7 +28652,7 @@
         <v>799</v>
       </c>
       <c r="Y268" s="10" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="Z268" s="15"/>
     </row>
@@ -28673,7 +28673,7 @@
       <c r="H269" s="10"/>
       <c r="I269" s="10"/>
       <c r="J269" s="7" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="K269" s="7" t="s">
         <v>1446</v>
@@ -28771,7 +28771,7 @@
         <v>1166</v>
       </c>
       <c r="Z270" s="14" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="271" spans="1:26" ht="34" x14ac:dyDescent="0.2">
@@ -29271,17 +29271,17 @@
         <v>77</v>
       </c>
       <c r="H279" s="7" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="I279" s="7"/>
       <c r="J279" s="7" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="K279" s="7" t="s">
+        <v>1736</v>
+      </c>
+      <c r="L279" s="7" t="s">
         <v>1737</v>
-      </c>
-      <c r="L279" s="7" t="s">
-        <v>1738</v>
       </c>
       <c r="M279" s="7" t="s">
         <v>630</v>
@@ -29295,7 +29295,7 @@
       </c>
       <c r="Q279" s="10"/>
       <c r="R279" s="10" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="S279" s="10"/>
       <c r="T279" s="10"/>
@@ -29303,10 +29303,10 @@
       <c r="V279" s="7"/>
       <c r="W279" s="7"/>
       <c r="X279" s="7" t="s">
+        <v>1752</v>
+      </c>
+      <c r="Y279" s="7" t="s">
         <v>1753</v>
-      </c>
-      <c r="Y279" s="7" t="s">
-        <v>1754</v>
       </c>
       <c r="Z279" s="15"/>
     </row>
@@ -29325,20 +29325,20 @@
         <v>77</v>
       </c>
       <c r="H280" s="7" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="I280" s="7"/>
       <c r="J280" s="7" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="K280" s="7" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="L280" s="7" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="M280" s="7" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="N280" s="7"/>
       <c r="O280" s="7">
@@ -29349,7 +29349,7 @@
       </c>
       <c r="Q280" s="7"/>
       <c r="R280" s="7" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="S280" s="10"/>
       <c r="T280" s="10"/>
@@ -29377,17 +29377,17 @@
         <v>77</v>
       </c>
       <c r="H281" s="7" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="I281" s="7"/>
       <c r="J281" s="7" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="K281" s="7" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="L281" s="7" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="M281" s="7" t="s">
         <v>1035</v>
@@ -29401,7 +29401,7 @@
       </c>
       <c r="Q281" s="7"/>
       <c r="R281" s="7" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="S281" s="10"/>
       <c r="T281" s="10"/>
@@ -29431,7 +29431,7 @@
       <c r="H282" s="10"/>
       <c r="I282" s="10"/>
       <c r="J282" s="10" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="K282" s="10"/>
       <c r="L282" s="10" t="s">
@@ -29479,7 +29479,7 @@
       <c r="H283" s="10"/>
       <c r="I283" s="10"/>
       <c r="J283" s="7" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="K283" s="7" t="s">
         <v>815</v>
@@ -29512,7 +29512,7 @@
         <v>1032</v>
       </c>
       <c r="Y283" s="10" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="Z283" s="13" t="s">
         <v>35</v>
@@ -29530,19 +29530,19 @@
         <v>591</v>
       </c>
       <c r="G284" s="7" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="H284" s="7" t="s">
+        <v>1811</v>
+      </c>
+      <c r="I284" s="7" t="s">
+        <v>1810</v>
+      </c>
+      <c r="J284" s="7" t="s">
         <v>1812</v>
       </c>
-      <c r="I284" s="7" t="s">
-        <v>1811</v>
-      </c>
-      <c r="J284" s="7" t="s">
-        <v>1813</v>
-      </c>
       <c r="K284" s="7" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="L284" s="7" t="s">
         <v>815</v>
@@ -29551,7 +29551,7 @@
         <v>498</v>
       </c>
       <c r="N284" s="57" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="O284" s="57">
         <v>3</v>
@@ -29560,14 +29560,14 @@
         <v>653</v>
       </c>
       <c r="Q284" s="7" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="R284" s="10">
         <v>843</v>
       </c>
       <c r="S284" s="10"/>
       <c r="T284" s="10" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="U284" s="10"/>
       <c r="V284" s="10"/>
@@ -29576,10 +29576,10 @@
         <v>641</v>
       </c>
       <c r="Y284" s="7" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="Z284" s="15" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="285" spans="1:26" ht="85" x14ac:dyDescent="0.2">
@@ -29594,19 +29594,19 @@
         <v>591</v>
       </c>
       <c r="G285" s="7" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="H285" s="7" t="s">
+        <v>1811</v>
+      </c>
+      <c r="I285" s="7" t="s">
+        <v>1810</v>
+      </c>
+      <c r="J285" s="7" t="s">
         <v>1812</v>
       </c>
-      <c r="I285" s="7" t="s">
-        <v>1811</v>
-      </c>
-      <c r="J285" s="7" t="s">
-        <v>1813</v>
-      </c>
       <c r="K285" s="7" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="L285" s="7" t="s">
         <v>815</v>
@@ -29624,14 +29624,14 @@
         <v>653</v>
       </c>
       <c r="Q285" s="7" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="R285" s="10">
         <v>843</v>
       </c>
       <c r="S285" s="10"/>
       <c r="T285" s="10" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="U285" s="10"/>
       <c r="V285" s="10"/>
@@ -29640,10 +29640,10 @@
         <v>641</v>
       </c>
       <c r="Y285" s="7" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="Z285" s="15" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="286" spans="1:26" ht="51" x14ac:dyDescent="0.2">
@@ -29658,19 +29658,19 @@
         <v>591</v>
       </c>
       <c r="G286" s="7" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="H286" s="7" t="s">
+        <v>1811</v>
+      </c>
+      <c r="I286" s="7" t="s">
+        <v>1810</v>
+      </c>
+      <c r="J286" s="7" t="s">
         <v>1812</v>
       </c>
-      <c r="I286" s="7" t="s">
-        <v>1811</v>
-      </c>
-      <c r="J286" s="7" t="s">
-        <v>1813</v>
-      </c>
       <c r="K286" s="7" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="L286" s="7" t="s">
         <v>815</v>
@@ -29688,14 +29688,14 @@
         <v>779</v>
       </c>
       <c r="Q286" s="7" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="R286" s="10">
         <v>843</v>
       </c>
       <c r="S286" s="10"/>
       <c r="T286" s="10" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="U286" s="10"/>
       <c r="V286" s="10"/>
@@ -29704,10 +29704,10 @@
         <v>641</v>
       </c>
       <c r="Y286" s="7" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="Z286" s="15" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="287" spans="1:26" ht="51" x14ac:dyDescent="0.2">
@@ -29722,19 +29722,19 @@
         <v>591</v>
       </c>
       <c r="G287" s="7" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="H287" s="7" t="s">
+        <v>1811</v>
+      </c>
+      <c r="I287" s="7" t="s">
+        <v>1810</v>
+      </c>
+      <c r="J287" s="7" t="s">
         <v>1812</v>
       </c>
-      <c r="I287" s="7" t="s">
-        <v>1811</v>
-      </c>
-      <c r="J287" s="7" t="s">
-        <v>1813</v>
-      </c>
       <c r="K287" s="7" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="L287" s="7" t="s">
         <v>815</v>
@@ -29752,14 +29752,14 @@
         <v>653</v>
       </c>
       <c r="Q287" s="7" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="R287" s="10">
         <v>843</v>
       </c>
       <c r="S287" s="10"/>
       <c r="T287" s="10" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="U287" s="10"/>
       <c r="V287" s="10"/>
@@ -29768,10 +29768,10 @@
         <v>641</v>
       </c>
       <c r="Y287" s="7" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="Z287" s="15" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="288" spans="1:26" ht="119" x14ac:dyDescent="0.2">
@@ -29786,19 +29786,19 @@
         <v>591</v>
       </c>
       <c r="G288" s="7" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="H288" s="7" t="s">
+        <v>1811</v>
+      </c>
+      <c r="I288" s="7" t="s">
+        <v>1810</v>
+      </c>
+      <c r="J288" s="7" t="s">
         <v>1812</v>
       </c>
-      <c r="I288" s="7" t="s">
-        <v>1811</v>
-      </c>
-      <c r="J288" s="7" t="s">
-        <v>1813</v>
-      </c>
       <c r="K288" s="7" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="L288" s="7" t="s">
         <v>815</v>
@@ -29807,23 +29807,23 @@
         <v>498</v>
       </c>
       <c r="N288" s="57" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="O288" s="57" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="P288" s="57" t="s">
         <v>779</v>
       </c>
       <c r="Q288" s="7" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="R288" s="10">
         <v>843</v>
       </c>
       <c r="S288" s="10"/>
       <c r="T288" s="10" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="U288" s="10"/>
       <c r="V288" s="10"/>
@@ -29832,10 +29832,10 @@
         <v>641</v>
       </c>
       <c r="Y288" s="7" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="Z288" s="15" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="289" spans="1:26" ht="119" x14ac:dyDescent="0.2">
@@ -29850,19 +29850,19 @@
         <v>591</v>
       </c>
       <c r="G289" s="7" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="H289" s="7" t="s">
+        <v>1811</v>
+      </c>
+      <c r="I289" s="7" t="s">
+        <v>1810</v>
+      </c>
+      <c r="J289" s="7" t="s">
         <v>1812</v>
       </c>
-      <c r="I289" s="7" t="s">
-        <v>1811</v>
-      </c>
-      <c r="J289" s="7" t="s">
-        <v>1813</v>
-      </c>
       <c r="K289" s="7" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="L289" s="7" t="s">
         <v>815</v>
@@ -29871,23 +29871,23 @@
         <v>498</v>
       </c>
       <c r="N289" s="57" t="s">
+        <v>1972</v>
+      </c>
+      <c r="O289" s="57" t="s">
         <v>1973</v>
-      </c>
-      <c r="O289" s="57" t="s">
-        <v>1974</v>
       </c>
       <c r="P289" s="57" t="s">
         <v>653</v>
       </c>
       <c r="Q289" s="7" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="R289" s="10">
         <v>843</v>
       </c>
       <c r="S289" s="10"/>
       <c r="T289" s="10" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="U289" s="10"/>
       <c r="V289" s="10"/>
@@ -29896,10 +29896,10 @@
         <v>641</v>
       </c>
       <c r="Y289" s="7" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="Z289" s="15" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="290" spans="1:26" ht="51" x14ac:dyDescent="0.2">
@@ -29917,13 +29917,13 @@
         <v>39</v>
       </c>
       <c r="H290" s="10" t="s">
+        <v>1821</v>
+      </c>
+      <c r="I290" s="10" t="s">
+        <v>1820</v>
+      </c>
+      <c r="J290" s="10" t="s">
         <v>1822</v>
-      </c>
-      <c r="I290" s="10" t="s">
-        <v>1821</v>
-      </c>
-      <c r="J290" s="10" t="s">
-        <v>1823</v>
       </c>
       <c r="K290" s="7" t="s">
         <v>194</v>
@@ -29981,13 +29981,13 @@
         <v>39</v>
       </c>
       <c r="H291" s="10" t="s">
+        <v>1821</v>
+      </c>
+      <c r="I291" s="10" t="s">
+        <v>1820</v>
+      </c>
+      <c r="J291" s="10" t="s">
         <v>1822</v>
-      </c>
-      <c r="I291" s="10" t="s">
-        <v>1821</v>
-      </c>
-      <c r="J291" s="10" t="s">
-        <v>1823</v>
       </c>
       <c r="K291" s="7" t="s">
         <v>194</v>
@@ -30045,13 +30045,13 @@
         <v>39</v>
       </c>
       <c r="H292" s="10" t="s">
+        <v>1821</v>
+      </c>
+      <c r="I292" s="10" t="s">
+        <v>1820</v>
+      </c>
+      <c r="J292" s="10" t="s">
         <v>1822</v>
-      </c>
-      <c r="I292" s="10" t="s">
-        <v>1821</v>
-      </c>
-      <c r="J292" s="10" t="s">
-        <v>1823</v>
       </c>
       <c r="K292" s="7" t="s">
         <v>194</v>
@@ -30109,13 +30109,13 @@
         <v>39</v>
       </c>
       <c r="H293" s="10" t="s">
+        <v>1821</v>
+      </c>
+      <c r="I293" s="10" t="s">
+        <v>1820</v>
+      </c>
+      <c r="J293" s="10" t="s">
         <v>1822</v>
-      </c>
-      <c r="I293" s="10" t="s">
-        <v>1821</v>
-      </c>
-      <c r="J293" s="10" t="s">
-        <v>1823</v>
       </c>
       <c r="K293" s="7" t="s">
         <v>162</v>
@@ -30173,13 +30173,13 @@
         <v>1577</v>
       </c>
       <c r="H294" s="53" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="I294" s="53" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="J294" s="10" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="K294" s="7" t="s">
         <v>388</v>
@@ -30211,13 +30211,13 @@
       <c r="V294" s="10"/>
       <c r="W294" s="7"/>
       <c r="X294" s="7" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="Y294" s="7" t="s">
         <v>831</v>
       </c>
       <c r="Z294" s="15" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="295" spans="1:26" ht="68" x14ac:dyDescent="0.2">
@@ -30731,7 +30731,7 @@
       <c r="H305" s="10"/>
       <c r="I305" s="10"/>
       <c r="J305" s="10" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="K305" s="10"/>
       <c r="L305" s="10" t="s">
@@ -30757,7 +30757,7 @@
       <c r="X305" s="10"/>
       <c r="Y305" s="10"/>
       <c r="Z305" s="15" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="306" spans="1:27" ht="68" x14ac:dyDescent="0.2">
@@ -30779,7 +30779,7 @@
       <c r="H306" s="10"/>
       <c r="I306" s="10"/>
       <c r="J306" s="10" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="K306" s="10"/>
       <c r="L306" s="10" t="s">
@@ -30805,7 +30805,7 @@
       <c r="X306" s="10"/>
       <c r="Y306" s="10"/>
       <c r="Z306" s="15" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="307" spans="1:27" ht="119" x14ac:dyDescent="0.2">
@@ -31358,10 +31358,10 @@
         <v>990</v>
       </c>
       <c r="H318" s="10" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="I318" s="10" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="J318" s="10" t="s">
         <v>215</v>
@@ -31408,13 +31408,13 @@
         <v>990</v>
       </c>
       <c r="H319" s="10" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="I319" s="10" t="s">
+        <v>1702</v>
+      </c>
+      <c r="J319" s="10" t="s">
         <v>1703</v>
-      </c>
-      <c r="J319" s="10" t="s">
-        <v>1704</v>
       </c>
       <c r="K319" s="10"/>
       <c r="L319" s="10" t="s">
@@ -31441,7 +31441,7 @@
       <c r="W319" s="10"/>
       <c r="X319" s="10"/>
       <c r="Y319" s="10" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="Z319" s="15"/>
     </row>
@@ -31460,13 +31460,13 @@
         <v>990</v>
       </c>
       <c r="H320" s="10" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="I320" s="10" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="J320" s="10" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="K320" s="10"/>
       <c r="L320" s="10" t="s">
@@ -31506,13 +31506,13 @@
         <v>1470</v>
       </c>
       <c r="H321" s="7" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="I321" s="7" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="J321" s="7" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="K321" s="7" t="s">
         <v>245</v>
@@ -31559,22 +31559,22 @@
         <v>591</v>
       </c>
       <c r="G322" s="7" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="H322" s="7" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="I322" s="7" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="J322" s="7" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="K322" s="7" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="L322" s="7" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="M322" s="7" t="s">
         <v>751</v>
@@ -31588,7 +31588,7 @@
       </c>
       <c r="Q322" s="7"/>
       <c r="R322" s="7" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="S322" s="10"/>
       <c r="T322" s="7">
@@ -31598,10 +31598,10 @@
       <c r="V322" s="10"/>
       <c r="W322" s="10"/>
       <c r="X322" s="7" t="s">
+        <v>1921</v>
+      </c>
+      <c r="Y322" s="7" t="s">
         <v>1922</v>
-      </c>
-      <c r="Y322" s="7" t="s">
-        <v>1923</v>
       </c>
       <c r="Z322" s="15"/>
     </row>
@@ -31756,10 +31756,10 @@
       <c r="V325" s="10"/>
       <c r="W325" s="10"/>
       <c r="X325" s="7" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="Y325" s="7" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="Z325" s="15"/>
     </row>
@@ -32016,19 +32016,19 @@
         <v>249</v>
       </c>
       <c r="H331" s="53" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="I331" s="53" t="s">
+        <v>1905</v>
+      </c>
+      <c r="J331" s="53" t="s">
         <v>1906</v>
-      </c>
-      <c r="J331" s="53" t="s">
-        <v>1907</v>
       </c>
       <c r="K331" s="7" t="s">
         <v>87</v>
       </c>
       <c r="L331" s="7" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="M331" s="7" t="s">
         <v>1178</v>
@@ -32052,11 +32052,11 @@
       <c r="V331" s="10"/>
       <c r="W331" s="10"/>
       <c r="X331" s="7" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="Y331" s="10"/>
       <c r="Z331" s="54" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="332" spans="1:26" ht="170" x14ac:dyDescent="0.2">
@@ -32338,10 +32338,10 @@
       <c r="H337" s="57"/>
       <c r="I337" s="57"/>
       <c r="J337" s="57" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="K337" s="57" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="L337" s="57" t="s">
         <v>815</v>
@@ -32358,7 +32358,7 @@
       </c>
       <c r="Q337" s="57"/>
       <c r="R337" s="57" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="S337" s="57">
         <v>1881</v>
@@ -32370,13 +32370,13 @@
       <c r="V337" s="10"/>
       <c r="W337" s="10"/>
       <c r="X337" s="57" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="Y337" s="57" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="Z337" s="14" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="338" spans="1:26" ht="85" x14ac:dyDescent="0.2">
@@ -33074,19 +33074,19 @@
         <v>77</v>
       </c>
       <c r="H352" s="7" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="I352" s="7" t="s">
+        <v>1803</v>
+      </c>
+      <c r="J352" s="7" t="s">
         <v>1804</v>
-      </c>
-      <c r="J352" s="7" t="s">
-        <v>1805</v>
       </c>
       <c r="K352" s="7" t="s">
         <v>815</v>
       </c>
       <c r="L352" s="7" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="M352" s="10" t="s">
         <v>1272</v>
@@ -33099,14 +33099,14 @@
       <c r="Q352" s="10"/>
       <c r="R352" s="10"/>
       <c r="S352" s="10" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="T352" s="10"/>
       <c r="U352" s="10"/>
       <c r="V352" s="10"/>
       <c r="W352" s="10"/>
       <c r="X352" s="7" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="Y352" s="10"/>
       <c r="Z352" s="14" t="s">
@@ -33783,7 +33783,7 @@
       </c>
       <c r="L366" s="6"/>
       <c r="M366" s="7" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="N366" s="6"/>
       <c r="O366" s="6">
@@ -33804,7 +33804,7 @@
       <c r="X366" s="6"/>
       <c r="Y366" s="6"/>
       <c r="Z366" s="14" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="367" spans="1:26" ht="404" x14ac:dyDescent="0.2">
@@ -34243,7 +34243,7 @@
       <c r="C375" s="7"/>
       <c r="D375" s="7"/>
       <c r="E375" s="28" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="F375" s="7" t="s">
         <v>164</v>
@@ -34255,7 +34255,7 @@
         <v>243</v>
       </c>
       <c r="I375" s="7" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="J375" s="6"/>
       <c r="K375" s="7" t="s">
@@ -34278,7 +34278,7 @@
       </c>
       <c r="S375" s="6"/>
       <c r="T375" s="6" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="U375" s="6"/>
       <c r="V375" s="6"/>
@@ -34336,7 +34336,7 @@
       </c>
       <c r="S376" s="6"/>
       <c r="T376" s="7" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="U376" s="6"/>
       <c r="V376" s="6"/>
@@ -34392,7 +34392,7 @@
       </c>
       <c r="S377" s="6"/>
       <c r="T377" s="7" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="U377" s="6"/>
       <c r="V377" s="6"/>
@@ -34448,7 +34448,7 @@
       </c>
       <c r="S378" s="6"/>
       <c r="T378" s="7" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="U378" s="6"/>
       <c r="V378" s="6"/>
@@ -34479,7 +34479,7 @@
         <v>1507</v>
       </c>
       <c r="I379" s="6" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="J379" s="6" t="s">
         <v>1506</v>
@@ -34489,7 +34489,7 @@
       </c>
       <c r="L379" s="7"/>
       <c r="M379" s="6" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="N379" s="6"/>
       <c r="O379" s="6">
@@ -34502,14 +34502,14 @@
       <c r="R379" s="6"/>
       <c r="S379" s="6"/>
       <c r="T379" s="7" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="U379" s="6"/>
       <c r="V379" s="6"/>
       <c r="W379" s="6"/>
       <c r="X379" s="6"/>
       <c r="Y379" s="6" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="Z379" s="14" t="s">
         <v>252</v>
@@ -34567,7 +34567,7 @@
       <c r="W380" s="6"/>
       <c r="X380" s="6"/>
       <c r="Y380" s="6" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="Z380" s="14" t="s">
         <v>78</v>
@@ -35004,7 +35004,7 @@
       <c r="B388" s="6"/>
       <c r="C388" s="6"/>
       <c r="D388" s="35" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="E388" s="6"/>
       <c r="F388" s="7" t="s">
@@ -35019,7 +35019,7 @@
       </c>
       <c r="J388" s="7"/>
       <c r="K388" s="7" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="L388" s="6"/>
       <c r="M388" s="7" t="s">
@@ -35038,11 +35038,11 @@
         <v>1062</v>
       </c>
       <c r="R388" s="7" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="S388" s="6"/>
-      <c r="T388" s="6" t="s">
-        <v>1683</v>
+      <c r="T388" s="57" t="s">
+        <v>2114</v>
       </c>
       <c r="U388" s="6"/>
       <c r="V388" s="6"/>
@@ -35058,7 +35058,7 @@
       <c r="B389" s="6"/>
       <c r="C389" s="6"/>
       <c r="D389" s="41" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="E389" s="6"/>
       <c r="F389" s="7" t="s">
@@ -35092,11 +35092,11 @@
         <v>1062</v>
       </c>
       <c r="R389" s="7" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="S389" s="7"/>
       <c r="T389" s="7" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="U389" s="6"/>
       <c r="V389" s="6"/>
@@ -35112,7 +35112,7 @@
       <c r="B390" s="6"/>
       <c r="C390" s="6"/>
       <c r="D390" s="35" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="E390" s="6"/>
       <c r="F390" s="7" t="s">
@@ -35164,7 +35164,7 @@
       <c r="B391" s="6"/>
       <c r="C391" s="6"/>
       <c r="D391" s="35" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="E391" s="6"/>
       <c r="F391" s="7" t="s">
@@ -35508,7 +35508,7 @@
       </c>
       <c r="S397" s="6"/>
       <c r="T397" s="7" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="U397" s="6"/>
       <c r="V397" s="6"/>
@@ -35582,10 +35582,10 @@
         <v>40</v>
       </c>
       <c r="H399" s="6" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="I399" s="6" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="J399" s="7" t="s">
         <v>1610</v>
@@ -35614,7 +35614,7 @@
         <v>1268</v>
       </c>
       <c r="T399" s="7" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="U399" s="7"/>
       <c r="V399" s="7"/>
@@ -35640,10 +35640,10 @@
         <v>40</v>
       </c>
       <c r="H400" s="6" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="I400" s="6" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="J400" s="7" t="s">
         <v>294</v>
@@ -35672,7 +35672,7 @@
         <v>1268</v>
       </c>
       <c r="T400" s="7" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="U400" s="7"/>
       <c r="V400" s="7"/>
@@ -35698,10 +35698,10 @@
         <v>210</v>
       </c>
       <c r="H401" s="6" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="I401" s="6" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="J401" s="7" t="s">
         <v>295</v>
@@ -35746,10 +35746,10 @@
         <v>210</v>
       </c>
       <c r="H402" s="6" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="I402" s="6" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="J402" s="7" t="s">
         <v>295</v>
@@ -35794,10 +35794,10 @@
         <v>210</v>
       </c>
       <c r="H403" s="6" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="I403" s="6" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="J403" s="7" t="s">
         <v>295</v>
@@ -35916,7 +35916,7 @@
       <c r="V405" s="7"/>
       <c r="W405" s="7"/>
       <c r="X405" s="7" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="Y405" s="7"/>
       <c r="Z405" s="15" t="s">
@@ -36151,7 +36151,7 @@
         <v>1579</v>
       </c>
       <c r="G410" s="7" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="H410" s="6" t="s">
         <v>251</v>
@@ -36159,7 +36159,7 @@
       <c r="I410" s="10"/>
       <c r="J410" s="7"/>
       <c r="K410" s="7" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="L410" s="7"/>
       <c r="M410" s="6" t="s">
@@ -36178,7 +36178,7 @@
         <v>1462</v>
       </c>
       <c r="T410" s="7" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="U410" s="7"/>
       <c r="V410" s="7"/>
@@ -36203,7 +36203,7 @@
       <c r="I411" s="6"/>
       <c r="J411" s="6"/>
       <c r="K411" s="7" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="L411" s="7"/>
       <c r="M411" s="7" t="s">
@@ -36235,7 +36235,7 @@
     </row>
     <row r="412" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A412" s="47" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="B412" s="7"/>
       <c r="C412" s="7"/>
@@ -36253,7 +36253,7 @@
         <v>1665</v>
       </c>
       <c r="K412" s="7" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="L412" s="7"/>
       <c r="M412" s="7" t="s">
@@ -36267,21 +36267,21 @@
       <c r="Q412" s="7"/>
       <c r="R412" s="7"/>
       <c r="S412" s="7" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="T412" s="7"/>
       <c r="U412" s="7"/>
       <c r="V412" s="7"/>
       <c r="W412" s="7"/>
       <c r="X412" s="7" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="Y412" s="7"/>
       <c r="Z412" s="14"/>
     </row>
     <row r="413" spans="1:26" s="42" customFormat="1" ht="153" x14ac:dyDescent="0.15">
       <c r="A413" s="47" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="B413" s="7"/>
       <c r="C413" s="7"/>
@@ -36294,20 +36294,20 @@
         <v>1591</v>
       </c>
       <c r="H413" s="57" t="s">
+        <v>2047</v>
+      </c>
+      <c r="I413" s="57" t="s">
         <v>2048</v>
       </c>
-      <c r="I413" s="57" t="s">
+      <c r="J413" s="57" t="s">
         <v>2049</v>
-      </c>
-      <c r="J413" s="57" t="s">
-        <v>2050</v>
       </c>
       <c r="K413" s="7" t="s">
         <v>1627</v>
       </c>
       <c r="L413" s="7"/>
       <c r="M413" s="57" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="N413" s="57" t="s">
         <v>1628</v>
@@ -36319,29 +36319,29 @@
         <v>653</v>
       </c>
       <c r="Q413" s="7" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="R413" s="57">
         <v>1360</v>
       </c>
       <c r="S413" s="6"/>
       <c r="T413" s="57" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="U413" s="7"/>
       <c r="V413" s="7"/>
       <c r="W413" s="7"/>
       <c r="X413" s="7"/>
       <c r="Y413" s="7" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="Z413" s="15" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="414" spans="1:26" s="42" customFormat="1" ht="153" x14ac:dyDescent="0.15">
       <c r="A414" s="47" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="B414" s="7"/>
       <c r="C414" s="7"/>
@@ -36354,20 +36354,20 @@
         <v>1591</v>
       </c>
       <c r="H414" s="57" t="s">
+        <v>2047</v>
+      </c>
+      <c r="I414" s="57" t="s">
         <v>2048</v>
       </c>
-      <c r="I414" s="57" t="s">
+      <c r="J414" s="57" t="s">
         <v>2049</v>
-      </c>
-      <c r="J414" s="57" t="s">
-        <v>2050</v>
       </c>
       <c r="K414" s="7" t="s">
         <v>1627</v>
       </c>
       <c r="L414" s="7"/>
       <c r="M414" s="57" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="N414" s="57" t="s">
         <v>1629</v>
@@ -36379,35 +36379,35 @@
         <v>653</v>
       </c>
       <c r="Q414" s="7" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="R414" s="57">
         <v>1360</v>
       </c>
       <c r="S414" s="6"/>
       <c r="T414" s="57" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="U414" s="7"/>
       <c r="V414" s="7"/>
       <c r="W414" s="7"/>
       <c r="X414" s="7"/>
       <c r="Y414" s="7" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="Z414" s="15" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="415" spans="1:26" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A415" s="47" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B415" s="7"/>
       <c r="C415" s="7"/>
       <c r="D415" s="7"/>
       <c r="E415" s="7" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="F415" s="7" t="s">
         <v>722</v>
@@ -36418,50 +36418,50 @@
       <c r="H415" s="6"/>
       <c r="I415" s="6"/>
       <c r="J415" s="57" t="s">
+        <v>2022</v>
+      </c>
+      <c r="K415" s="7" t="s">
         <v>2023</v>
-      </c>
-      <c r="K415" s="7" t="s">
-        <v>2024</v>
       </c>
       <c r="L415" s="7"/>
       <c r="M415" s="57" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="N415" s="6"/>
       <c r="O415" s="6">
         <v>6</v>
       </c>
       <c r="P415" s="7" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="Q415" s="7"/>
       <c r="R415" s="57" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="S415" s="57">
         <v>1881</v>
       </c>
       <c r="T415" s="53" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="U415" s="7"/>
       <c r="V415" s="7"/>
       <c r="W415" s="7"/>
       <c r="X415" s="57" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="Y415" s="7"/>
       <c r="Z415" s="15"/>
     </row>
     <row r="416" spans="1:26" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
       <c r="A416" s="47" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="B416" s="7"/>
       <c r="C416" s="7"/>
       <c r="D416" s="7"/>
       <c r="E416" s="7" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="F416" s="7" t="s">
         <v>722</v>
@@ -36472,14 +36472,14 @@
       <c r="H416" s="6"/>
       <c r="I416" s="6"/>
       <c r="J416" s="53" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="K416" s="53" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="L416" s="7"/>
       <c r="M416" s="57" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="N416" s="6"/>
       <c r="O416" s="6">
@@ -36494,22 +36494,22 @@
         <v>614</v>
       </c>
       <c r="T416" s="57" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="U416" s="7"/>
       <c r="V416" s="7"/>
       <c r="W416" s="7"/>
       <c r="X416" s="57" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="Y416" s="7"/>
       <c r="Z416" s="15" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="417" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A417" s="47" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="B417" s="7"/>
       <c r="C417" s="7"/>
@@ -36519,19 +36519,19 @@
         <v>591</v>
       </c>
       <c r="G417" s="57" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="H417" s="57" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="I417" s="6"/>
       <c r="J417" s="6"/>
       <c r="K417" s="57" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="L417" s="7"/>
       <c r="M417" s="6" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="N417" s="7"/>
       <c r="O417" s="7">
@@ -36541,31 +36541,31 @@
         <v>779</v>
       </c>
       <c r="Q417" s="7" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="R417" s="7"/>
       <c r="S417" s="7" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="T417" s="57" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="U417" s="7"/>
       <c r="V417" s="7"/>
       <c r="W417" s="7"/>
       <c r="X417" s="57" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="Y417" s="7" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="Z417" s="15" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="418" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A418" s="47" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="B418" s="7"/>
       <c r="C418" s="7"/>
@@ -36575,53 +36575,53 @@
         <v>591</v>
       </c>
       <c r="G418" s="57" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="H418" s="57" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="I418" s="6"/>
       <c r="J418" s="6"/>
       <c r="K418" s="57" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="L418" s="7"/>
       <c r="M418" s="6" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="N418" s="7"/>
       <c r="O418" s="7" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="P418" s="7" t="s">
         <v>779</v>
       </c>
       <c r="Q418" s="7" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="R418" s="7"/>
       <c r="S418" s="7" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="T418" s="57" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="U418" s="7"/>
       <c r="V418" s="7"/>
       <c r="W418" s="7"/>
       <c r="X418" s="57" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="Y418" s="7" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="Z418" s="15" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="419" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A419" s="26" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="B419" s="7"/>
       <c r="C419" s="7"/>
@@ -36669,7 +36669,7 @@
     </row>
     <row r="420" spans="1:29" ht="85" x14ac:dyDescent="0.2">
       <c r="A420" s="47" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B420" s="7"/>
       <c r="C420" s="7"/>
@@ -36682,25 +36682,25 @@
         <v>57</v>
       </c>
       <c r="H420" s="53" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="I420" s="53"/>
       <c r="J420" s="55" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="K420" s="7"/>
       <c r="L420" s="7"/>
       <c r="M420" s="7" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="N420" s="7"/>
       <c r="O420" s="7" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="P420" s="7"/>
       <c r="Q420" s="7"/>
       <c r="R420" s="7" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="S420" s="7"/>
       <c r="T420" s="7"/>
@@ -36708,18 +36708,18 @@
       <c r="V420" s="7"/>
       <c r="W420" s="7"/>
       <c r="X420" s="7" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="Y420" s="7" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="Z420" s="15" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="421" spans="1:29" ht="85" x14ac:dyDescent="0.2">
       <c r="A421" s="47" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B421" s="7"/>
       <c r="C421" s="7"/>
@@ -36732,25 +36732,25 @@
         <v>57</v>
       </c>
       <c r="H421" s="53" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="I421" s="53"/>
       <c r="J421" s="55" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="K421" s="7"/>
       <c r="L421" s="7"/>
       <c r="M421" s="7" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="N421" s="7"/>
       <c r="O421" s="7" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="P421" s="7"/>
       <c r="Q421" s="7"/>
       <c r="R421" s="7" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="S421" s="7"/>
       <c r="T421" s="7"/>
@@ -36758,24 +36758,24 @@
       <c r="V421" s="7"/>
       <c r="W421" s="7"/>
       <c r="X421" s="7" t="s">
+        <v>1782</v>
+      </c>
+      <c r="Y421" s="7" t="s">
         <v>1783</v>
       </c>
-      <c r="Y421" s="7" t="s">
-        <v>1784</v>
-      </c>
       <c r="Z421" s="15" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="422" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A422" s="26" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B422" s="7"/>
       <c r="C422" s="7"/>
       <c r="D422" s="7"/>
       <c r="E422" s="56" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="F422" s="7" t="s">
         <v>591</v>
@@ -36784,20 +36784,20 @@
         <v>57</v>
       </c>
       <c r="H422" s="53" t="s">
+        <v>1695</v>
+      </c>
+      <c r="I422" s="53" t="s">
         <v>1696</v>
       </c>
-      <c r="I422" s="53" t="s">
+      <c r="J422" s="55" t="s">
         <v>1697</v>
       </c>
-      <c r="J422" s="55" t="s">
+      <c r="K422" s="7" t="s">
         <v>1698</v>
-      </c>
-      <c r="K422" s="7" t="s">
-        <v>1699</v>
       </c>
       <c r="L422" s="7"/>
       <c r="M422" s="7" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="N422" s="7" t="s">
         <v>443</v>
@@ -36809,7 +36809,7 @@
         <v>653</v>
       </c>
       <c r="Q422" s="7" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="R422" s="7">
         <v>974</v>
@@ -36822,32 +36822,32 @@
       <c r="X422" s="7"/>
       <c r="Y422" s="7"/>
       <c r="Z422" s="15" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="423" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A423" s="47" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="B423" s="7"/>
       <c r="C423" s="7"/>
       <c r="D423" s="7"/>
       <c r="E423" s="56" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="F423" s="7" t="s">
         <v>591</v>
       </c>
       <c r="G423" s="7" t="s">
+        <v>1755</v>
+      </c>
+      <c r="H423" s="7" t="s">
         <v>1756</v>
-      </c>
-      <c r="H423" s="7" t="s">
-        <v>1757</v>
       </c>
       <c r="I423" s="53"/>
       <c r="J423" s="55"/>
       <c r="K423" s="7" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="L423" s="7"/>
       <c r="M423" s="7"/>
@@ -36866,12 +36866,12 @@
       <c r="X423" s="7"/>
       <c r="Y423" s="7"/>
       <c r="Z423" s="15" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="424" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A424" s="47" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="B424" s="7"/>
       <c r="C424" s="7"/>
@@ -36885,11 +36885,11 @@
       <c r="I424" s="53"/>
       <c r="J424" s="55"/>
       <c r="K424" s="7" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="L424" s="7"/>
       <c r="M424" s="57" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="N424" s="7"/>
       <c r="O424" s="7"/>
@@ -36908,12 +36908,12 @@
       <c r="X424" s="53"/>
       <c r="Y424" s="7"/>
       <c r="Z424" s="15" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="425" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A425" s="47" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="B425" s="7"/>
       <c r="C425" s="7"/>
@@ -36929,11 +36929,11 @@
       <c r="I425" s="6"/>
       <c r="J425" s="7"/>
       <c r="K425" s="53" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="L425" s="7"/>
       <c r="M425" s="53" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="N425" s="7"/>
       <c r="O425" s="6">
@@ -36944,21 +36944,21 @@
       </c>
       <c r="Q425" s="7"/>
       <c r="R425" s="7" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="S425" s="7"/>
       <c r="T425" s="7" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="U425" s="7"/>
       <c r="V425" s="7"/>
       <c r="W425" s="7"/>
       <c r="X425" s="53"/>
       <c r="Y425" s="53" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="Z425" s="15" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="AA425"/>
       <c r="AB425"/>
@@ -36966,7 +36966,7 @@
     </row>
     <row r="426" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A426" s="47" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="B426" s="7"/>
       <c r="C426" s="7"/>
@@ -36982,11 +36982,11 @@
       <c r="I426" s="6"/>
       <c r="J426" s="7"/>
       <c r="K426" s="53" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="L426" s="7"/>
       <c r="M426" s="53" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="N426" s="7"/>
       <c r="O426" s="6">
@@ -36997,21 +36997,21 @@
       </c>
       <c r="Q426" s="7"/>
       <c r="R426" s="7" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="S426" s="7"/>
       <c r="T426" s="7" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="U426" s="7"/>
       <c r="V426" s="7"/>
       <c r="W426" s="7"/>
       <c r="X426" s="53"/>
       <c r="Y426" s="53" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="Z426" s="15" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="AA426"/>
       <c r="AB426"/>
@@ -37019,7 +37019,7 @@
     </row>
     <row r="427" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A427" s="47" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="B427" s="7"/>
       <c r="C427" s="7"/>
@@ -37035,11 +37035,11 @@
       <c r="I427" s="6"/>
       <c r="J427" s="7"/>
       <c r="K427" s="53" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="L427" s="7"/>
       <c r="M427" s="53" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="N427" s="7"/>
       <c r="O427" s="6">
@@ -37050,21 +37050,21 @@
       </c>
       <c r="Q427" s="7"/>
       <c r="R427" s="7" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="S427" s="7"/>
       <c r="T427" s="7" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="U427" s="7"/>
       <c r="V427" s="7"/>
       <c r="W427" s="7"/>
       <c r="X427" s="53"/>
       <c r="Y427" s="53" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="Z427" s="15" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="AA427"/>
       <c r="AB427"/>
@@ -37072,7 +37072,7 @@
     </row>
     <row r="428" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A428" s="47" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="B428" s="7"/>
       <c r="C428" s="7"/>
@@ -37088,11 +37088,11 @@
       <c r="I428" s="6"/>
       <c r="J428" s="7"/>
       <c r="K428" s="53" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="L428" s="7"/>
       <c r="M428" s="53" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="N428" s="7"/>
       <c r="O428" s="6">
@@ -37103,21 +37103,21 @@
       </c>
       <c r="Q428" s="7"/>
       <c r="R428" s="7" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="S428" s="7"/>
       <c r="T428" s="7" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="U428" s="7"/>
       <c r="V428" s="7"/>
       <c r="W428" s="7"/>
       <c r="X428" s="53"/>
       <c r="Y428" s="53" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="Z428" s="15" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="AA428"/>
       <c r="AB428"/>
@@ -37125,7 +37125,7 @@
     </row>
     <row r="429" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A429" s="47" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="B429" s="7"/>
       <c r="C429" s="7"/>
@@ -37135,51 +37135,51 @@
         <v>591</v>
       </c>
       <c r="G429" s="7" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="H429" s="7" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="I429" s="7" t="s">
+        <v>1814</v>
+      </c>
+      <c r="J429" s="7" t="s">
         <v>1815</v>
       </c>
-      <c r="J429" s="7" t="s">
-        <v>1816</v>
-      </c>
       <c r="K429" s="6" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="L429" s="7"/>
       <c r="M429" s="7" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="N429" s="53"/>
       <c r="O429" s="53"/>
       <c r="P429" s="7" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="Q429" s="7" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="R429" s="7"/>
       <c r="S429" s="7"/>
       <c r="T429" s="53" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="U429" s="7"/>
       <c r="V429" s="7"/>
       <c r="W429" s="7"/>
       <c r="X429" s="7"/>
       <c r="Y429" s="7" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="Z429" s="15" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="430" spans="1:29" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A430" s="47" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="B430" s="7"/>
       <c r="C430" s="7"/>
@@ -37195,11 +37195,11 @@
       <c r="I430" s="6"/>
       <c r="J430" s="53"/>
       <c r="K430" s="53" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
       <c r="L430" s="7"/>
       <c r="M430" s="53" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="N430" s="7"/>
       <c r="O430" s="6"/>
@@ -37208,20 +37208,20 @@
       </c>
       <c r="Q430" s="7"/>
       <c r="R430" s="7" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="S430" s="7"/>
       <c r="T430" s="7" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="U430" s="7"/>
       <c r="V430" s="7"/>
       <c r="W430" s="7"/>
       <c r="X430" s="7" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="Y430" s="7" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="Z430" s="15"/>
       <c r="AA430"/>
@@ -37230,7 +37230,7 @@
     </row>
     <row r="431" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A431" s="47" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="B431" s="7"/>
       <c r="C431" s="7"/>
@@ -37245,11 +37245,11 @@
       <c r="H431" s="6"/>
       <c r="I431" s="6"/>
       <c r="K431" s="53" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="L431" s="7"/>
       <c r="M431" s="53" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="N431" s="7"/>
       <c r="O431" s="6">
@@ -37260,7 +37260,7 @@
       </c>
       <c r="Q431" s="7"/>
       <c r="R431" s="7" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="S431" s="7"/>
       <c r="T431" s="7"/>
@@ -37268,11 +37268,11 @@
       <c r="V431" s="7"/>
       <c r="W431" s="7"/>
       <c r="X431" s="7" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="Y431" s="7"/>
       <c r="Z431" s="15" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="AA431"/>
       <c r="AB431"/>
@@ -37280,7 +37280,7 @@
     </row>
     <row r="432" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A432" s="47" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="B432" s="7"/>
       <c r="C432" s="7"/>
@@ -37295,22 +37295,22 @@
       <c r="H432" s="6"/>
       <c r="I432" s="6"/>
       <c r="K432" s="53" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="L432" s="7"/>
       <c r="M432" s="53" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="N432" s="7"/>
       <c r="O432" s="6">
         <v>3</v>
       </c>
       <c r="P432" s="7" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
       <c r="Q432" s="7"/>
       <c r="R432" s="7" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="S432" s="7"/>
       <c r="T432" s="7"/>
@@ -37318,11 +37318,11 @@
       <c r="V432" s="7"/>
       <c r="W432" s="7"/>
       <c r="X432" s="7" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="Y432" s="7"/>
       <c r="Z432" s="15" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="AA432"/>
       <c r="AB432"/>
@@ -37459,7 +37459,7 @@
       <c r="R435" s="41"/>
       <c r="S435" s="41"/>
       <c r="T435" s="59" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="U435" s="41"/>
       <c r="V435" s="41"/>
@@ -37507,7 +37507,7 @@
       <c r="R436" s="7"/>
       <c r="S436" s="7"/>
       <c r="T436" s="53" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="U436" s="7"/>
       <c r="V436" s="7"/>
@@ -37538,7 +37538,7 @@
         <v>1395</v>
       </c>
       <c r="K437" s="7" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="L437" s="7"/>
       <c r="M437" s="7" t="s">
@@ -37555,7 +37555,7 @@
       <c r="R437" s="7"/>
       <c r="S437" s="7"/>
       <c r="T437" s="53" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="U437" s="7"/>
       <c r="V437" s="7"/>
@@ -37571,7 +37571,7 @@
     </row>
     <row r="438" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A438" s="47" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="B438" s="7"/>
       <c r="C438" s="7"/>
@@ -37602,7 +37602,7 @@
       <c r="X438" s="7"/>
       <c r="Y438" s="7"/>
       <c r="Z438" s="15" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="AA438"/>
       <c r="AB438"/>
@@ -37610,7 +37610,7 @@
     </row>
     <row r="439" spans="1:29" s="42" customFormat="1" ht="153" x14ac:dyDescent="0.15">
       <c r="A439" s="47" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="B439" s="7"/>
       <c r="C439" s="7"/>
@@ -37623,35 +37623,35 @@
         <v>39</v>
       </c>
       <c r="H439" s="7" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="I439" s="7" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="J439" s="7" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="K439" s="7" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="L439" s="7"/>
       <c r="M439" s="7" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="N439" s="7"/>
       <c r="O439" s="6" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="P439" s="7" t="s">
         <v>779</v>
       </c>
       <c r="Q439" s="7" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="R439" s="7"/>
       <c r="S439" s="7"/>
       <c r="T439" s="7" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="U439" s="7"/>
       <c r="V439" s="7"/>
@@ -37665,7 +37665,7 @@
     </row>
     <row r="440" spans="1:29" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A440" s="47" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="B440" s="7"/>
       <c r="C440" s="7"/>
@@ -37679,11 +37679,11 @@
       <c r="I440" s="6"/>
       <c r="J440" s="7"/>
       <c r="K440" s="53" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="L440" s="7"/>
       <c r="M440" s="53" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="N440" s="7"/>
       <c r="O440" s="6">
@@ -37694,13 +37694,13 @@
       <c r="R440" s="7"/>
       <c r="S440" s="7"/>
       <c r="T440" s="7" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="U440" s="7"/>
       <c r="V440" s="7"/>
       <c r="W440" s="7"/>
       <c r="X440" s="7" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="Y440" s="7"/>
       <c r="Z440" s="15"/>
@@ -37710,7 +37710,7 @@
     </row>
     <row r="441" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
       <c r="A441" s="47" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="B441" s="7"/>
       <c r="C441" s="7"/>
@@ -37723,20 +37723,20 @@
         <v>77</v>
       </c>
       <c r="H441" s="6" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="I441" s="6" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="J441" s="53" t="s">
+        <v>1843</v>
+      </c>
+      <c r="K441" s="7" t="s">
         <v>1844</v>
-      </c>
-      <c r="K441" s="7" t="s">
-        <v>1845</v>
       </c>
       <c r="L441" s="7"/>
       <c r="M441" s="53" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="N441" s="7"/>
       <c r="O441" s="6">
@@ -37744,7 +37744,7 @@
       </c>
       <c r="P441" s="7"/>
       <c r="Q441" s="7" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="R441" s="7"/>
       <c r="S441" s="7"/>
@@ -37755,7 +37755,7 @@
       <c r="X441" s="7"/>
       <c r="Y441" s="7"/>
       <c r="Z441" s="15" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="AA441"/>
       <c r="AB441"/>
@@ -37844,7 +37844,7 @@
       <c r="R443" s="6"/>
       <c r="S443" s="6"/>
       <c r="T443" s="7" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="U443" s="7"/>
       <c r="V443" s="7"/>
@@ -37855,7 +37855,7 @@
     </row>
     <row r="444" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A444" s="47" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="B444" s="7"/>
       <c r="C444" s="7"/>
@@ -37865,10 +37865,10 @@
         <v>591</v>
       </c>
       <c r="G444" s="7" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="H444" s="7" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="I444" s="7" t="s">
         <v>1679</v>
@@ -37877,11 +37877,11 @@
         <v>1680</v>
       </c>
       <c r="K444" s="7" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="L444" s="7"/>
       <c r="M444" s="7" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="N444" s="53"/>
       <c r="O444" s="7">
@@ -37891,14 +37891,14 @@
         <v>653</v>
       </c>
       <c r="Q444" s="7" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="R444" s="53">
         <v>1265</v>
       </c>
       <c r="S444" s="7"/>
       <c r="T444" s="7" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="U444" s="7"/>
       <c r="V444" s="7"/>
@@ -37911,7 +37911,7 @@
     </row>
     <row r="446" spans="1:29" s="42" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A446" s="47" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="B446" s="7"/>
       <c r="C446" s="7"/>
@@ -37921,23 +37921,23 @@
         <v>591</v>
       </c>
       <c r="G446" s="7" t="s">
+        <v>1806</v>
+      </c>
+      <c r="H446" s="7" t="s">
+        <v>1808</v>
+      </c>
+      <c r="I446" s="7" t="s">
         <v>1807</v>
       </c>
-      <c r="H446" s="7" t="s">
-        <v>1809</v>
-      </c>
-      <c r="I446" s="7" t="s">
-        <v>1808</v>
-      </c>
       <c r="J446" s="7" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="K446" s="7" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="L446" s="7"/>
       <c r="M446" s="6" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="N446" s="53" t="s">
         <v>443</v>
@@ -37949,27 +37949,27 @@
         <v>779</v>
       </c>
       <c r="Q446" s="7" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="R446" s="7"/>
       <c r="S446" s="53" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="T446" s="7" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="U446" s="7"/>
       <c r="V446" s="7"/>
       <c r="W446" s="7"/>
       <c r="X446" s="7"/>
       <c r="Y446" s="53" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="Z446" s="15"/>
     </row>
     <row r="447" spans="1:29" s="42" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A447" s="47" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="B447" s="7"/>
       <c r="C447" s="7"/>
@@ -37979,23 +37979,23 @@
         <v>591</v>
       </c>
       <c r="G447" s="7" t="s">
+        <v>1806</v>
+      </c>
+      <c r="H447" s="7" t="s">
+        <v>1808</v>
+      </c>
+      <c r="I447" s="7" t="s">
         <v>1807</v>
       </c>
-      <c r="H447" s="7" t="s">
-        <v>1809</v>
-      </c>
-      <c r="I447" s="7" t="s">
-        <v>1808</v>
-      </c>
       <c r="J447" s="7" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="K447" s="7" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="L447" s="7"/>
       <c r="M447" s="6" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="N447" s="53" t="s">
         <v>1251</v>
@@ -38007,11 +38007,11 @@
         <v>680</v>
       </c>
       <c r="Q447" s="7" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="R447" s="7"/>
       <c r="S447" s="53" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="T447" s="7"/>
       <c r="U447" s="7"/>
@@ -38019,13 +38019,13 @@
       <c r="W447" s="7"/>
       <c r="X447" s="7"/>
       <c r="Y447" s="53" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="Z447" s="15"/>
     </row>
     <row r="448" spans="1:29" s="42" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A448" s="47" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="B448" s="7"/>
       <c r="C448" s="7"/>
@@ -38035,55 +38035,55 @@
         <v>591</v>
       </c>
       <c r="G448" s="7" t="s">
+        <v>1806</v>
+      </c>
+      <c r="H448" s="7" t="s">
+        <v>1808</v>
+      </c>
+      <c r="I448" s="7" t="s">
         <v>1807</v>
       </c>
-      <c r="H448" s="7" t="s">
-        <v>1809</v>
-      </c>
-      <c r="I448" s="7" t="s">
-        <v>1808</v>
-      </c>
       <c r="J448" s="7" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="K448" s="7" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="L448" s="7"/>
       <c r="M448" s="6" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="N448" s="53" t="s">
         <v>444</v>
       </c>
       <c r="O448" s="53" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="P448" s="53" t="s">
         <v>680</v>
       </c>
       <c r="Q448" s="7" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="R448" s="7"/>
       <c r="S448" s="53" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="T448" s="7" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="U448" s="7"/>
       <c r="V448" s="7"/>
       <c r="W448" s="7"/>
       <c r="X448" s="7"/>
       <c r="Y448" s="53" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="Z448" s="15"/>
     </row>
     <row r="449" spans="1:26" s="42" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A449" s="47" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="B449" s="7"/>
       <c r="C449" s="7"/>
@@ -38093,49 +38093,49 @@
         <v>591</v>
       </c>
       <c r="G449" s="7" t="s">
+        <v>1806</v>
+      </c>
+      <c r="H449" s="7" t="s">
+        <v>1808</v>
+      </c>
+      <c r="I449" s="7" t="s">
         <v>1807</v>
       </c>
-      <c r="H449" s="7" t="s">
-        <v>1809</v>
-      </c>
-      <c r="I449" s="7" t="s">
-        <v>1808</v>
-      </c>
       <c r="J449" s="7" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="K449" s="7" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="L449" s="7"/>
       <c r="M449" s="6" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="N449" s="53" t="s">
         <v>577</v>
       </c>
       <c r="O449" s="53" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="P449" s="53" t="s">
         <v>680</v>
       </c>
       <c r="Q449" s="7" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="R449" s="7"/>
       <c r="S449" s="53" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="T449" s="7" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="U449" s="7"/>
       <c r="V449" s="7"/>
       <c r="W449" s="7"/>
       <c r="X449" s="7"/>
       <c r="Y449" s="53" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="Z449" s="15"/>
     </row>
@@ -38152,13 +38152,13 @@
         <v>45</v>
       </c>
       <c r="H450" s="6" t="s">
+        <v>2070</v>
+      </c>
+      <c r="I450" s="6" t="s">
         <v>2071</v>
       </c>
-      <c r="I450" s="6" t="s">
+      <c r="J450" s="6" t="s">
         <v>2072</v>
-      </c>
-      <c r="J450" s="6" t="s">
-        <v>2073</v>
       </c>
       <c r="K450" s="6"/>
       <c r="L450" s="7"/>
@@ -38178,7 +38178,7 @@
       <c r="X450" s="7"/>
       <c r="Y450" s="7"/>
       <c r="Z450" s="15" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="451" spans="1:26" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
@@ -38196,14 +38196,14 @@
       <c r="H451" s="6"/>
       <c r="I451" s="6"/>
       <c r="J451" s="6" t="s">
+        <v>1940</v>
+      </c>
+      <c r="K451" s="6" t="s">
         <v>1941</v>
-      </c>
-      <c r="K451" s="6" t="s">
-        <v>1942</v>
       </c>
       <c r="L451" s="7"/>
       <c r="M451" s="6" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="N451" s="7"/>
       <c r="O451" s="7"/>
@@ -38217,7 +38217,7 @@
       <c r="W451" s="7"/>
       <c r="X451" s="7"/>
       <c r="Y451" s="7" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="Z451" s="15"/>
     </row>
@@ -38235,7 +38235,7 @@
       <c r="I452" s="6"/>
       <c r="J452" s="6"/>
       <c r="K452" s="53" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="L452" s="7"/>
       <c r="M452" s="6" t="s">
@@ -38271,7 +38271,7 @@
       <c r="I453" s="6"/>
       <c r="J453" s="6"/>
       <c r="K453" s="7" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="L453" s="7"/>
       <c r="M453" s="6" t="s">
@@ -38310,7 +38310,7 @@
       <c r="H454" s="10"/>
       <c r="I454" s="10"/>
       <c r="J454" s="6" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="K454" s="7" t="s">
         <v>897</v>
@@ -38341,7 +38341,7 @@
     </row>
     <row r="455" spans="1:26" s="42" customFormat="1" ht="255" x14ac:dyDescent="0.15">
       <c r="A455" s="26" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="B455" s="7"/>
       <c r="C455" s="7"/>
@@ -38354,30 +38354,30 @@
         <v>45</v>
       </c>
       <c r="H455" s="6" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="I455" s="6"/>
       <c r="J455" s="6" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="K455" s="6" t="s">
         <v>815</v>
       </c>
       <c r="L455" s="7"/>
       <c r="M455" s="7" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="N455" s="7"/>
       <c r="O455" s="60" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="P455" s="53" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="Q455" s="7"/>
       <c r="R455" s="7"/>
       <c r="S455" s="53" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="T455" s="7"/>
       <c r="U455" s="7"/>
@@ -38386,7 +38386,7 @@
       <c r="X455" s="7"/>
       <c r="Y455" s="7"/>
       <c r="Z455" s="15" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="456" spans="1:26" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
modified metadata and rtfs
</commit_message>
<xml_diff>
--- a/metadata/InventaireCampa.xlsx
+++ b/metadata/InventaireCampa.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arlogriffiths/Documents/GitHub/DHARMA/tfc-campa-epigraphy/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{E80ACA52-2CC8-F84C-BC40-02D927E6AC6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{04FFAD1A-04AF-5449-82E9-2D207C6CC06A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4900" windowWidth="33520" windowHeight="15380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$Z$454</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$Z$455</definedName>
   </definedNames>
   <calcPr calcId="110000"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5209" uniqueCount="2115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5224" uniqueCount="2115">
   <si>
     <t>Quảng Nam</t>
     <phoneticPr fontId="1"/>
@@ -13188,12 +13188,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC456"/>
+  <dimension ref="A1:AC457"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1300" topLeftCell="A289" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1300" topLeftCell="A419" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="V294" sqref="V294"/>
+      <selection pane="bottomLeft" activeCell="A424" sqref="A424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36768,7 +36768,7 @@
       </c>
     </row>
     <row r="422" spans="1:29" ht="34" x14ac:dyDescent="0.2">
-      <c r="A422" s="26" t="s">
+      <c r="A422" s="47" t="s">
         <v>2013</v>
       </c>
       <c r="B422" s="7"/>
@@ -36826,38 +36826,52 @@
       </c>
     </row>
     <row r="423" spans="1:29" ht="34" x14ac:dyDescent="0.2">
-      <c r="A423" s="47" t="s">
-        <v>2038</v>
+      <c r="A423" s="26" t="s">
+        <v>2013</v>
       </c>
       <c r="B423" s="7"/>
       <c r="C423" s="7"/>
       <c r="D423" s="7"/>
       <c r="E423" s="56" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="F423" s="7" t="s">
         <v>591</v>
       </c>
       <c r="G423" s="7" t="s">
-        <v>1754</v>
-      </c>
-      <c r="H423" s="7" t="s">
-        <v>1755</v>
-      </c>
-      <c r="I423" s="53"/>
-      <c r="J423" s="55"/>
+        <v>57</v>
+      </c>
+      <c r="H423" s="53" t="s">
+        <v>1694</v>
+      </c>
+      <c r="I423" s="53" t="s">
+        <v>1695</v>
+      </c>
+      <c r="J423" s="55" t="s">
+        <v>1696</v>
+      </c>
       <c r="K423" s="7" t="s">
-        <v>1756</v>
+        <v>1697</v>
       </c>
       <c r="L423" s="7"/>
-      <c r="M423" s="7"/>
-      <c r="N423" s="7"/>
+      <c r="M423" s="7" t="s">
+        <v>1688</v>
+      </c>
+      <c r="N423" s="7" t="s">
+        <v>611</v>
+      </c>
       <c r="O423" s="7">
-        <v>2</v>
-      </c>
-      <c r="P423" s="7"/>
-      <c r="Q423" s="7"/>
-      <c r="R423" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="P423" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q423" s="7" t="s">
+        <v>1689</v>
+      </c>
+      <c r="R423" s="7">
+        <v>974</v>
+      </c>
       <c r="S423" s="7"/>
       <c r="T423" s="7"/>
       <c r="U423" s="7"/>
@@ -36866,107 +36880,102 @@
       <c r="X423" s="7"/>
       <c r="Y423" s="7"/>
       <c r="Z423" s="15" t="s">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="424" spans="1:29" ht="68" x14ac:dyDescent="0.2">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="424" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A424" s="47" t="s">
-        <v>2066</v>
+        <v>2038</v>
       </c>
       <c r="B424" s="7"/>
       <c r="C424" s="7"/>
       <c r="D424" s="7"/>
-      <c r="E424" s="56"/>
+      <c r="E424" s="56" t="s">
+        <v>1770</v>
+      </c>
       <c r="F424" s="7" t="s">
         <v>591</v>
       </c>
-      <c r="G424" s="7"/>
-      <c r="H424" s="7"/>
+      <c r="G424" s="7" t="s">
+        <v>1754</v>
+      </c>
+      <c r="H424" s="7" t="s">
+        <v>1755</v>
+      </c>
       <c r="I424" s="53"/>
       <c r="J424" s="55"/>
       <c r="K424" s="7" t="s">
-        <v>1998</v>
+        <v>1756</v>
       </c>
       <c r="L424" s="7"/>
-      <c r="M424" s="57" t="s">
-        <v>2065</v>
+      <c r="M424" s="7" t="s">
+        <v>1688</v>
       </c>
       <c r="N424" s="7"/>
-      <c r="O424" s="7"/>
+      <c r="O424" s="7">
+        <v>2</v>
+      </c>
       <c r="P424" s="7" t="s">
-        <v>653</v>
+        <v>779</v>
       </c>
       <c r="Q424" s="7"/>
-      <c r="R424" s="7">
-        <v>1013</v>
-      </c>
+      <c r="R424" s="7"/>
       <c r="S424" s="7"/>
       <c r="T424" s="7"/>
       <c r="U424" s="7"/>
       <c r="V424" s="7"/>
       <c r="W424" s="7"/>
-      <c r="X424" s="53"/>
+      <c r="X424" s="7"/>
       <c r="Y424" s="7"/>
       <c r="Z424" s="15" t="s">
-        <v>1999</v>
-      </c>
-    </row>
-    <row r="425" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="425" spans="1:29" ht="68" x14ac:dyDescent="0.2">
       <c r="A425" s="47" t="s">
-        <v>2086</v>
+        <v>2066</v>
       </c>
       <c r="B425" s="7"/>
       <c r="C425" s="7"/>
       <c r="D425" s="7"/>
-      <c r="E425" s="7"/>
+      <c r="E425" s="56"/>
       <c r="F425" s="7" t="s">
         <v>591</v>
       </c>
-      <c r="G425" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H425" s="6"/>
-      <c r="I425" s="6"/>
-      <c r="J425" s="7"/>
-      <c r="K425" s="53" t="s">
-        <v>1864</v>
+      <c r="G425" s="7"/>
+      <c r="H425" s="7"/>
+      <c r="I425" s="53"/>
+      <c r="J425" s="55"/>
+      <c r="K425" s="7" t="s">
+        <v>1998</v>
       </c>
       <c r="L425" s="7"/>
-      <c r="M425" s="53" t="s">
-        <v>2093</v>
+      <c r="M425" s="57" t="s">
+        <v>2065</v>
       </c>
       <c r="N425" s="7"/>
-      <c r="O425" s="6">
-        <v>1</v>
-      </c>
+      <c r="O425" s="7"/>
       <c r="P425" s="7" t="s">
-        <v>779</v>
+        <v>653</v>
       </c>
       <c r="Q425" s="7"/>
-      <c r="R425" s="7" t="s">
-        <v>2094</v>
+      <c r="R425" s="7">
+        <v>1013</v>
       </c>
       <c r="S425" s="7"/>
-      <c r="T425" s="7" t="s">
-        <v>1863</v>
-      </c>
+      <c r="T425" s="7"/>
       <c r="U425" s="7"/>
       <c r="V425" s="7"/>
       <c r="W425" s="7"/>
       <c r="X425" s="53"/>
-      <c r="Y425" s="53" t="s">
-        <v>2091</v>
-      </c>
+      <c r="Y425" s="7"/>
       <c r="Z425" s="15" t="s">
-        <v>2095</v>
-      </c>
-      <c r="AA425"/>
-      <c r="AB425"/>
-      <c r="AC425"/>
+        <v>1999</v>
+      </c>
     </row>
     <row r="426" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A426" s="47" t="s">
-        <v>2088</v>
+        <v>2086</v>
       </c>
       <c r="B426" s="7"/>
       <c r="C426" s="7"/>
@@ -36982,7 +36991,7 @@
       <c r="I426" s="6"/>
       <c r="J426" s="7"/>
       <c r="K426" s="53" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="L426" s="7"/>
       <c r="M426" s="53" t="s">
@@ -37001,7 +37010,7 @@
       </c>
       <c r="S426" s="7"/>
       <c r="T426" s="7" t="s">
-        <v>1866</v>
+        <v>1863</v>
       </c>
       <c r="U426" s="7"/>
       <c r="V426" s="7"/>
@@ -37019,7 +37028,7 @@
     </row>
     <row r="427" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A427" s="47" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="B427" s="7"/>
       <c r="C427" s="7"/>
@@ -37035,7 +37044,7 @@
       <c r="I427" s="6"/>
       <c r="J427" s="7"/>
       <c r="K427" s="53" t="s">
-        <v>1867</v>
+        <v>1865</v>
       </c>
       <c r="L427" s="7"/>
       <c r="M427" s="53" t="s">
@@ -37054,7 +37063,7 @@
       </c>
       <c r="S427" s="7"/>
       <c r="T427" s="7" t="s">
-        <v>1868</v>
+        <v>1866</v>
       </c>
       <c r="U427" s="7"/>
       <c r="V427" s="7"/>
@@ -37072,7 +37081,7 @@
     </row>
     <row r="428" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A428" s="47" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="B428" s="7"/>
       <c r="C428" s="7"/>
@@ -37088,7 +37097,7 @@
       <c r="I428" s="6"/>
       <c r="J428" s="7"/>
       <c r="K428" s="53" t="s">
-        <v>1869</v>
+        <v>1867</v>
       </c>
       <c r="L428" s="7"/>
       <c r="M428" s="53" t="s">
@@ -37107,7 +37116,7 @@
       </c>
       <c r="S428" s="7"/>
       <c r="T428" s="7" t="s">
-        <v>1870</v>
+        <v>1868</v>
       </c>
       <c r="U428" s="7"/>
       <c r="V428" s="7"/>
@@ -37117,7 +37126,7 @@
         <v>2091</v>
       </c>
       <c r="Z428" s="15" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="AA428"/>
       <c r="AB428"/>
@@ -37125,7 +37134,7 @@
     </row>
     <row r="429" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A429" s="47" t="s">
-        <v>2112</v>
+        <v>2090</v>
       </c>
       <c r="B429" s="7"/>
       <c r="C429" s="7"/>
@@ -37135,51 +37144,50 @@
         <v>591</v>
       </c>
       <c r="G429" s="7" t="s">
-        <v>1805</v>
-      </c>
-      <c r="H429" s="7" t="s">
-        <v>1810</v>
-      </c>
-      <c r="I429" s="7" t="s">
-        <v>1813</v>
-      </c>
-      <c r="J429" s="7" t="s">
-        <v>1814</v>
-      </c>
-      <c r="K429" s="6" t="s">
-        <v>1880</v>
+        <v>77</v>
+      </c>
+      <c r="H429" s="6"/>
+      <c r="I429" s="6"/>
+      <c r="J429" s="7"/>
+      <c r="K429" s="53" t="s">
+        <v>1869</v>
       </c>
       <c r="L429" s="7"/>
-      <c r="M429" s="7" t="s">
-        <v>1881</v>
-      </c>
-      <c r="N429" s="53"/>
-      <c r="O429" s="53"/>
+      <c r="M429" s="53" t="s">
+        <v>2093</v>
+      </c>
+      <c r="N429" s="7"/>
+      <c r="O429" s="6">
+        <v>1</v>
+      </c>
       <c r="P429" s="7" t="s">
-        <v>1882</v>
-      </c>
-      <c r="Q429" s="7" t="s">
-        <v>1884</v>
-      </c>
-      <c r="R429" s="7"/>
+        <v>779</v>
+      </c>
+      <c r="Q429" s="7"/>
+      <c r="R429" s="7" t="s">
+        <v>2094</v>
+      </c>
       <c r="S429" s="7"/>
-      <c r="T429" s="53" t="s">
-        <v>1985</v>
+      <c r="T429" s="7" t="s">
+        <v>1870</v>
       </c>
       <c r="U429" s="7"/>
       <c r="V429" s="7"/>
       <c r="W429" s="7"/>
-      <c r="X429" s="7"/>
-      <c r="Y429" s="7" t="s">
-        <v>1912</v>
+      <c r="X429" s="53"/>
+      <c r="Y429" s="53" t="s">
+        <v>2091</v>
       </c>
       <c r="Z429" s="15" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="430" spans="1:29" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
+        <v>2096</v>
+      </c>
+      <c r="AA429"/>
+      <c r="AB429"/>
+      <c r="AC429"/>
+    </row>
+    <row r="430" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A430" s="47" t="s">
-        <v>2092</v>
+        <v>2112</v>
       </c>
       <c r="B430" s="7"/>
       <c r="C430" s="7"/>
@@ -37189,46 +37197,49 @@
         <v>591</v>
       </c>
       <c r="G430" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H430" s="6"/>
-      <c r="I430" s="6"/>
-      <c r="J430" s="53"/>
-      <c r="K430" s="53" t="s">
-        <v>2101</v>
+        <v>1805</v>
+      </c>
+      <c r="H430" s="7" t="s">
+        <v>1810</v>
+      </c>
+      <c r="I430" s="7" t="s">
+        <v>1813</v>
+      </c>
+      <c r="J430" s="7" t="s">
+        <v>1814</v>
+      </c>
+      <c r="K430" s="6" t="s">
+        <v>1880</v>
       </c>
       <c r="L430" s="7"/>
-      <c r="M430" s="53" t="s">
-        <v>1851</v>
-      </c>
-      <c r="N430" s="7"/>
-      <c r="O430" s="6"/>
+      <c r="M430" s="7" t="s">
+        <v>1881</v>
+      </c>
+      <c r="N430" s="53"/>
+      <c r="O430" s="53"/>
       <c r="P430" s="7" t="s">
-        <v>653</v>
-      </c>
-      <c r="Q430" s="7"/>
-      <c r="R430" s="7" t="s">
-        <v>2087</v>
-      </c>
+        <v>1882</v>
+      </c>
+      <c r="Q430" s="7" t="s">
+        <v>1884</v>
+      </c>
+      <c r="R430" s="7"/>
       <c r="S430" s="7"/>
-      <c r="T430" s="7" t="s">
-        <v>1850</v>
+      <c r="T430" s="53" t="s">
+        <v>1985</v>
       </c>
       <c r="U430" s="7"/>
       <c r="V430" s="7"/>
       <c r="W430" s="7"/>
-      <c r="X430" s="7" t="s">
-        <v>2105</v>
-      </c>
+      <c r="X430" s="7"/>
       <c r="Y430" s="7" t="s">
-        <v>1927</v>
-      </c>
-      <c r="Z430" s="15"/>
-      <c r="AA430"/>
-      <c r="AB430"/>
-      <c r="AC430"/>
-    </row>
-    <row r="431" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+        <v>1912</v>
+      </c>
+      <c r="Z430" s="15" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="431" spans="1:29" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A431" s="47" t="s">
         <v>2092</v>
       </c>
@@ -37244,36 +37255,37 @@
       </c>
       <c r="H431" s="6"/>
       <c r="I431" s="6"/>
+      <c r="J431" s="53"/>
       <c r="K431" s="53" t="s">
-        <v>2100</v>
+        <v>2101</v>
       </c>
       <c r="L431" s="7"/>
       <c r="M431" s="53" t="s">
-        <v>1855</v>
+        <v>1851</v>
       </c>
       <c r="N431" s="7"/>
-      <c r="O431" s="6">
-        <v>3</v>
-      </c>
+      <c r="O431" s="6"/>
       <c r="P431" s="7" t="s">
         <v>653</v>
       </c>
       <c r="Q431" s="7"/>
       <c r="R431" s="7" t="s">
-        <v>2103</v>
+        <v>2087</v>
       </c>
       <c r="S431" s="7"/>
-      <c r="T431" s="7"/>
+      <c r="T431" s="7" t="s">
+        <v>1850</v>
+      </c>
       <c r="U431" s="7"/>
       <c r="V431" s="7"/>
       <c r="W431" s="7"/>
       <c r="X431" s="7" t="s">
-        <v>2104</v>
-      </c>
-      <c r="Y431" s="7"/>
-      <c r="Z431" s="15" t="s">
-        <v>2106</v>
-      </c>
+        <v>2105</v>
+      </c>
+      <c r="Y431" s="7" t="s">
+        <v>1927</v>
+      </c>
+      <c r="Z431" s="15"/>
       <c r="AA431"/>
       <c r="AB431"/>
       <c r="AC431"/>
@@ -37306,7 +37318,7 @@
         <v>3</v>
       </c>
       <c r="P432" s="7" t="s">
-        <v>2102</v>
+        <v>653</v>
       </c>
       <c r="Q432" s="7"/>
       <c r="R432" s="7" t="s">
@@ -37322,63 +37334,65 @@
       </c>
       <c r="Y432" s="7"/>
       <c r="Z432" s="15" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="AA432"/>
       <c r="AB432"/>
       <c r="AC432"/>
     </row>
-    <row r="433" spans="1:29" ht="51" x14ac:dyDescent="0.2">
-      <c r="A433" s="26" t="s">
-        <v>1410</v>
+    <row r="433" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+      <c r="A433" s="47" t="s">
+        <v>2092</v>
       </c>
       <c r="B433" s="7"/>
       <c r="C433" s="7"/>
       <c r="D433" s="7"/>
       <c r="E433" s="7"/>
       <c r="F433" s="7" t="s">
-        <v>1456</v>
-      </c>
-      <c r="G433" s="7"/>
+        <v>591</v>
+      </c>
+      <c r="G433" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="H433" s="6"/>
       <c r="I433" s="6"/>
-      <c r="J433" s="7"/>
-      <c r="K433" s="6" t="s">
-        <v>1409</v>
+      <c r="K433" s="53" t="s">
+        <v>2100</v>
       </c>
       <c r="L433" s="7"/>
-      <c r="M433" s="7" t="s">
-        <v>1457</v>
-      </c>
-      <c r="N433" s="7" t="s">
-        <v>1411</v>
-      </c>
-      <c r="O433" s="7">
-        <v>4</v>
+      <c r="M433" s="53" t="s">
+        <v>1855</v>
+      </c>
+      <c r="N433" s="7"/>
+      <c r="O433" s="6">
+        <v>3</v>
       </c>
       <c r="P433" s="7" t="s">
-        <v>1314</v>
-      </c>
-      <c r="Q433" s="7" t="s">
-        <v>1459</v>
-      </c>
-      <c r="R433" s="7"/>
-      <c r="S433" s="6" t="s">
-        <v>1326</v>
-      </c>
+        <v>2102</v>
+      </c>
+      <c r="Q433" s="7"/>
+      <c r="R433" s="7" t="s">
+        <v>2103</v>
+      </c>
+      <c r="S433" s="7"/>
       <c r="T433" s="7"/>
       <c r="U433" s="7"/>
       <c r="V433" s="7"/>
       <c r="W433" s="7"/>
-      <c r="X433" s="7"/>
+      <c r="X433" s="7" t="s">
+        <v>2104</v>
+      </c>
       <c r="Y433" s="7"/>
       <c r="Z433" s="15" t="s">
-        <v>1325</v>
-      </c>
-    </row>
-    <row r="434" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+        <v>2107</v>
+      </c>
+      <c r="AA433"/>
+      <c r="AB433"/>
+      <c r="AC433"/>
+    </row>
+    <row r="434" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A434" s="26" t="s">
-        <v>1398</v>
+        <v>1410</v>
       </c>
       <c r="B434" s="7"/>
       <c r="C434" s="7"/>
@@ -37396,19 +37410,19 @@
       </c>
       <c r="L434" s="7"/>
       <c r="M434" s="7" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="N434" s="7" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="O434" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P434" s="7" t="s">
-        <v>1396</v>
+        <v>1314</v>
       </c>
       <c r="Q434" s="7" t="s">
-        <v>1397</v>
+        <v>1459</v>
       </c>
       <c r="R434" s="7"/>
       <c r="S434" s="6" t="s">
@@ -37424,128 +37438,128 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="435" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
-      <c r="A435" s="41" t="s">
+    <row r="435" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+      <c r="A435" s="26" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B435" s="7"/>
+      <c r="C435" s="7"/>
+      <c r="D435" s="7"/>
+      <c r="E435" s="7"/>
+      <c r="F435" s="7" t="s">
+        <v>1456</v>
+      </c>
+      <c r="G435" s="7"/>
+      <c r="H435" s="6"/>
+      <c r="I435" s="6"/>
+      <c r="J435" s="7"/>
+      <c r="K435" s="6" t="s">
+        <v>1409</v>
+      </c>
+      <c r="L435" s="7"/>
+      <c r="M435" s="7" t="s">
+        <v>1458</v>
+      </c>
+      <c r="N435" s="7" t="s">
+        <v>1412</v>
+      </c>
+      <c r="O435" s="7">
+        <v>2</v>
+      </c>
+      <c r="P435" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="Q435" s="7" t="s">
+        <v>1397</v>
+      </c>
+      <c r="R435" s="7"/>
+      <c r="S435" s="6" t="s">
+        <v>1326</v>
+      </c>
+      <c r="T435" s="7"/>
+      <c r="U435" s="7"/>
+      <c r="V435" s="7"/>
+      <c r="W435" s="7"/>
+      <c r="X435" s="7"/>
+      <c r="Y435" s="7"/>
+      <c r="Z435" s="15" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="436" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
+      <c r="A436" s="41" t="s">
         <v>1395</v>
       </c>
-      <c r="B435" s="41"/>
-      <c r="C435" s="41"/>
-      <c r="D435" s="41"/>
-      <c r="E435" s="41"/>
-      <c r="F435" s="41" t="s">
+      <c r="B436" s="41"/>
+      <c r="C436" s="41"/>
+      <c r="D436" s="41"/>
+      <c r="E436" s="41"/>
+      <c r="F436" s="41" t="s">
         <v>1332</v>
       </c>
-      <c r="G435" s="7" t="s">
+      <c r="G436" s="7" t="s">
         <v>1629</v>
       </c>
-      <c r="H435" s="41"/>
-      <c r="I435" s="41"/>
-      <c r="J435" s="41" t="s">
+      <c r="H436" s="41"/>
+      <c r="I436" s="41"/>
+      <c r="J436" s="41" t="s">
         <v>1394</v>
       </c>
-      <c r="K435" s="41" t="s">
+      <c r="K436" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="L435" s="41"/>
-      <c r="M435" s="41" t="s">
+      <c r="L436" s="41"/>
+      <c r="M436" s="41" t="s">
         <v>1595</v>
       </c>
-      <c r="N435" s="41"/>
-      <c r="O435" s="7">
+      <c r="N436" s="41"/>
+      <c r="O436" s="7">
         <v>3</v>
       </c>
-      <c r="P435" s="41"/>
-      <c r="Q435" s="41"/>
-      <c r="R435" s="41"/>
-      <c r="S435" s="41"/>
-      <c r="T435" s="59" t="s">
+      <c r="P436" s="41"/>
+      <c r="Q436" s="41"/>
+      <c r="R436" s="41"/>
+      <c r="S436" s="41"/>
+      <c r="T436" s="59" t="s">
         <v>2063</v>
       </c>
-      <c r="U435" s="41"/>
-      <c r="V435" s="41"/>
-      <c r="W435" s="41"/>
-      <c r="X435" s="41"/>
-      <c r="Y435" s="41"/>
-      <c r="Z435" s="43" t="s">
+      <c r="U436" s="41"/>
+      <c r="V436" s="41"/>
+      <c r="W436" s="41"/>
+      <c r="X436" s="41"/>
+      <c r="Y436" s="41"/>
+      <c r="Z436" s="43" t="s">
         <v>1386</v>
       </c>
     </row>
-    <row r="436" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
-      <c r="A436" s="26" t="s">
+    <row r="437" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
+      <c r="A437" s="26" t="s">
         <v>1327</v>
-      </c>
-      <c r="B436" s="7"/>
-      <c r="C436" s="7"/>
-      <c r="D436" s="7"/>
-      <c r="E436" s="7"/>
-      <c r="F436" s="7" t="s">
-        <v>1333</v>
-      </c>
-      <c r="G436" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H436" s="6"/>
-      <c r="I436" s="6"/>
-      <c r="J436" s="7" t="s">
-        <v>1426</v>
-      </c>
-      <c r="K436" s="7" t="s">
-        <v>1567</v>
-      </c>
-      <c r="L436" s="7"/>
-      <c r="M436" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="N436" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="O436" s="6">
-        <v>9</v>
-      </c>
-      <c r="P436" s="7"/>
-      <c r="Q436" s="7"/>
-      <c r="R436" s="7"/>
-      <c r="S436" s="7"/>
-      <c r="T436" s="53" t="s">
-        <v>2064</v>
-      </c>
-      <c r="U436" s="7"/>
-      <c r="V436" s="7"/>
-      <c r="W436" s="7"/>
-      <c r="X436" s="7"/>
-      <c r="Y436" s="7"/>
-      <c r="Z436" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="437" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
-      <c r="A437" s="47" t="s">
-        <v>68</v>
       </c>
       <c r="B437" s="7"/>
       <c r="C437" s="7"/>
       <c r="D437" s="7"/>
       <c r="E437" s="7"/>
       <c r="F437" s="7" t="s">
-        <v>591</v>
+        <v>1333</v>
       </c>
       <c r="G437" s="7" t="s">
-        <v>989</v>
+        <v>29</v>
       </c>
       <c r="H437" s="6"/>
       <c r="I437" s="6"/>
       <c r="J437" s="7" t="s">
-        <v>1394</v>
+        <v>1426</v>
       </c>
       <c r="K437" s="7" t="s">
-        <v>1933</v>
+        <v>1567</v>
       </c>
       <c r="L437" s="7"/>
       <c r="M437" s="7" t="s">
-        <v>167</v>
+        <v>66</v>
       </c>
       <c r="N437" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O437" s="6">
         <v>9</v>
@@ -37563,15 +37577,12 @@
       <c r="X437" s="7"/>
       <c r="Y437" s="7"/>
       <c r="Z437" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="AA437"/>
-      <c r="AB437"/>
-      <c r="AC437"/>
-    </row>
-    <row r="438" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="438" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
       <c r="A438" s="47" t="s">
-        <v>1759</v>
+        <v>68</v>
       </c>
       <c r="B438" s="7"/>
       <c r="C438" s="7"/>
@@ -37585,32 +37596,44 @@
       </c>
       <c r="H438" s="6"/>
       <c r="I438" s="6"/>
-      <c r="J438" s="7"/>
-      <c r="K438" s="7"/>
+      <c r="J438" s="7" t="s">
+        <v>1394</v>
+      </c>
+      <c r="K438" s="7" t="s">
+        <v>1933</v>
+      </c>
       <c r="L438" s="7"/>
-      <c r="M438" s="7"/>
-      <c r="N438" s="7"/>
-      <c r="O438" s="6"/>
+      <c r="M438" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="N438" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O438" s="6">
+        <v>9</v>
+      </c>
       <c r="P438" s="7"/>
       <c r="Q438" s="7"/>
       <c r="R438" s="7"/>
       <c r="S438" s="7"/>
-      <c r="T438" s="7"/>
+      <c r="T438" s="53" t="s">
+        <v>2064</v>
+      </c>
       <c r="U438" s="7"/>
       <c r="V438" s="7"/>
       <c r="W438" s="7"/>
       <c r="X438" s="7"/>
       <c r="Y438" s="7"/>
       <c r="Z438" s="15" t="s">
-        <v>1760</v>
+        <v>206</v>
       </c>
       <c r="AA438"/>
       <c r="AB438"/>
       <c r="AC438"/>
     </row>
-    <row r="439" spans="1:29" s="42" customFormat="1" ht="170" x14ac:dyDescent="0.15">
+    <row r="439" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A439" s="47" t="s">
-        <v>1906</v>
+        <v>1759</v>
       </c>
       <c r="B439" s="7"/>
       <c r="C439" s="7"/>
@@ -37620,52 +37643,36 @@
         <v>591</v>
       </c>
       <c r="G439" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H439" s="7" t="s">
-        <v>1818</v>
-      </c>
-      <c r="I439" s="7" t="s">
-        <v>1817</v>
-      </c>
-      <c r="J439" s="7" t="s">
-        <v>1816</v>
-      </c>
-      <c r="K439" s="7" t="s">
-        <v>1934</v>
-      </c>
+        <v>989</v>
+      </c>
+      <c r="H439" s="6"/>
+      <c r="I439" s="6"/>
+      <c r="J439" s="7"/>
+      <c r="K439" s="7"/>
       <c r="L439" s="7"/>
-      <c r="M439" s="7" t="s">
-        <v>1907</v>
-      </c>
+      <c r="M439" s="7"/>
       <c r="N439" s="7"/>
-      <c r="O439" s="6" t="s">
-        <v>1908</v>
-      </c>
-      <c r="P439" s="7" t="s">
-        <v>779</v>
-      </c>
-      <c r="Q439" s="7" t="s">
-        <v>1909</v>
-      </c>
+      <c r="O439" s="6"/>
+      <c r="P439" s="7"/>
+      <c r="Q439" s="7"/>
       <c r="R439" s="7"/>
       <c r="S439" s="7"/>
-      <c r="T439" s="7" t="s">
-        <v>1961</v>
-      </c>
+      <c r="T439" s="7"/>
       <c r="U439" s="7"/>
       <c r="V439" s="7"/>
       <c r="W439" s="7"/>
       <c r="X439" s="7"/>
       <c r="Y439" s="7"/>
-      <c r="Z439" s="15"/>
+      <c r="Z439" s="15" t="s">
+        <v>1760</v>
+      </c>
       <c r="AA439"/>
       <c r="AB439"/>
       <c r="AC439"/>
     </row>
-    <row r="440" spans="1:29" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="440" spans="1:29" s="42" customFormat="1" ht="170" x14ac:dyDescent="0.15">
       <c r="A440" s="47" t="s">
-        <v>1853</v>
+        <v>1906</v>
       </c>
       <c r="B440" s="7"/>
       <c r="C440" s="7"/>
@@ -37674,43 +37681,53 @@
       <c r="F440" s="7" t="s">
         <v>591</v>
       </c>
-      <c r="G440" s="7"/>
-      <c r="H440" s="6"/>
-      <c r="I440" s="6"/>
-      <c r="J440" s="7"/>
-      <c r="K440" s="53" t="s">
-        <v>1935</v>
+      <c r="G440" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H440" s="7" t="s">
+        <v>1818</v>
+      </c>
+      <c r="I440" s="7" t="s">
+        <v>1817</v>
+      </c>
+      <c r="J440" s="7" t="s">
+        <v>1816</v>
+      </c>
+      <c r="K440" s="7" t="s">
+        <v>1934</v>
       </c>
       <c r="L440" s="7"/>
-      <c r="M440" s="53" t="s">
-        <v>1855</v>
+      <c r="M440" s="7" t="s">
+        <v>1907</v>
       </c>
       <c r="N440" s="7"/>
-      <c r="O440" s="6">
-        <v>1</v>
-      </c>
-      <c r="P440" s="7"/>
-      <c r="Q440" s="7"/>
+      <c r="O440" s="6" t="s">
+        <v>1908</v>
+      </c>
+      <c r="P440" s="7" t="s">
+        <v>779</v>
+      </c>
+      <c r="Q440" s="7" t="s">
+        <v>1909</v>
+      </c>
       <c r="R440" s="7"/>
       <c r="S440" s="7"/>
       <c r="T440" s="7" t="s">
-        <v>1854</v>
+        <v>1961</v>
       </c>
       <c r="U440" s="7"/>
       <c r="V440" s="7"/>
       <c r="W440" s="7"/>
-      <c r="X440" s="7" t="s">
-        <v>1926</v>
-      </c>
+      <c r="X440" s="7"/>
       <c r="Y440" s="7"/>
       <c r="Z440" s="15"/>
       <c r="AA440"/>
       <c r="AB440"/>
       <c r="AC440"/>
     </row>
-    <row r="441" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
+    <row r="441" spans="1:29" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A441" s="47" t="s">
-        <v>1849</v>
+        <v>1853</v>
       </c>
       <c r="B441" s="7"/>
       <c r="C441" s="7"/>
@@ -37719,133 +37736,128 @@
       <c r="F441" s="7" t="s">
         <v>591</v>
       </c>
-      <c r="G441" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H441" s="6" t="s">
-        <v>1845</v>
-      </c>
-      <c r="I441" s="6" t="s">
-        <v>1844</v>
-      </c>
-      <c r="J441" s="53" t="s">
-        <v>1842</v>
-      </c>
-      <c r="K441" s="7" t="s">
-        <v>1843</v>
+      <c r="G441" s="7"/>
+      <c r="H441" s="6"/>
+      <c r="I441" s="6"/>
+      <c r="J441" s="7"/>
+      <c r="K441" s="53" t="s">
+        <v>1935</v>
       </c>
       <c r="L441" s="7"/>
       <c r="M441" s="53" t="s">
-        <v>1846</v>
+        <v>1855</v>
       </c>
       <c r="N441" s="7"/>
       <c r="O441" s="6">
         <v>1</v>
       </c>
       <c r="P441" s="7"/>
-      <c r="Q441" s="7" t="s">
-        <v>1848</v>
-      </c>
+      <c r="Q441" s="7"/>
       <c r="R441" s="7"/>
       <c r="S441" s="7"/>
-      <c r="T441" s="7"/>
+      <c r="T441" s="7" t="s">
+        <v>1854</v>
+      </c>
       <c r="U441" s="7"/>
       <c r="V441" s="7"/>
       <c r="W441" s="7"/>
-      <c r="X441" s="7"/>
+      <c r="X441" s="7" t="s">
+        <v>1926</v>
+      </c>
       <c r="Y441" s="7"/>
-      <c r="Z441" s="15" t="s">
-        <v>1847</v>
-      </c>
+      <c r="Z441" s="15"/>
       <c r="AA441"/>
       <c r="AB441"/>
       <c r="AC441"/>
     </row>
     <row r="442" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
       <c r="A442" s="47" t="s">
-        <v>1515</v>
+        <v>1849</v>
       </c>
       <c r="B442" s="7"/>
       <c r="C442" s="7"/>
       <c r="D442" s="7"/>
       <c r="E442" s="7"/>
       <c r="F442" s="7" t="s">
-        <v>1516</v>
+        <v>591</v>
       </c>
       <c r="G442" s="7" t="s">
-        <v>1517</v>
+        <v>77</v>
       </c>
       <c r="H442" s="6" t="s">
-        <v>1519</v>
-      </c>
-      <c r="I442" s="6"/>
-      <c r="J442" s="6"/>
-      <c r="K442" s="6" t="s">
-        <v>109</v>
+        <v>1845</v>
+      </c>
+      <c r="I442" s="6" t="s">
+        <v>1844</v>
+      </c>
+      <c r="J442" s="53" t="s">
+        <v>1842</v>
+      </c>
+      <c r="K442" s="7" t="s">
+        <v>1843</v>
       </c>
       <c r="L442" s="7"/>
-      <c r="M442" s="6" t="s">
-        <v>1518</v>
+      <c r="M442" s="53" t="s">
+        <v>1846</v>
       </c>
       <c r="N442" s="7"/>
-      <c r="O442" s="7"/>
+      <c r="O442" s="6">
+        <v>1</v>
+      </c>
       <c r="P442" s="7"/>
-      <c r="Q442" s="7"/>
-      <c r="R442" s="6" t="s">
-        <v>1520</v>
-      </c>
-      <c r="S442" s="6"/>
+      <c r="Q442" s="7" t="s">
+        <v>1848</v>
+      </c>
+      <c r="R442" s="7"/>
+      <c r="S442" s="7"/>
       <c r="T442" s="7"/>
       <c r="U442" s="7"/>
       <c r="V442" s="7"/>
       <c r="W442" s="7"/>
       <c r="X442" s="7"/>
       <c r="Y442" s="7"/>
-      <c r="Z442" s="15"/>
-    </row>
-    <row r="443" spans="1:29" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+      <c r="Z442" s="15" t="s">
+        <v>1847</v>
+      </c>
+      <c r="AA442"/>
+      <c r="AB442"/>
+      <c r="AC442"/>
+    </row>
+    <row r="443" spans="1:29" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
       <c r="A443" s="47" t="s">
-        <v>1630</v>
+        <v>1515</v>
       </c>
       <c r="B443" s="7"/>
       <c r="C443" s="7"/>
       <c r="D443" s="7"/>
       <c r="E443" s="7"/>
       <c r="F443" s="7" t="s">
-        <v>1631</v>
+        <v>1516</v>
       </c>
       <c r="G443" s="7" t="s">
-        <v>1601</v>
-      </c>
-      <c r="H443" s="7" t="s">
-        <v>1616</v>
-      </c>
-      <c r="I443" s="7" t="s">
-        <v>1617</v>
-      </c>
-      <c r="J443" s="6" t="s">
-        <v>1632</v>
-      </c>
-      <c r="K443" s="7" t="s">
-        <v>1428</v>
+        <v>1517</v>
+      </c>
+      <c r="H443" s="6" t="s">
+        <v>1519</v>
+      </c>
+      <c r="I443" s="6"/>
+      <c r="J443" s="6"/>
+      <c r="K443" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="L443" s="7"/>
       <c r="M443" s="6" t="s">
-        <v>1565</v>
-      </c>
-      <c r="N443" s="7" t="s">
-        <v>1566</v>
-      </c>
-      <c r="O443" s="6">
-        <v>4</v>
-      </c>
+        <v>1518</v>
+      </c>
+      <c r="N443" s="7"/>
+      <c r="O443" s="7"/>
       <c r="P443" s="7"/>
       <c r="Q443" s="7"/>
-      <c r="R443" s="6"/>
+      <c r="R443" s="6" t="s">
+        <v>1520</v>
+      </c>
       <c r="S443" s="6"/>
-      <c r="T443" s="7" t="s">
-        <v>1862</v>
-      </c>
+      <c r="T443" s="7"/>
       <c r="U443" s="7"/>
       <c r="V443" s="7"/>
       <c r="W443" s="7"/>
@@ -37853,119 +37865,111 @@
       <c r="Y443" s="7"/>
       <c r="Z443" s="15"/>
     </row>
-    <row r="444" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+    <row r="444" spans="1:29" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A444" s="47" t="s">
-        <v>1812</v>
+        <v>1630</v>
       </c>
       <c r="B444" s="7"/>
       <c r="C444" s="7"/>
       <c r="D444" s="7"/>
       <c r="E444" s="7"/>
       <c r="F444" s="7" t="s">
-        <v>591</v>
+        <v>1631</v>
       </c>
       <c r="G444" s="7" t="s">
-        <v>1805</v>
+        <v>1601</v>
       </c>
       <c r="H444" s="7" t="s">
-        <v>1885</v>
+        <v>1616</v>
       </c>
       <c r="I444" s="7" t="s">
-        <v>1678</v>
-      </c>
-      <c r="J444" s="7" t="s">
-        <v>1679</v>
+        <v>1617</v>
+      </c>
+      <c r="J444" s="6" t="s">
+        <v>1632</v>
       </c>
       <c r="K444" s="7" t="s">
-        <v>1886</v>
+        <v>1428</v>
       </c>
       <c r="L444" s="7"/>
-      <c r="M444" s="7" t="s">
-        <v>1887</v>
-      </c>
-      <c r="N444" s="53"/>
-      <c r="O444" s="7">
+      <c r="M444" s="6" t="s">
+        <v>1565</v>
+      </c>
+      <c r="N444" s="7" t="s">
+        <v>1566</v>
+      </c>
+      <c r="O444" s="6">
         <v>4</v>
       </c>
-      <c r="P444" s="7" t="s">
-        <v>653</v>
-      </c>
-      <c r="Q444" s="7" t="s">
-        <v>1888</v>
-      </c>
-      <c r="R444" s="53">
-        <v>1265</v>
-      </c>
-      <c r="S444" s="7"/>
+      <c r="P444" s="7"/>
+      <c r="Q444" s="7"/>
+      <c r="R444" s="6"/>
+      <c r="S444" s="6"/>
       <c r="T444" s="7" t="s">
-        <v>1978</v>
+        <v>1862</v>
       </c>
       <c r="U444" s="7"/>
       <c r="V444" s="7"/>
       <c r="W444" s="7"/>
       <c r="X444" s="7"/>
       <c r="Y444" s="7"/>
-      <c r="Z444" s="15" t="s">
+      <c r="Z444" s="15"/>
+    </row>
+    <row r="445" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+      <c r="A445" s="47" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B445" s="7"/>
+      <c r="C445" s="7"/>
+      <c r="D445" s="7"/>
+      <c r="E445" s="7"/>
+      <c r="F445" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="G445" s="7" t="s">
+        <v>1805</v>
+      </c>
+      <c r="H445" s="7" t="s">
+        <v>1885</v>
+      </c>
+      <c r="I445" s="7" t="s">
+        <v>1678</v>
+      </c>
+      <c r="J445" s="7" t="s">
+        <v>1679</v>
+      </c>
+      <c r="K445" s="7" t="s">
+        <v>1886</v>
+      </c>
+      <c r="L445" s="7"/>
+      <c r="M445" s="7" t="s">
+        <v>1887</v>
+      </c>
+      <c r="N445" s="53"/>
+      <c r="O445" s="7">
+        <v>4</v>
+      </c>
+      <c r="P445" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q445" s="7" t="s">
+        <v>1888</v>
+      </c>
+      <c r="R445" s="53">
+        <v>1265</v>
+      </c>
+      <c r="S445" s="7"/>
+      <c r="T445" s="7" t="s">
+        <v>1978</v>
+      </c>
+      <c r="U445" s="7"/>
+      <c r="V445" s="7"/>
+      <c r="W445" s="7"/>
+      <c r="X445" s="7"/>
+      <c r="Y445" s="7"/>
+      <c r="Z445" s="15" t="s">
         <v>1680</v>
       </c>
-    </row>
-    <row r="446" spans="1:29" s="42" customFormat="1" ht="136" x14ac:dyDescent="0.15">
-      <c r="A446" s="47" t="s">
-        <v>1871</v>
-      </c>
-      <c r="B446" s="7"/>
-      <c r="C446" s="7"/>
-      <c r="D446" s="7"/>
-      <c r="E446" s="7"/>
-      <c r="F446" s="7" t="s">
-        <v>591</v>
-      </c>
-      <c r="G446" s="7" t="s">
-        <v>1805</v>
-      </c>
-      <c r="H446" s="7" t="s">
-        <v>1807</v>
-      </c>
-      <c r="I446" s="7" t="s">
-        <v>1806</v>
-      </c>
-      <c r="J446" s="7" t="s">
-        <v>1876</v>
-      </c>
-      <c r="K446" s="7" t="s">
-        <v>1979</v>
-      </c>
-      <c r="L446" s="7"/>
-      <c r="M446" s="6" t="s">
-        <v>1877</v>
-      </c>
-      <c r="N446" s="53" t="s">
-        <v>443</v>
-      </c>
-      <c r="O446" s="53">
-        <v>13</v>
-      </c>
-      <c r="P446" s="7" t="s">
-        <v>779</v>
-      </c>
-      <c r="Q446" s="7" t="s">
-        <v>1878</v>
-      </c>
-      <c r="R446" s="7"/>
-      <c r="S446" s="53" t="s">
-        <v>1879</v>
-      </c>
-      <c r="T446" s="7" t="s">
-        <v>1983</v>
-      </c>
-      <c r="U446" s="7"/>
-      <c r="V446" s="7"/>
-      <c r="W446" s="7"/>
-      <c r="X446" s="7"/>
-      <c r="Y446" s="53" t="s">
-        <v>1883</v>
-      </c>
-      <c r="Z446" s="15"/>
     </row>
     <row r="447" spans="1:29" s="42" customFormat="1" ht="136" x14ac:dyDescent="0.15">
       <c r="A447" s="47" t="s">
@@ -37998,13 +38002,13 @@
         <v>1877</v>
       </c>
       <c r="N447" s="53" t="s">
-        <v>1250</v>
-      </c>
-      <c r="O447" s="53" t="s">
-        <v>680</v>
-      </c>
-      <c r="P447" s="53" t="s">
-        <v>680</v>
+        <v>443</v>
+      </c>
+      <c r="O447" s="53">
+        <v>13</v>
+      </c>
+      <c r="P447" s="7" t="s">
+        <v>779</v>
       </c>
       <c r="Q447" s="7" t="s">
         <v>1878</v>
@@ -38013,7 +38017,9 @@
       <c r="S447" s="53" t="s">
         <v>1879</v>
       </c>
-      <c r="T447" s="7"/>
+      <c r="T447" s="7" t="s">
+        <v>1983</v>
+      </c>
       <c r="U447" s="7"/>
       <c r="V447" s="7"/>
       <c r="W447" s="7"/>
@@ -38054,10 +38060,10 @@
         <v>1877</v>
       </c>
       <c r="N448" s="53" t="s">
-        <v>444</v>
+        <v>1250</v>
       </c>
       <c r="O448" s="53" t="s">
-        <v>1981</v>
+        <v>680</v>
       </c>
       <c r="P448" s="53" t="s">
         <v>680</v>
@@ -38069,9 +38075,7 @@
       <c r="S448" s="53" t="s">
         <v>1879</v>
       </c>
-      <c r="T448" s="7" t="s">
-        <v>1980</v>
-      </c>
+      <c r="T448" s="7"/>
       <c r="U448" s="7"/>
       <c r="V448" s="7"/>
       <c r="W448" s="7"/>
@@ -38112,10 +38116,10 @@
         <v>1877</v>
       </c>
       <c r="N449" s="53" t="s">
-        <v>577</v>
+        <v>444</v>
       </c>
       <c r="O449" s="53" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="P449" s="53" t="s">
         <v>680</v>
@@ -38128,7 +38132,7 @@
         <v>1879</v>
       </c>
       <c r="T449" s="7" t="s">
-        <v>1984</v>
+        <v>1980</v>
       </c>
       <c r="U449" s="7"/>
       <c r="V449" s="7"/>
@@ -38139,71 +38143,89 @@
       </c>
       <c r="Z449" s="15"/>
     </row>
-    <row r="450" spans="1:26" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
-      <c r="A450" s="26" t="s">
-        <v>302</v>
+    <row r="450" spans="1:26" s="42" customFormat="1" ht="136" x14ac:dyDescent="0.15">
+      <c r="A450" s="47" t="s">
+        <v>1871</v>
       </c>
       <c r="B450" s="7"/>
       <c r="C450" s="7"/>
       <c r="D450" s="7"/>
       <c r="E450" s="7"/>
-      <c r="F450" s="6"/>
-      <c r="G450" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H450" s="6" t="s">
-        <v>2069</v>
-      </c>
-      <c r="I450" s="6" t="s">
-        <v>2070</v>
-      </c>
-      <c r="J450" s="6" t="s">
-        <v>2071</v>
-      </c>
-      <c r="K450" s="6"/>
+      <c r="F450" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="G450" s="7" t="s">
+        <v>1805</v>
+      </c>
+      <c r="H450" s="7" t="s">
+        <v>1807</v>
+      </c>
+      <c r="I450" s="7" t="s">
+        <v>1806</v>
+      </c>
+      <c r="J450" s="7" t="s">
+        <v>1876</v>
+      </c>
+      <c r="K450" s="7" t="s">
+        <v>1979</v>
+      </c>
       <c r="L450" s="7"/>
       <c r="M450" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="N450" s="7"/>
-      <c r="O450" s="7"/>
-      <c r="P450" s="7"/>
-      <c r="Q450" s="7"/>
+        <v>1877</v>
+      </c>
+      <c r="N450" s="53" t="s">
+        <v>577</v>
+      </c>
+      <c r="O450" s="53" t="s">
+        <v>1982</v>
+      </c>
+      <c r="P450" s="53" t="s">
+        <v>680</v>
+      </c>
+      <c r="Q450" s="7" t="s">
+        <v>1878</v>
+      </c>
       <c r="R450" s="7"/>
-      <c r="S450" s="7"/>
-      <c r="T450" s="7"/>
+      <c r="S450" s="53" t="s">
+        <v>1879</v>
+      </c>
+      <c r="T450" s="7" t="s">
+        <v>1984</v>
+      </c>
       <c r="U450" s="7"/>
       <c r="V450" s="7"/>
       <c r="W450" s="7"/>
       <c r="X450" s="7"/>
-      <c r="Y450" s="7"/>
-      <c r="Z450" s="15" t="s">
-        <v>2072</v>
-      </c>
-    </row>
-    <row r="451" spans="1:26" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
-      <c r="A451" s="47"/>
+      <c r="Y450" s="53" t="s">
+        <v>1883</v>
+      </c>
+      <c r="Z450" s="15"/>
+    </row>
+    <row r="451" spans="1:26" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
+      <c r="A451" s="26" t="s">
+        <v>302</v>
+      </c>
       <c r="B451" s="7"/>
       <c r="C451" s="7"/>
       <c r="D451" s="7"/>
       <c r="E451" s="7"/>
-      <c r="F451" s="6" t="s">
-        <v>591</v>
-      </c>
+      <c r="F451" s="6"/>
       <c r="G451" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="H451" s="6"/>
-      <c r="I451" s="6"/>
+        <v>45</v>
+      </c>
+      <c r="H451" s="6" t="s">
+        <v>2069</v>
+      </c>
+      <c r="I451" s="6" t="s">
+        <v>2070</v>
+      </c>
       <c r="J451" s="6" t="s">
-        <v>1939</v>
-      </c>
-      <c r="K451" s="6" t="s">
-        <v>1940</v>
-      </c>
+        <v>2071</v>
+      </c>
+      <c r="K451" s="6"/>
       <c r="L451" s="7"/>
       <c r="M451" s="6" t="s">
-        <v>1941</v>
+        <v>110</v>
       </c>
       <c r="N451" s="7"/>
       <c r="O451" s="7"/>
@@ -38216,50 +38238,54 @@
       <c r="V451" s="7"/>
       <c r="W451" s="7"/>
       <c r="X451" s="7"/>
-      <c r="Y451" s="7" t="s">
-        <v>1942</v>
-      </c>
-      <c r="Z451" s="15"/>
-    </row>
-    <row r="452" spans="1:26" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
-      <c r="A452" s="47" t="s">
-        <v>1652</v>
-      </c>
+      <c r="Y451" s="7"/>
+      <c r="Z451" s="15" t="s">
+        <v>2072</v>
+      </c>
+    </row>
+    <row r="452" spans="1:26" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+      <c r="A452" s="47"/>
       <c r="B452" s="7"/>
       <c r="C452" s="7"/>
       <c r="D452" s="7"/>
       <c r="E452" s="7"/>
-      <c r="F452" s="7"/>
-      <c r="G452" s="7"/>
+      <c r="F452" s="6" t="s">
+        <v>591</v>
+      </c>
+      <c r="G452" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="H452" s="6"/>
       <c r="I452" s="6"/>
-      <c r="J452" s="6"/>
-      <c r="K452" s="53" t="s">
-        <v>1761</v>
+      <c r="J452" s="6" t="s">
+        <v>1939</v>
+      </c>
+      <c r="K452" s="6" t="s">
+        <v>1940</v>
       </c>
       <c r="L452" s="7"/>
       <c r="M452" s="6" t="s">
-        <v>1654</v>
+        <v>1941</v>
       </c>
       <c r="N452" s="7"/>
-      <c r="O452" s="6"/>
+      <c r="O452" s="7"/>
       <c r="P452" s="7"/>
       <c r="Q452" s="7"/>
-      <c r="R452" s="6"/>
-      <c r="S452" s="6"/>
+      <c r="R452" s="7"/>
+      <c r="S452" s="7"/>
       <c r="T452" s="7"/>
       <c r="U452" s="7"/>
       <c r="V452" s="7"/>
       <c r="W452" s="7"/>
       <c r="X452" s="7"/>
-      <c r="Y452" s="7"/>
-      <c r="Z452" s="15" t="s">
-        <v>1656</v>
-      </c>
+      <c r="Y452" s="7" t="s">
+        <v>1942</v>
+      </c>
+      <c r="Z452" s="15"/>
     </row>
     <row r="453" spans="1:26" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A453" s="47" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="B453" s="7"/>
       <c r="C453" s="7"/>
@@ -38270,12 +38296,12 @@
       <c r="H453" s="6"/>
       <c r="I453" s="6"/>
       <c r="J453" s="6"/>
-      <c r="K453" s="7" t="s">
-        <v>1762</v>
+      <c r="K453" s="53" t="s">
+        <v>1761</v>
       </c>
       <c r="L453" s="7"/>
       <c r="M453" s="6" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="N453" s="7"/>
       <c r="O453" s="6"/>
@@ -38290,110 +38316,146 @@
       <c r="X453" s="7"/>
       <c r="Y453" s="7"/>
       <c r="Z453" s="15" t="s">
-        <v>1657</v>
-      </c>
-    </row>
-    <row r="454" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="454" spans="1:26" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A454" s="47" t="s">
-        <v>1658</v>
+        <v>1653</v>
       </c>
       <c r="B454" s="7"/>
       <c r="C454" s="7"/>
       <c r="D454" s="7"/>
       <c r="E454" s="7"/>
-      <c r="F454" s="6" t="s">
-        <v>1188</v>
-      </c>
-      <c r="G454" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="H454" s="10"/>
-      <c r="I454" s="10"/>
-      <c r="J454" s="6" t="s">
-        <v>1758</v>
-      </c>
+      <c r="F454" s="7"/>
+      <c r="G454" s="7"/>
+      <c r="H454" s="6"/>
+      <c r="I454" s="6"/>
+      <c r="J454" s="6"/>
       <c r="K454" s="7" t="s">
-        <v>896</v>
-      </c>
-      <c r="L454" s="6"/>
+        <v>1762</v>
+      </c>
+      <c r="L454" s="7"/>
       <c r="M454" s="6" t="s">
-        <v>1189</v>
+        <v>1655</v>
       </c>
       <c r="N454" s="7"/>
-      <c r="O454" s="7"/>
-      <c r="P454" s="7" t="s">
-        <v>676</v>
-      </c>
+      <c r="O454" s="6"/>
+      <c r="P454" s="7"/>
       <c r="Q454" s="7"/>
-      <c r="R454" s="7"/>
-      <c r="S454" s="7"/>
+      <c r="R454" s="6"/>
+      <c r="S454" s="6"/>
       <c r="T454" s="7"/>
       <c r="U454" s="7"/>
       <c r="V454" s="7"/>
       <c r="W454" s="7"/>
-      <c r="X454" s="7" t="s">
-        <v>796</v>
-      </c>
+      <c r="X454" s="7"/>
       <c r="Y454" s="7"/>
-      <c r="Z454" s="14" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="455" spans="1:26" s="42" customFormat="1" ht="289" x14ac:dyDescent="0.15">
-      <c r="A455" s="26" t="s">
-        <v>2073</v>
+      <c r="Z454" s="15" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="455" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+      <c r="A455" s="47" t="s">
+        <v>1658</v>
       </c>
       <c r="B455" s="7"/>
       <c r="C455" s="7"/>
       <c r="D455" s="7"/>
       <c r="E455" s="7"/>
       <c r="F455" s="6" t="s">
-        <v>591</v>
+        <v>1188</v>
       </c>
       <c r="G455" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H455" s="6" t="s">
-        <v>2074</v>
-      </c>
-      <c r="I455" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="H455" s="10"/>
+      <c r="I455" s="10"/>
       <c r="J455" s="6" t="s">
-        <v>2075</v>
-      </c>
-      <c r="K455" s="6" t="s">
-        <v>815</v>
-      </c>
-      <c r="L455" s="7"/>
-      <c r="M455" s="7" t="s">
-        <v>2076</v>
+        <v>1758</v>
+      </c>
+      <c r="K455" s="7" t="s">
+        <v>896</v>
+      </c>
+      <c r="L455" s="6"/>
+      <c r="M455" s="6" t="s">
+        <v>1189</v>
       </c>
       <c r="N455" s="7"/>
-      <c r="O455" s="60" t="s">
-        <v>2077</v>
-      </c>
-      <c r="P455" s="53" t="s">
-        <v>2079</v>
+      <c r="O455" s="7"/>
+      <c r="P455" s="7" t="s">
+        <v>676</v>
       </c>
       <c r="Q455" s="7"/>
       <c r="R455" s="7"/>
-      <c r="S455" s="53" t="s">
-        <v>2078</v>
-      </c>
+      <c r="S455" s="7"/>
       <c r="T455" s="7"/>
       <c r="U455" s="7"/>
       <c r="V455" s="7"/>
       <c r="W455" s="7"/>
-      <c r="X455" s="7"/>
+      <c r="X455" s="7" t="s">
+        <v>796</v>
+      </c>
       <c r="Y455" s="7"/>
-      <c r="Z455" s="15" t="s">
+      <c r="Z455" s="14" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="456" spans="1:26" s="42" customFormat="1" ht="289" x14ac:dyDescent="0.15">
+      <c r="A456" s="26" t="s">
+        <v>2073</v>
+      </c>
+      <c r="B456" s="7"/>
+      <c r="C456" s="7"/>
+      <c r="D456" s="7"/>
+      <c r="E456" s="7"/>
+      <c r="F456" s="6" t="s">
+        <v>591</v>
+      </c>
+      <c r="G456" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H456" s="6" t="s">
+        <v>2074</v>
+      </c>
+      <c r="I456" s="6"/>
+      <c r="J456" s="6" t="s">
+        <v>2075</v>
+      </c>
+      <c r="K456" s="6" t="s">
+        <v>815</v>
+      </c>
+      <c r="L456" s="7"/>
+      <c r="M456" s="7" t="s">
+        <v>2076</v>
+      </c>
+      <c r="N456" s="7"/>
+      <c r="O456" s="60" t="s">
+        <v>2077</v>
+      </c>
+      <c r="P456" s="53" t="s">
+        <v>2079</v>
+      </c>
+      <c r="Q456" s="7"/>
+      <c r="R456" s="7"/>
+      <c r="S456" s="53" t="s">
+        <v>2078</v>
+      </c>
+      <c r="T456" s="7"/>
+      <c r="U456" s="7"/>
+      <c r="V456" s="7"/>
+      <c r="W456" s="7"/>
+      <c r="X456" s="7"/>
+      <c r="Y456" s="7"/>
+      <c r="Z456" s="15" t="s">
         <v>2080</v>
       </c>
     </row>
-    <row r="456" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="Z456" s="8"/>
+    <row r="457" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z457" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z454" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Z455" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA417">
     <sortCondition ref="A3:A417"/>
   </sortState>

</xml_diff>

<commit_message>
modif of inventaire xlsx
</commit_message>
<xml_diff>
--- a/metadata/InventaireCampa.xlsx
+++ b/metadata/InventaireCampa.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <fileSharing readOnlyRecommended="1" userName="Microsoft Office User" algorithmName="SHA-512" hashValue="UnG+o7R59VgX65WVs+ji3HTvfzo0sunkoL8BqnVOB2lIbjYUNILgvx4poeuKhCh+2BB7Bd2bAPc/AnOX0WZOdA==" saltValue="Ncv7cTDbBFcSFZismwlwuA==" spinCount="100000"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arlogriffiths/Documents/GitHub/DHARMA/tfc-campa-epigraphy/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salomepichon/Documents/GitHub/DHARMA/tfc-campa-epigraphy/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{C02D774A-2948-864D-B896-5932827F3DA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{7F4E6AB3-0A04-D643-BCC2-98ECABEC81F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="33520" windowHeight="15380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2060" windowWidth="28800" windowHeight="15380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -12255,10 +12255,10 @@
     <t>n. 1953</t>
   </si>
   <si>
-    <t>*253</t>
-  </si>
-  <si>
-    <t>*254</t>
+    <t>*260</t>
+  </si>
+  <si>
+    <t>*267</t>
   </si>
 </sst>
 </file>
@@ -13217,9 +13217,9 @@
   <dimension ref="A1:AC459"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1300" topLeftCell="A430" activePane="bottomLeft"/>
+      <pane ySplit="1300" topLeftCell="A428" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="D432" sqref="D432"/>
+      <selection pane="bottomLeft" activeCell="D431" sqref="D431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
few modif on the inventory
</commit_message>
<xml_diff>
--- a/metadata/InventaireCampa.xlsx
+++ b/metadata/InventaireCampa.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salomepichon/Documents/GitHub/DHARMA/tfc-campa-epigraphy/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{7F4E6AB3-0A04-D643-BCC2-98ECABEC81F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{9C65CD48-B6D3-654A-92ED-A0425CA1AC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2060" windowWidth="28800" windowHeight="15380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2040" windowWidth="10000" windowHeight="15380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5240" uniqueCount="2124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5240" uniqueCount="2126">
   <si>
     <t>Quảng Nam</t>
     <phoneticPr fontId="1"/>
@@ -12138,9 +12138,6 @@
     <t>BEFEO 106</t>
   </si>
   <si>
-    <t>*KhuongMy</t>
-  </si>
-  <si>
     <t>cuve à ablutions</t>
   </si>
   <si>
@@ -12259,6 +12256,15 @@
   </si>
   <si>
     <t>*267</t>
+  </si>
+  <si>
+    <t>*253</t>
+  </si>
+  <si>
+    <t>*254</t>
+  </si>
+  <si>
+    <t>*255</t>
   </si>
 </sst>
 </file>
@@ -13217,9 +13223,9 @@
   <dimension ref="A1:AC459"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1300" topLeftCell="A428" activePane="bottomLeft"/>
+      <pane ySplit="1300" topLeftCell="A432" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="D431" sqref="D431"/>
+      <selection pane="bottomLeft" activeCell="A436" sqref="A436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14607,7 +14613,7 @@
         <v>255</v>
       </c>
       <c r="U23" s="57" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
@@ -14663,7 +14669,7 @@
         <v>255</v>
       </c>
       <c r="U24" s="57" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="V24" s="10"/>
       <c r="W24" s="10"/>
@@ -14719,7 +14725,7 @@
         <v>255</v>
       </c>
       <c r="U25" s="57" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="V25" s="10"/>
       <c r="W25" s="10"/>
@@ -14775,7 +14781,7 @@
         <v>255</v>
       </c>
       <c r="U26" s="57" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="V26" s="10"/>
       <c r="W26" s="10"/>
@@ -15545,7 +15551,7 @@
         <v>1088</v>
       </c>
       <c r="Y39" s="10" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="Z39" s="15" t="s">
         <v>424</v>
@@ -19380,7 +19386,7 @@
       <c r="W108" s="10"/>
       <c r="X108" s="10"/>
       <c r="Y108" s="57" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="Z108" s="15"/>
     </row>
@@ -19432,7 +19438,7 @@
       <c r="W109" s="10"/>
       <c r="X109" s="10"/>
       <c r="Y109" s="57" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="Z109" s="15"/>
     </row>
@@ -19484,7 +19490,7 @@
       <c r="W110" s="10"/>
       <c r="X110" s="10"/>
       <c r="Y110" s="57" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="Z110" s="15"/>
     </row>
@@ -20103,13 +20109,13 @@
       <c r="V121" s="10"/>
       <c r="W121" s="10"/>
       <c r="X121" s="57" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="Y121" s="10" t="s">
         <v>888</v>
       </c>
       <c r="Z121" s="15" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="122" spans="1:26" ht="170" x14ac:dyDescent="0.2">
@@ -20155,13 +20161,13 @@
       <c r="R122" s="10"/>
       <c r="S122" s="10"/>
       <c r="T122" s="57" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="U122" s="10"/>
       <c r="V122" s="10"/>
       <c r="W122" s="10"/>
       <c r="X122" s="57" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="Y122" s="10" t="s">
         <v>888</v>
@@ -30248,7 +30254,7 @@
         <v>1923</v>
       </c>
       <c r="Y294" s="7" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="Z294" s="15" t="s">
         <v>1913</v>
@@ -34085,7 +34091,7 @@
       </c>
       <c r="H371" s="40"/>
       <c r="I371" s="6" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="J371" s="46" t="s">
         <v>1495</v>
@@ -34116,11 +34122,11 @@
       <c r="T371" s="7"/>
       <c r="U371" s="7"/>
       <c r="V371" s="7" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="W371" s="7"/>
       <c r="X371" s="7" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="Y371" s="7"/>
       <c r="Z371" s="15"/>
@@ -34141,7 +34147,7 @@
       </c>
       <c r="H372" s="6"/>
       <c r="I372" s="6" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="J372" s="7" t="s">
         <v>1495</v>
@@ -34172,11 +34178,11 @@
       <c r="T372" s="7"/>
       <c r="U372" s="7"/>
       <c r="V372" s="7" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="W372" s="7"/>
       <c r="X372" s="7" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="Y372" s="7"/>
       <c r="Z372" s="15"/>
@@ -34197,7 +34203,7 @@
       </c>
       <c r="H373" s="6"/>
       <c r="I373" s="6" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="J373" s="7" t="s">
         <v>1495</v>
@@ -34228,11 +34234,11 @@
       <c r="T373" s="7"/>
       <c r="U373" s="7"/>
       <c r="V373" s="7" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="W373" s="7"/>
       <c r="X373" s="7" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="Y373" s="7"/>
       <c r="Z373" s="15"/>
@@ -34253,7 +34259,7 @@
       </c>
       <c r="H374" s="6"/>
       <c r="I374" s="6" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="J374" s="7" t="s">
         <v>1495</v>
@@ -34284,11 +34290,11 @@
       <c r="T374" s="7"/>
       <c r="U374" s="7"/>
       <c r="V374" s="7" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="W374" s="7"/>
       <c r="X374" s="7" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="Y374" s="7"/>
       <c r="Z374" s="15"/>
@@ -35100,7 +35106,7 @@
       </c>
       <c r="S388" s="6"/>
       <c r="T388" s="57" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="U388" s="6"/>
       <c r="V388" s="6"/>
@@ -36606,7 +36612,7 @@
         <v>2049</v>
       </c>
       <c r="T417" s="57" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="U417" s="7"/>
       <c r="V417" s="7"/>
@@ -36662,7 +36668,7 @@
         <v>2049</v>
       </c>
       <c r="T418" s="57" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="U418" s="7"/>
       <c r="V418" s="7"/>
@@ -37053,7 +37059,7 @@
       </c>
       <c r="L426" s="7"/>
       <c r="M426" s="53" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="N426" s="7"/>
       <c r="O426" s="6">
@@ -37064,7 +37070,7 @@
       </c>
       <c r="Q426" s="7"/>
       <c r="R426" s="7" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="S426" s="7"/>
       <c r="T426" s="7" t="s">
@@ -37078,7 +37084,7 @@
         <v>2089</v>
       </c>
       <c r="Z426" s="15" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="AA426"/>
       <c r="AB426"/>
@@ -37106,7 +37112,7 @@
       </c>
       <c r="L427" s="7"/>
       <c r="M427" s="53" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="N427" s="7"/>
       <c r="O427" s="6">
@@ -37117,7 +37123,7 @@
       </c>
       <c r="Q427" s="7"/>
       <c r="R427" s="7" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="S427" s="7"/>
       <c r="T427" s="7" t="s">
@@ -37131,7 +37137,7 @@
         <v>2089</v>
       </c>
       <c r="Z427" s="15" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="AA427"/>
       <c r="AB427"/>
@@ -37159,7 +37165,7 @@
       </c>
       <c r="L428" s="7"/>
       <c r="M428" s="53" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="N428" s="7"/>
       <c r="O428" s="6">
@@ -37170,7 +37176,7 @@
       </c>
       <c r="Q428" s="7"/>
       <c r="R428" s="7" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="S428" s="7"/>
       <c r="T428" s="7" t="s">
@@ -37184,7 +37190,7 @@
         <v>2089</v>
       </c>
       <c r="Z428" s="15" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="AA428"/>
       <c r="AB428"/>
@@ -37212,7 +37218,7 @@
       </c>
       <c r="L429" s="7"/>
       <c r="M429" s="53" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="N429" s="7"/>
       <c r="O429" s="6">
@@ -37223,7 +37229,7 @@
       </c>
       <c r="Q429" s="7"/>
       <c r="R429" s="7" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="S429" s="7"/>
       <c r="T429" s="7" t="s">
@@ -37237,7 +37243,7 @@
         <v>2089</v>
       </c>
       <c r="Z429" s="15" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="AA429"/>
       <c r="AB429"/>
@@ -37245,7 +37251,7 @@
     </row>
     <row r="430" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A430" s="47" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="B430" s="7"/>
       <c r="C430" s="7"/>
@@ -37299,7 +37305,7 @@
     </row>
     <row r="431" spans="1:29" s="42" customFormat="1" ht="170" x14ac:dyDescent="0.15">
       <c r="A431" s="47" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="B431" s="7"/>
       <c r="C431" s="7"/>
@@ -37354,7 +37360,7 @@
     </row>
     <row r="432" spans="1:29" s="42" customFormat="1" ht="136" x14ac:dyDescent="0.15">
       <c r="A432" s="47" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="B432" s="7"/>
       <c r="C432" s="7"/>
@@ -37412,7 +37418,7 @@
     </row>
     <row r="433" spans="1:29" s="42" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A433" s="47" t="s">
-        <v>2090</v>
+        <v>2123</v>
       </c>
       <c r="B433" s="7"/>
       <c r="C433" s="7"/>
@@ -37428,7 +37434,7 @@
       <c r="I433" s="6"/>
       <c r="J433" s="53"/>
       <c r="K433" s="53" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="L433" s="7"/>
       <c r="M433" s="53" t="s">
@@ -37451,7 +37457,7 @@
       <c r="V433" s="7"/>
       <c r="W433" s="7"/>
       <c r="X433" s="7" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
       <c r="Y433" s="7" t="s">
         <v>1925</v>
@@ -37463,7 +37469,7 @@
     </row>
     <row r="434" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A434" s="47" t="s">
-        <v>2090</v>
+        <v>2124</v>
       </c>
       <c r="B434" s="7"/>
       <c r="C434" s="7"/>
@@ -37478,7 +37484,7 @@
       <c r="H434" s="6"/>
       <c r="I434" s="6"/>
       <c r="K434" s="53" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="L434" s="7"/>
       <c r="M434" s="53" t="s">
@@ -37493,7 +37499,7 @@
       </c>
       <c r="Q434" s="7"/>
       <c r="R434" s="7" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="S434" s="7"/>
       <c r="T434" s="7"/>
@@ -37501,11 +37507,11 @@
       <c r="V434" s="7"/>
       <c r="W434" s="7"/>
       <c r="X434" s="7" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="Y434" s="7"/>
       <c r="Z434" s="15" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
       <c r="AA434"/>
       <c r="AB434"/>
@@ -37513,7 +37519,7 @@
     </row>
     <row r="435" spans="1:29" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A435" s="47" t="s">
-        <v>2090</v>
+        <v>2125</v>
       </c>
       <c r="B435" s="7"/>
       <c r="C435" s="7"/>
@@ -37528,7 +37534,7 @@
       <c r="H435" s="6"/>
       <c r="I435" s="6"/>
       <c r="K435" s="53" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="L435" s="7"/>
       <c r="M435" s="53" t="s">
@@ -37539,11 +37545,11 @@
         <v>3</v>
       </c>
       <c r="P435" s="7" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="Q435" s="7"/>
       <c r="R435" s="7" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="S435" s="7"/>
       <c r="T435" s="7"/>
@@ -37551,11 +37557,11 @@
       <c r="V435" s="7"/>
       <c r="W435" s="7"/>
       <c r="X435" s="7" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="Y435" s="7"/>
       <c r="Z435" s="15" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="AA435"/>
       <c r="AB435"/>

</xml_diff>

<commit_message>
modifications of C. 66
</commit_message>
<xml_diff>
--- a/metadata/InventaireCampa.xlsx
+++ b/metadata/InventaireCampa.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salomepichon/Documents/GitHub/DHARMA/tfc-campa-epigraphy/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{9C65CD48-B6D3-654A-92ED-A0425CA1AC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{B0AFE0DE-58DA-AD41-A169-CF81352FEA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2040" windowWidth="10000" windowHeight="15380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13222,8 +13222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC459"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1300" topLeftCell="A432" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <pane ySplit="900" topLeftCell="A431" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A436" sqref="A436"/>
     </sheetView>

</xml_diff>